<commit_message>
2022/11.06 1:30 update ae folder and compare table, but compare table has a problem
</commit_message>
<xml_diff>
--- a/documents/latent_vector/dqn_enc.xlsx
+++ b/documents/latent_vector/dqn_enc.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -449,13 +449,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>-1.804817914962769</v>
+        <v>1.38260817527771</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.7457171678543091</v>
+        <v>1.333788394927979</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.9858357906341553</v>
+        <v>1.201528906822205</v>
       </c>
     </row>
     <row r="3">
@@ -463,13 +463,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-1.842819452285767</v>
+        <v>1.354099035263062</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.7561498880386353</v>
+        <v>1.364193081855774</v>
       </c>
       <c r="D3" t="n">
-        <v>-1.003324627876282</v>
+        <v>1.130824208259583</v>
       </c>
     </row>
     <row r="4">
@@ -477,13 +477,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-1.752893209457397</v>
+        <v>1.373066663742065</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.7375474572181702</v>
+        <v>1.338040351867676</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.9895057678222656</v>
+        <v>1.233564019203186</v>
       </c>
     </row>
     <row r="5">
@@ -491,13 +491,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-1.817406296730042</v>
+        <v>1.425849795341492</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.7681790590286255</v>
+        <v>1.327592730522156</v>
       </c>
       <c r="D5" t="n">
-        <v>-1.054257273674011</v>
+        <v>1.14039421081543</v>
       </c>
     </row>
     <row r="6">
@@ -505,13 +505,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.688421249389648</v>
+        <v>1.422983169555664</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.6858738660812378</v>
+        <v>1.244916796684265</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.9194484949111938</v>
+        <v>1.197114706039429</v>
       </c>
     </row>
     <row r="7">
@@ -519,13 +519,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-1.758177161216736</v>
+        <v>1.468718647956848</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.7343792915344238</v>
+        <v>1.213865280151367</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.9929815530776978</v>
+        <v>1.130855798721313</v>
       </c>
     </row>
     <row r="8">
@@ -533,13 +533,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-1.672529101371765</v>
+        <v>1.351692199707031</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.6964911222457886</v>
+        <v>1.352370619773865</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.907404363155365</v>
+        <v>1.207689523696899</v>
       </c>
     </row>
     <row r="9">
@@ -547,13 +547,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>-1.81227695941925</v>
+        <v>1.417201161384583</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.7631452083587646</v>
+        <v>1.261340022087097</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.9966180920600891</v>
+        <v>1.163723468780518</v>
       </c>
     </row>
     <row r="10">
@@ -561,13 +561,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-1.768460631370544</v>
+        <v>1.337443947792053</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.7390385866165161</v>
+        <v>1.393130660057068</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.9835760593414307</v>
+        <v>1.222345590591431</v>
       </c>
     </row>
     <row r="11">
@@ -575,13 +575,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-1.885640859603882</v>
+        <v>1.689168453216553</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.7889618873596191</v>
+        <v>1.32054615020752</v>
       </c>
       <c r="D11" t="n">
-        <v>-1.118070602416992</v>
+        <v>1.064882278442383</v>
       </c>
     </row>
     <row r="12">
@@ -589,13 +589,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>-1.814296722412109</v>
+        <v>1.278378486633301</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.7921395897865295</v>
+        <v>1.265823006629944</v>
       </c>
       <c r="D12" t="n">
-        <v>-1.069849252700806</v>
+        <v>1.240287661552429</v>
       </c>
     </row>
     <row r="13">
@@ -603,13 +603,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>-1.990875482559204</v>
+        <v>1.483158230781555</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.8428611159324646</v>
+        <v>1.163116693496704</v>
       </c>
       <c r="D13" t="n">
-        <v>-1.188817739486694</v>
+        <v>1.099806904792786</v>
       </c>
     </row>
     <row r="14">
@@ -617,13 +617,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>-1.867579340934753</v>
+        <v>1.361065864562988</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.7806336879730225</v>
+        <v>1.128326177597046</v>
       </c>
       <c r="D14" t="n">
-        <v>-1.056787014007568</v>
+        <v>1.12185275554657</v>
       </c>
     </row>
     <row r="15">
@@ -631,13 +631,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>-1.868052840232849</v>
+        <v>1.474859237670898</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.8228552341461182</v>
+        <v>1.013247489929199</v>
       </c>
       <c r="D15" t="n">
-        <v>-1.130872011184692</v>
+        <v>1.253808736801147</v>
       </c>
     </row>
     <row r="16">
@@ -645,13 +645,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>-2.083102464675903</v>
+        <v>1.495231986045837</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.953387439250946</v>
+        <v>0.6499451994895935</v>
       </c>
       <c r="D16" t="n">
-        <v>-1.367717266082764</v>
+        <v>1.076823353767395</v>
       </c>
     </row>
     <row r="17">
@@ -659,13 +659,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>-2.327433824539185</v>
+        <v>1.505747437477112</v>
       </c>
       <c r="C17" t="n">
-        <v>-1.058062076568604</v>
+        <v>0.5570793151855469</v>
       </c>
       <c r="D17" t="n">
-        <v>-1.524826645851135</v>
+        <v>1.072927594184875</v>
       </c>
     </row>
     <row r="18">
@@ -673,13 +673,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>-2.153461217880249</v>
+        <v>1.541347622871399</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.9556836485862732</v>
+        <v>0.8448512554168701</v>
       </c>
       <c r="D18" t="n">
-        <v>-1.375689744949341</v>
+        <v>1.157833933830261</v>
       </c>
     </row>
     <row r="19">
@@ -687,13 +687,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>-1.816317558288574</v>
+        <v>1.403221726417542</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.7623054981231689</v>
+        <v>1.130003452301025</v>
       </c>
       <c r="D19" t="n">
-        <v>-1.002848863601685</v>
+        <v>1.184401512145996</v>
       </c>
     </row>
     <row r="20">
@@ -701,13 +701,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>-1.60998272895813</v>
+        <v>1.367342591285706</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.7072997093200684</v>
+        <v>1.480726838111877</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.9607411026954651</v>
+        <v>1.181585669517517</v>
       </c>
     </row>
     <row r="21">
@@ -715,13 +715,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>-1.566832780838013</v>
+        <v>1.32216215133667</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.7122123837471008</v>
+        <v>1.402876973152161</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.9549753069877625</v>
+        <v>1.188481092453003</v>
       </c>
     </row>
     <row r="22">
@@ -729,13 +729,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>-1.816654086112976</v>
+        <v>1.420353889465332</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.7488046288490295</v>
+        <v>1.298616766929626</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.9716614484786987</v>
+        <v>1.124613285064697</v>
       </c>
     </row>
     <row r="23">
@@ -743,13 +743,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>-1.845195174217224</v>
+        <v>1.555728673934937</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.7863808274269104</v>
+        <v>1.26674211025238</v>
       </c>
       <c r="D23" t="n">
-        <v>-1.021561980247498</v>
+        <v>1.281672477722168</v>
       </c>
     </row>
     <row r="24">
@@ -757,13 +757,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>-1.913802862167358</v>
+        <v>1.518223404884338</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.8384944200515747</v>
+        <v>1.248093605041504</v>
       </c>
       <c r="D24" t="n">
-        <v>-1.179059624671936</v>
+        <v>1.142714023590088</v>
       </c>
     </row>
     <row r="25">
@@ -771,13 +771,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>-1.554999709129333</v>
+        <v>1.207995653152466</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.7268901467323303</v>
+        <v>1.573805093765259</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.9569593071937561</v>
+        <v>1.117763757705688</v>
       </c>
     </row>
     <row r="26">
@@ -785,13 +785,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>-1.570622801780701</v>
+        <v>1.442306518554688</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.7294943332672119</v>
+        <v>1.293964862823486</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.9901238679885864</v>
+        <v>1.278120875358582</v>
       </c>
     </row>
     <row r="27">
@@ -799,13 +799,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>-1.5758296251297</v>
+        <v>1.409911632537842</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.7567796111106873</v>
+        <v>1.277731657028198</v>
       </c>
       <c r="D27" t="n">
-        <v>-1.023313164710999</v>
+        <v>1.145419239997864</v>
       </c>
     </row>
     <row r="28">
@@ -813,13 +813,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>-1.931238055229187</v>
+        <v>1.351502060890198</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.8066573739051819</v>
+        <v>1.41516375541687</v>
       </c>
       <c r="D28" t="n">
-        <v>-1.134705066680908</v>
+        <v>1.105902433395386</v>
       </c>
     </row>
     <row r="29">
@@ -827,13 +827,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>-2.397109746932983</v>
+        <v>1.5245600938797</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.9008634686470032</v>
+        <v>1.446593999862671</v>
       </c>
       <c r="D29" t="n">
-        <v>-1.297834992408752</v>
+        <v>1.248631596565247</v>
       </c>
     </row>
     <row r="30">
@@ -841,13 +841,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>-2.545792579650879</v>
+        <v>1.514808177947998</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.9257643818855286</v>
+        <v>1.428151845932007</v>
       </c>
       <c r="D30" t="n">
-        <v>-1.329272150993347</v>
+        <v>1.204763293266296</v>
       </c>
     </row>
     <row r="31">
@@ -855,13 +855,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>-2.476603269577026</v>
+        <v>1.433529615402222</v>
       </c>
       <c r="C31" t="n">
-        <v>-0.9286524653434753</v>
+        <v>1.576170682907104</v>
       </c>
       <c r="D31" t="n">
-        <v>-1.347123622894287</v>
+        <v>1.230529546737671</v>
       </c>
     </row>
     <row r="32">
@@ -869,13 +869,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>-2.498184204101562</v>
+        <v>1.508894324302673</v>
       </c>
       <c r="C32" t="n">
-        <v>-0.9224339127540588</v>
+        <v>1.51477038860321</v>
       </c>
       <c r="D32" t="n">
-        <v>-1.330761313438416</v>
+        <v>1.254737019538879</v>
       </c>
     </row>
     <row r="33">
@@ -883,13 +883,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>-2.477077007293701</v>
+        <v>1.452756524085999</v>
       </c>
       <c r="C33" t="n">
-        <v>-0.9349939227104187</v>
+        <v>1.55369770526886</v>
       </c>
       <c r="D33" t="n">
-        <v>-1.350234031677246</v>
+        <v>1.223751902580261</v>
       </c>
     </row>
     <row r="34">
@@ -897,13 +897,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>-2.48888373374939</v>
+        <v>1.465547800064087</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.9501974582672119</v>
+        <v>1.805693507194519</v>
       </c>
       <c r="D34" t="n">
-        <v>-1.360457420349121</v>
+        <v>1.158925533294678</v>
       </c>
     </row>
     <row r="35">
@@ -911,13 +911,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>-1.781359076499939</v>
+        <v>1.495615482330322</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.8303424715995789</v>
+        <v>1.570710778236389</v>
       </c>
       <c r="D35" t="n">
-        <v>-1.175341725349426</v>
+        <v>1.082826614379883</v>
       </c>
     </row>
     <row r="36">
@@ -925,13 +925,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>-1.672664880752563</v>
+        <v>1.441281080245972</v>
       </c>
       <c r="C36" t="n">
-        <v>-0.712371289730072</v>
+        <v>1.184831619262695</v>
       </c>
       <c r="D36" t="n">
-        <v>-0.9311130046844482</v>
+        <v>1.076450228691101</v>
       </c>
     </row>
     <row r="37">
@@ -939,13 +939,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>-1.710269689559937</v>
+        <v>1.354833841323853</v>
       </c>
       <c r="C37" t="n">
-        <v>-0.6481561064720154</v>
+        <v>1.344171404838562</v>
       </c>
       <c r="D37" t="n">
-        <v>-0.7834929227828979</v>
+        <v>1.114040613174438</v>
       </c>
     </row>
     <row r="38">
@@ -953,13 +953,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>-1.716058254241943</v>
+        <v>1.336213350296021</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.7021717429161072</v>
+        <v>1.237080216407776</v>
       </c>
       <c r="D38" t="n">
-        <v>-0.9554701447486877</v>
+        <v>1.16956639289856</v>
       </c>
     </row>
     <row r="39">
@@ -967,13 +967,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>-1.608031392097473</v>
+        <v>1.404897332191467</v>
       </c>
       <c r="C39" t="n">
-        <v>-0.5995925664901733</v>
+        <v>1.409415483474731</v>
       </c>
       <c r="D39" t="n">
-        <v>-0.751476526260376</v>
+        <v>1.172039747238159</v>
       </c>
     </row>
     <row r="40">
@@ -981,13 +981,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>-1.649003863334656</v>
+        <v>1.458954215049744</v>
       </c>
       <c r="C40" t="n">
-        <v>-0.5620434880256653</v>
+        <v>1.541328072547913</v>
       </c>
       <c r="D40" t="n">
-        <v>-0.6755598783493042</v>
+        <v>1.223782181739807</v>
       </c>
     </row>
     <row r="41">
@@ -995,13 +995,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>-1.629265904426575</v>
+        <v>1.477116227149963</v>
       </c>
       <c r="C41" t="n">
-        <v>-0.589668333530426</v>
+        <v>1.454416871070862</v>
       </c>
       <c r="D41" t="n">
-        <v>-0.7485846877098083</v>
+        <v>1.134784460067749</v>
       </c>
     </row>
     <row r="42">
@@ -1009,13 +1009,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>-1.635043740272522</v>
+        <v>1.157425403594971</v>
       </c>
       <c r="C42" t="n">
-        <v>-0.5808716416358948</v>
+        <v>1.523772358894348</v>
       </c>
       <c r="D42" t="n">
-        <v>-0.7202155590057373</v>
+        <v>0.9534440636634827</v>
       </c>
     </row>
     <row r="43">
@@ -1023,13 +1023,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>-1.718000054359436</v>
+        <v>1.413660764694214</v>
       </c>
       <c r="C43" t="n">
-        <v>-0.6297159790992737</v>
+        <v>1.423832893371582</v>
       </c>
       <c r="D43" t="n">
-        <v>-0.8216192722320557</v>
+        <v>1.146169304847717</v>
       </c>
     </row>
     <row r="44">
@@ -1037,13 +1037,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>-1.714700818061829</v>
+        <v>1.421111583709717</v>
       </c>
       <c r="C44" t="n">
-        <v>-0.6511770486831665</v>
+        <v>1.391638994216919</v>
       </c>
       <c r="D44" t="n">
-        <v>-0.8037546873092651</v>
+        <v>1.283087372779846</v>
       </c>
     </row>
     <row r="45">
@@ -1051,13 +1051,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>-1.696038246154785</v>
+        <v>1.258317947387695</v>
       </c>
       <c r="C45" t="n">
-        <v>-0.6533209085464478</v>
+        <v>1.422221899032593</v>
       </c>
       <c r="D45" t="n">
-        <v>-0.8160655498504639</v>
+        <v>1.184150338172913</v>
       </c>
     </row>
     <row r="46">
@@ -1065,13 +1065,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>-1.682503819465637</v>
+        <v>1.284511089324951</v>
       </c>
       <c r="C46" t="n">
-        <v>-0.643196165561676</v>
+        <v>1.363954663276672</v>
       </c>
       <c r="D46" t="n">
-        <v>-0.8149964809417725</v>
+        <v>1.182343363761902</v>
       </c>
     </row>
     <row r="47">
@@ -1079,13 +1079,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>-1.734731674194336</v>
+        <v>1.272263169288635</v>
       </c>
       <c r="C47" t="n">
-        <v>-0.6707489490509033</v>
+        <v>1.39550244808197</v>
       </c>
       <c r="D47" t="n">
-        <v>-0.8589866161346436</v>
+        <v>1.180385828018188</v>
       </c>
     </row>
     <row r="48">
@@ -1093,13 +1093,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>-1.729385733604431</v>
+        <v>1.349089384078979</v>
       </c>
       <c r="C48" t="n">
-        <v>-0.6780252456665039</v>
+        <v>1.321830987930298</v>
       </c>
       <c r="D48" t="n">
-        <v>-0.8704227209091187</v>
+        <v>1.232503652572632</v>
       </c>
     </row>
     <row r="49">
@@ -1107,13 +1107,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>-2.198524236679077</v>
+        <v>1.437482833862305</v>
       </c>
       <c r="C49" t="n">
-        <v>-0.9302652478218079</v>
+        <v>0.8898297548294067</v>
       </c>
       <c r="D49" t="n">
-        <v>-1.32914400100708</v>
+        <v>1.153773188591003</v>
       </c>
     </row>
     <row r="50">
@@ -1121,13 +1121,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>-4.12371826171875</v>
+        <v>2.003695249557495</v>
       </c>
       <c r="C50" t="n">
-        <v>-1.302573561668396</v>
+        <v>1.489593029022217</v>
       </c>
       <c r="D50" t="n">
-        <v>-1.689361333847046</v>
+        <v>0.9864022135734558</v>
       </c>
     </row>
     <row r="51">
@@ -1135,13 +1135,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>-0.5815984606742859</v>
+        <v>1.427159905433655</v>
       </c>
       <c r="C51" t="n">
-        <v>-0.2422083169221878</v>
+        <v>2.127187728881836</v>
       </c>
       <c r="D51" t="n">
-        <v>-0.3212054967880249</v>
+        <v>1.645982980728149</v>
       </c>
     </row>
     <row r="52">
@@ -1149,13 +1149,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>-0.4668937027454376</v>
+        <v>1.441756963729858</v>
       </c>
       <c r="C52" t="n">
-        <v>-0.1954708248376846</v>
+        <v>1.967534184455872</v>
       </c>
       <c r="D52" t="n">
-        <v>-0.2730388641357422</v>
+        <v>1.679003477096558</v>
       </c>
     </row>
     <row r="53">
@@ -1163,13 +1163,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>-3.472342252731323</v>
+        <v>1.834468483924866</v>
       </c>
       <c r="C53" t="n">
-        <v>-1.139289855957031</v>
+        <v>1.619353055953979</v>
       </c>
       <c r="D53" t="n">
-        <v>-1.509552836418152</v>
+        <v>1.002636075019836</v>
       </c>
     </row>
     <row r="54">
@@ -1177,13 +1177,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>-1.750209093093872</v>
+        <v>1.759117603302002</v>
       </c>
       <c r="C54" t="n">
-        <v>-0.6600785255432129</v>
+        <v>1.733428120613098</v>
       </c>
       <c r="D54" t="n">
-        <v>-0.9139671921730042</v>
+        <v>1.47888457775116</v>
       </c>
     </row>
     <row r="55">
@@ -1191,13 +1191,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>-1.752214074134827</v>
+        <v>2.024714469909668</v>
       </c>
       <c r="C55" t="n">
-        <v>-0.6259041428565979</v>
+        <v>1.591212749481201</v>
       </c>
       <c r="D55" t="n">
-        <v>-0.8485372066497803</v>
+        <v>1.511135339736938</v>
       </c>
     </row>
     <row r="56">
@@ -1205,13 +1205,13 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>-1.911943197250366</v>
+        <v>1.346579432487488</v>
       </c>
       <c r="C56" t="n">
-        <v>-0.8501628637313843</v>
+        <v>1.412426471710205</v>
       </c>
       <c r="D56" t="n">
-        <v>-1.174604296684265</v>
+        <v>1.121132016181946</v>
       </c>
     </row>
     <row r="57">
@@ -1219,13 +1219,13 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>-1.74122166633606</v>
+        <v>1.29625415802002</v>
       </c>
       <c r="C57" t="n">
-        <v>-0.7121137976646423</v>
+        <v>2.180815935134888</v>
       </c>
       <c r="D57" t="n">
-        <v>-0.9788232445716858</v>
+        <v>1.243563413619995</v>
       </c>
     </row>
     <row r="58">
@@ -1233,13 +1233,13 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>-1.834718823432922</v>
+        <v>1.388128042221069</v>
       </c>
       <c r="C58" t="n">
-        <v>-0.7811413407325745</v>
+        <v>1.691631555557251</v>
       </c>
       <c r="D58" t="n">
-        <v>-1.090695977210999</v>
+        <v>1.266273021697998</v>
       </c>
     </row>
     <row r="59">
@@ -1247,13 +1247,13 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>-1.868539452552795</v>
+        <v>1.510433673858643</v>
       </c>
       <c r="C59" t="n">
-        <v>-0.8027967214584351</v>
+        <v>1.473437786102295</v>
       </c>
       <c r="D59" t="n">
-        <v>-1.140784740447998</v>
+        <v>1.235455632209778</v>
       </c>
     </row>
     <row r="60">
@@ -1261,13 +1261,13 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>-4.282875061035156</v>
+        <v>1.908511877059937</v>
       </c>
       <c r="C60" t="n">
-        <v>-1.330974459648132</v>
+        <v>1.423482894897461</v>
       </c>
       <c r="D60" t="n">
-        <v>-1.720424652099609</v>
+        <v>0.9577713012695312</v>
       </c>
     </row>
     <row r="61">
@@ -1275,13 +1275,13 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>-2.16096019744873</v>
+        <v>1.473905682563782</v>
       </c>
       <c r="C61" t="n">
-        <v>-0.9315779209136963</v>
+        <v>1.641622185707092</v>
       </c>
       <c r="D61" t="n">
-        <v>-1.285930752754211</v>
+        <v>1.170886874198914</v>
       </c>
     </row>
     <row r="62">
@@ -1289,13 +1289,13 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>-1.959317207336426</v>
+        <v>1.400728464126587</v>
       </c>
       <c r="C62" t="n">
-        <v>-0.8681929707527161</v>
+        <v>1.397239923477173</v>
       </c>
       <c r="D62" t="n">
-        <v>-1.220816135406494</v>
+        <v>1.263144493103027</v>
       </c>
     </row>
     <row r="63">
@@ -1303,13 +1303,13 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>-1.260993599891663</v>
+        <v>1.360970735549927</v>
       </c>
       <c r="C63" t="n">
-        <v>-0.5212345719337463</v>
+        <v>1.237980604171753</v>
       </c>
       <c r="D63" t="n">
-        <v>-0.7430819272994995</v>
+        <v>1.327872633934021</v>
       </c>
     </row>
     <row r="64">
@@ -1317,13 +1317,13 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>-1.897513866424561</v>
+        <v>1.375050187110901</v>
       </c>
       <c r="C64" t="n">
-        <v>-0.7372351884841919</v>
+        <v>2.153771162033081</v>
       </c>
       <c r="D64" t="n">
-        <v>-1.035364627838135</v>
+        <v>0.4185846447944641</v>
       </c>
     </row>
     <row r="65">
@@ -1331,13 +1331,13 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>-2.010767221450806</v>
+        <v>1.09211802482605</v>
       </c>
       <c r="C65" t="n">
-        <v>-0.6829560399055481</v>
+        <v>1.731274366378784</v>
       </c>
       <c r="D65" t="n">
-        <v>-0.7586294412612915</v>
+        <v>0.9569756984710693</v>
       </c>
     </row>
     <row r="66">
@@ -1345,13 +1345,13 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>-2.03809118270874</v>
+        <v>0.9766467809677124</v>
       </c>
       <c r="C66" t="n">
-        <v>-0.7164682745933533</v>
+        <v>1.121377944946289</v>
       </c>
       <c r="D66" t="n">
-        <v>-0.7551247477531433</v>
+        <v>1.017995595932007</v>
       </c>
     </row>
     <row r="67">
@@ -1359,13 +1359,13 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>-1.787686586380005</v>
+        <v>0.4934731721878052</v>
       </c>
       <c r="C67" t="n">
-        <v>-0.71003657579422</v>
+        <v>1.053953051567078</v>
       </c>
       <c r="D67" t="n">
-        <v>-0.911588728427887</v>
+        <v>0.2388256192207336</v>
       </c>
     </row>
     <row r="68">
@@ -1373,13 +1373,13 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>-1.895616292953491</v>
+        <v>1.677116513252258</v>
       </c>
       <c r="C68" t="n">
-        <v>-0.6808487772941589</v>
+        <v>0.9818514585494995</v>
       </c>
       <c r="D68" t="n">
-        <v>-0.8917305469512939</v>
+        <v>1.063097596168518</v>
       </c>
     </row>
     <row r="69">
@@ -1387,13 +1387,13 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>-2.009149551391602</v>
+        <v>1.17270302772522</v>
       </c>
       <c r="C69" t="n">
-        <v>-0.6689597368240356</v>
+        <v>1.504634618759155</v>
       </c>
       <c r="D69" t="n">
-        <v>-0.7179586887359619</v>
+        <v>1.054217219352722</v>
       </c>
     </row>
     <row r="70">
@@ -1401,13 +1401,13 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>-1.939312696456909</v>
+        <v>1.561233639717102</v>
       </c>
       <c r="C70" t="n">
-        <v>-0.8536956906318665</v>
+        <v>1.228689908981323</v>
       </c>
       <c r="D70" t="n">
-        <v>-1.206344842910767</v>
+        <v>1.22369909286499</v>
       </c>
     </row>
     <row r="71">
@@ -1415,13 +1415,13 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>-2.136771678924561</v>
+        <v>1.471372127532959</v>
       </c>
       <c r="C71" t="n">
-        <v>-0.8859877586364746</v>
+        <v>1.548112392425537</v>
       </c>
       <c r="D71" t="n">
-        <v>-1.227130532264709</v>
+        <v>1.11443817615509</v>
       </c>
     </row>
     <row r="72">
@@ -1429,13 +1429,13 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>-1.865845084190369</v>
+        <v>1.328602194786072</v>
       </c>
       <c r="C72" t="n">
-        <v>-0.7301976680755615</v>
+        <v>1.61630117893219</v>
       </c>
       <c r="D72" t="n">
-        <v>-1.012540817260742</v>
+        <v>1.039539217948914</v>
       </c>
     </row>
     <row r="73">
@@ -1443,13 +1443,13 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>-2.012890577316284</v>
+        <v>1.302505135536194</v>
       </c>
       <c r="C73" t="n">
-        <v>-0.7358832359313965</v>
+        <v>1.705398917198181</v>
       </c>
       <c r="D73" t="n">
-        <v>-0.9259873628616333</v>
+        <v>1.058629274368286</v>
       </c>
     </row>
     <row r="74">
@@ -1457,13 +1457,13 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>-2.021487951278687</v>
+        <v>1.205953478813171</v>
       </c>
       <c r="C74" t="n">
-        <v>-0.6804131269454956</v>
+        <v>1.596913814544678</v>
       </c>
       <c r="D74" t="n">
-        <v>-0.7393114566802979</v>
+        <v>1.028964638710022</v>
       </c>
     </row>
     <row r="75">
@@ -1471,13 +1471,13 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>-2.054004430770874</v>
+        <v>1.0496826171875</v>
       </c>
       <c r="C75" t="n">
-        <v>-0.6757668852806091</v>
+        <v>1.467570185661316</v>
       </c>
       <c r="D75" t="n">
-        <v>-0.6882221102714539</v>
+        <v>0.9656482338905334</v>
       </c>
     </row>
     <row r="76">
@@ -1485,13 +1485,13 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>-2.052809476852417</v>
+        <v>1.192092299461365</v>
       </c>
       <c r="C76" t="n">
-        <v>-0.8354023694992065</v>
+        <v>1.203312158584595</v>
       </c>
       <c r="D76" t="n">
-        <v>-1.027785420417786</v>
+        <v>1.066016554832458</v>
       </c>
     </row>
     <row r="77">
@@ -1499,13 +1499,13 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>-0.8854876756668091</v>
+        <v>1.154064655303955</v>
       </c>
       <c r="C77" t="n">
-        <v>-0.5007829070091248</v>
+        <v>1.726412653923035</v>
       </c>
       <c r="D77" t="n">
-        <v>-0.6184034943580627</v>
+        <v>1.149245023727417</v>
       </c>
     </row>
     <row r="78">
@@ -1513,13 +1513,13 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>-1.008615732192993</v>
+        <v>1.071556925773621</v>
       </c>
       <c r="C78" t="n">
-        <v>-0.5066577196121216</v>
+        <v>1.720579028129578</v>
       </c>
       <c r="D78" t="n">
-        <v>-0.6097976565361023</v>
+        <v>1.178492903709412</v>
       </c>
     </row>
     <row r="79">
@@ -1527,13 +1527,13 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>-2.066196441650391</v>
+        <v>1.455895781517029</v>
       </c>
       <c r="C79" t="n">
-        <v>-0.9593336582183838</v>
+        <v>0.8853147029876709</v>
       </c>
       <c r="D79" t="n">
-        <v>-1.375103354454041</v>
+        <v>1.021504521369934</v>
       </c>
     </row>
     <row r="80">
@@ -1541,13 +1541,13 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>-0.8313243985176086</v>
+        <v>1.136869788169861</v>
       </c>
       <c r="C80" t="n">
-        <v>-0.5034492611885071</v>
+        <v>1.874251484870911</v>
       </c>
       <c r="D80" t="n">
-        <v>-0.6336386203765869</v>
+        <v>1.145687460899353</v>
       </c>
     </row>
     <row r="81">
@@ -1555,13 +1555,13 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>-0.9884328246116638</v>
+        <v>1.043880105018616</v>
       </c>
       <c r="C81" t="n">
-        <v>-0.5436252951622009</v>
+        <v>1.676045536994934</v>
       </c>
       <c r="D81" t="n">
-        <v>-0.6422144770622253</v>
+        <v>1.10271143913269</v>
       </c>
     </row>
     <row r="82">
@@ -1569,13 +1569,13 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>-1.859105467796326</v>
+        <v>1.245814323425293</v>
       </c>
       <c r="C82" t="n">
-        <v>-0.5857151746749878</v>
+        <v>1.601518750190735</v>
       </c>
       <c r="D82" t="n">
-        <v>-0.6164712905883789</v>
+        <v>1.173317193984985</v>
       </c>
     </row>
     <row r="83">
@@ -1583,13 +1583,13 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>-1.543596386909485</v>
+        <v>1.282585263252258</v>
       </c>
       <c r="C83" t="n">
-        <v>-0.4646015167236328</v>
+        <v>1.48673951625824</v>
       </c>
       <c r="D83" t="n">
-        <v>-0.4727726578712463</v>
+        <v>1.180336475372314</v>
       </c>
     </row>
     <row r="84">
@@ -1597,13 +1597,13 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>-0.8613018393516541</v>
+        <v>1.484570264816284</v>
       </c>
       <c r="C84" t="n">
-        <v>-0.2896124720573425</v>
+        <v>1.692958831787109</v>
       </c>
       <c r="D84" t="n">
-        <v>-0.3932195901870728</v>
+        <v>1.364233613014221</v>
       </c>
     </row>
     <row r="85">
@@ -1611,13 +1611,13 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>-1.668151259422302</v>
+        <v>1.307663917541504</v>
       </c>
       <c r="C85" t="n">
-        <v>-0.5021902918815613</v>
+        <v>1.595051646232605</v>
       </c>
       <c r="D85" t="n">
-        <v>-0.5139888525009155</v>
+        <v>1.144386291503906</v>
       </c>
     </row>
     <row r="86">
@@ -1625,13 +1625,13 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>-1.711201190948486</v>
+        <v>1.199769258499146</v>
       </c>
       <c r="C86" t="n">
-        <v>-0.5395349264144897</v>
+        <v>1.55948543548584</v>
       </c>
       <c r="D86" t="n">
-        <v>-0.5884987115859985</v>
+        <v>1.026269555091858</v>
       </c>
     </row>
     <row r="87">
@@ -1639,13 +1639,13 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>-1.706868767738342</v>
+        <v>1.382409572601318</v>
       </c>
       <c r="C87" t="n">
-        <v>-0.5292763113975525</v>
+        <v>1.517946481704712</v>
       </c>
       <c r="D87" t="n">
-        <v>-0.5613619089126587</v>
+        <v>1.197680711746216</v>
       </c>
     </row>
     <row r="88">
@@ -1653,13 +1653,13 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>-1.694087624549866</v>
+        <v>1.268410086631775</v>
       </c>
       <c r="C88" t="n">
-        <v>-0.7385697364807129</v>
+        <v>0.7043652534484863</v>
       </c>
       <c r="D88" t="n">
-        <v>-0.9891839027404785</v>
+        <v>1.1117844581604</v>
       </c>
     </row>
     <row r="89">
@@ -1667,13 +1667,13 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>-1.561675548553467</v>
+        <v>1.396916627883911</v>
       </c>
       <c r="C89" t="n">
-        <v>-0.4956406652927399</v>
+        <v>1.605281114578247</v>
       </c>
       <c r="D89" t="n">
-        <v>-0.540553867816925</v>
+        <v>1.24239706993103</v>
       </c>
     </row>
     <row r="90">
@@ -1681,13 +1681,13 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>-1.606193542480469</v>
+        <v>1.352335929870605</v>
       </c>
       <c r="C90" t="n">
-        <v>-0.5046840906143188</v>
+        <v>1.642978549003601</v>
       </c>
       <c r="D90" t="n">
-        <v>-0.5382999181747437</v>
+        <v>1.213842153549194</v>
       </c>
     </row>
     <row r="91">
@@ -1695,13 +1695,13 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>-3.532552003860474</v>
+        <v>1.430204391479492</v>
       </c>
       <c r="C91" t="n">
-        <v>-0.9429133534431458</v>
+        <v>0.9190539121627808</v>
       </c>
       <c r="D91" t="n">
-        <v>-1.097814440727234</v>
+        <v>0.6131792664527893</v>
       </c>
     </row>
     <row r="92">
@@ -1709,13 +1709,13 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>-2.476305723190308</v>
+        <v>1.0543133020401</v>
       </c>
       <c r="C92" t="n">
-        <v>-0.6461484432220459</v>
+        <v>0.8825486898422241</v>
       </c>
       <c r="D92" t="n">
-        <v>-0.7181442379951477</v>
+        <v>0.6587885022163391</v>
       </c>
     </row>
     <row r="93">
@@ -1723,13 +1723,13 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>-2.509866237640381</v>
+        <v>1.071239113807678</v>
       </c>
       <c r="C93" t="n">
-        <v>-0.6998847126960754</v>
+        <v>1.013058185577393</v>
       </c>
       <c r="D93" t="n">
-        <v>-0.8264195322990417</v>
+        <v>0.6216095685958862</v>
       </c>
     </row>
     <row r="94">
@@ -1737,13 +1737,13 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>-2.549698829650879</v>
+        <v>1.122625231742859</v>
       </c>
       <c r="C94" t="n">
-        <v>-0.6855171322822571</v>
+        <v>0.9549543857574463</v>
       </c>
       <c r="D94" t="n">
-        <v>-0.8101048469543457</v>
+        <v>0.7096114158630371</v>
       </c>
     </row>
     <row r="95">
@@ -1751,13 +1751,13 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>-1.158012628555298</v>
+        <v>1.109021544456482</v>
       </c>
       <c r="C95" t="n">
-        <v>-0.4707844853401184</v>
+        <v>0.8717786073684692</v>
       </c>
       <c r="D95" t="n">
-        <v>-0.5695822834968567</v>
+        <v>0.8313714861869812</v>
       </c>
     </row>
     <row r="96">
@@ -1765,13 +1765,13 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>-2.727942228317261</v>
+        <v>1.376821160316467</v>
       </c>
       <c r="C96" t="n">
-        <v>-0.9903284907341003</v>
+        <v>1.643838047981262</v>
       </c>
       <c r="D96" t="n">
-        <v>-1.401057958602905</v>
+        <v>1.057790398597717</v>
       </c>
     </row>
     <row r="97">
@@ -1779,13 +1779,13 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>-1.561463117599487</v>
+        <v>1.355890870094299</v>
       </c>
       <c r="C97" t="n">
-        <v>-0.494594395160675</v>
+        <v>1.675790905952454</v>
       </c>
       <c r="D97" t="n">
-        <v>-0.5376922488212585</v>
+        <v>1.23691201210022</v>
       </c>
     </row>
     <row r="98">
@@ -1793,13 +1793,13 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>-2.269003629684448</v>
+        <v>1.170557737350464</v>
       </c>
       <c r="C98" t="n">
-        <v>-0.9718067049980164</v>
+        <v>1.105569243431091</v>
       </c>
       <c r="D98" t="n">
-        <v>-1.350801467895508</v>
+        <v>0.8687484264373779</v>
       </c>
     </row>
     <row r="99">
@@ -1807,13 +1807,13 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>-2.493216514587402</v>
+        <v>0.9825742840766907</v>
       </c>
       <c r="C99" t="n">
-        <v>-1.044402241706848</v>
+        <v>1.544201612472534</v>
       </c>
       <c r="D99" t="n">
-        <v>-1.495896577835083</v>
+        <v>0.8120055198669434</v>
       </c>
     </row>
     <row r="100">
@@ -1821,13 +1821,13 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>-1.849697589874268</v>
+        <v>1.192088842391968</v>
       </c>
       <c r="C100" t="n">
-        <v>-0.8648609519004822</v>
+        <v>1.318864941596985</v>
       </c>
       <c r="D100" t="n">
-        <v>-1.354768633842468</v>
+        <v>0.9891304969787598</v>
       </c>
     </row>
     <row r="101">
@@ -1835,13 +1835,13 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>-1.774544358253479</v>
+        <v>1.211865305900574</v>
       </c>
       <c r="C101" t="n">
-        <v>-0.8900589346885681</v>
+        <v>1.458596348762512</v>
       </c>
       <c r="D101" t="n">
-        <v>-1.48644745349884</v>
+        <v>0.7452729940414429</v>
       </c>
     </row>
     <row r="102">
@@ -1849,13 +1849,13 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>-1.450439929962158</v>
+        <v>1.519873857498169</v>
       </c>
       <c r="C102" t="n">
-        <v>-0.7862412929534912</v>
+        <v>1.331158876419067</v>
       </c>
       <c r="D102" t="n">
-        <v>-1.115618467330933</v>
+        <v>0.9322522282600403</v>
       </c>
     </row>
     <row r="103">
@@ -1863,13 +1863,13 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>-1.36408519744873</v>
+        <v>1.470897555351257</v>
       </c>
       <c r="C103" t="n">
-        <v>-0.7199391722679138</v>
+        <v>1.390973925590515</v>
       </c>
       <c r="D103" t="n">
-        <v>-1.053801417350769</v>
+        <v>0.8680629730224609</v>
       </c>
     </row>
     <row r="104">
@@ -1877,13 +1877,13 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>-1.607887029647827</v>
+        <v>1.809769034385681</v>
       </c>
       <c r="C104" t="n">
-        <v>-0.7761088013648987</v>
+        <v>1.058686971664429</v>
       </c>
       <c r="D104" t="n">
-        <v>-1.036706924438477</v>
+        <v>1.468475341796875</v>
       </c>
     </row>
     <row r="105">
@@ -1891,13 +1891,13 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>-1.623658180236816</v>
+        <v>1.589665293693542</v>
       </c>
       <c r="C105" t="n">
-        <v>-0.7819808125495911</v>
+        <v>1.549652218818665</v>
       </c>
       <c r="D105" t="n">
-        <v>-1.067117691040039</v>
+        <v>1.158284306526184</v>
       </c>
     </row>
     <row r="106">
@@ -1905,13 +1905,13 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>-2.59604024887085</v>
+        <v>0.8239054083824158</v>
       </c>
       <c r="C106" t="n">
-        <v>-0.7657448053359985</v>
+        <v>0.8499857187271118</v>
       </c>
       <c r="D106" t="n">
-        <v>-0.9143847227096558</v>
+        <v>0.4693102836608887</v>
       </c>
     </row>
     <row r="107">
@@ -1919,13 +1919,13 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>-2.579322814941406</v>
+        <v>1.024374842643738</v>
       </c>
       <c r="C107" t="n">
-        <v>-0.6728182435035706</v>
+        <v>0.8772999048233032</v>
       </c>
       <c r="D107" t="n">
-        <v>-0.7537860870361328</v>
+        <v>0.5714027285575867</v>
       </c>
     </row>
     <row r="108">
@@ -1933,13 +1933,13 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>-2.836318969726562</v>
+        <v>1.260234832763672</v>
       </c>
       <c r="C108" t="n">
-        <v>-1.190938234329224</v>
+        <v>0.5600496530532837</v>
       </c>
       <c r="D108" t="n">
-        <v>-1.632987022399902</v>
+        <v>0.9083471894264221</v>
       </c>
     </row>
     <row r="109">
@@ -1947,13 +1947,13 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>-1.927772521972656</v>
+        <v>1.621909856796265</v>
       </c>
       <c r="C109" t="n">
-        <v>-0.844409704208374</v>
+        <v>1.171980500221252</v>
       </c>
       <c r="D109" t="n">
-        <v>-1.205763936042786</v>
+        <v>1.04813539981842</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2022/11.06 21:30 update gen, compare table, ae
</commit_message>
<xml_diff>
--- a/documents/latent_vector/dqn_enc.xlsx
+++ b/documents/latent_vector/dqn_enc.xlsx
@@ -449,13 +449,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.38260817527771</v>
+        <v>-1.788830041885376</v>
       </c>
       <c r="C2" t="n">
-        <v>1.333788394927979</v>
+        <v>2.761813163757324</v>
       </c>
       <c r="D2" t="n">
-        <v>1.201528906822205</v>
+        <v>0.1770073771476746</v>
       </c>
     </row>
     <row r="3">
@@ -463,13 +463,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.354099035263062</v>
+        <v>-1.796534776687622</v>
       </c>
       <c r="C3" t="n">
-        <v>1.364193081855774</v>
+        <v>2.82730770111084</v>
       </c>
       <c r="D3" t="n">
-        <v>1.130824208259583</v>
+        <v>0.02859849482774734</v>
       </c>
     </row>
     <row r="4">
@@ -477,13 +477,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1.373066663742065</v>
+        <v>-1.785569071769714</v>
       </c>
       <c r="C4" t="n">
-        <v>1.338040351867676</v>
+        <v>2.735684394836426</v>
       </c>
       <c r="D4" t="n">
-        <v>1.233564019203186</v>
+        <v>0.2609202265739441</v>
       </c>
     </row>
     <row r="5">
@@ -491,13 +491,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1.425849795341492</v>
+        <v>-1.793572783470154</v>
       </c>
       <c r="C5" t="n">
-        <v>1.327592730522156</v>
+        <v>2.871055126190186</v>
       </c>
       <c r="D5" t="n">
-        <v>1.14039421081543</v>
+        <v>-0.1036283895373344</v>
       </c>
     </row>
     <row r="6">
@@ -505,13 +505,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>1.422983169555664</v>
+        <v>-1.770533204078674</v>
       </c>
       <c r="C6" t="n">
-        <v>1.244916796684265</v>
+        <v>2.83265495300293</v>
       </c>
       <c r="D6" t="n">
-        <v>1.197114706039429</v>
+        <v>0.05916494876146317</v>
       </c>
     </row>
     <row r="7">
@@ -519,13 +519,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1.468718647956848</v>
+        <v>-1.74581241607666</v>
       </c>
       <c r="C7" t="n">
-        <v>1.213865280151367</v>
+        <v>2.842475414276123</v>
       </c>
       <c r="D7" t="n">
-        <v>1.130855798721313</v>
+        <v>-0.1689754724502563</v>
       </c>
     </row>
     <row r="8">
@@ -533,13 +533,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>1.351692199707031</v>
+        <v>-1.803113222122192</v>
       </c>
       <c r="C8" t="n">
-        <v>1.352370619773865</v>
+        <v>2.7734055519104</v>
       </c>
       <c r="D8" t="n">
-        <v>1.207689523696899</v>
+        <v>0.3271746635437012</v>
       </c>
     </row>
     <row r="9">
@@ -547,13 +547,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>1.417201161384583</v>
+        <v>-1.759005308151245</v>
       </c>
       <c r="C9" t="n">
-        <v>1.261340022087097</v>
+        <v>2.781376123428345</v>
       </c>
       <c r="D9" t="n">
-        <v>1.163723468780518</v>
+        <v>0.1302592158317566</v>
       </c>
     </row>
     <row r="10">
@@ -561,13 +561,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>1.337443947792053</v>
+        <v>-1.83262026309967</v>
       </c>
       <c r="C10" t="n">
-        <v>1.393130660057068</v>
+        <v>2.703132629394531</v>
       </c>
       <c r="D10" t="n">
-        <v>1.222345590591431</v>
+        <v>0.4844480752944946</v>
       </c>
     </row>
     <row r="11">
@@ -575,13 +575,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>1.689168453216553</v>
+        <v>-1.457583546638489</v>
       </c>
       <c r="C11" t="n">
-        <v>1.32054615020752</v>
+        <v>2.556679964065552</v>
       </c>
       <c r="D11" t="n">
-        <v>1.064882278442383</v>
+        <v>-0.5258376598358154</v>
       </c>
     </row>
     <row r="12">
@@ -589,13 +589,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>1.278378486633301</v>
+        <v>-1.954383373260498</v>
       </c>
       <c r="C12" t="n">
-        <v>1.265823006629944</v>
+        <v>2.729389190673828</v>
       </c>
       <c r="D12" t="n">
-        <v>1.240287661552429</v>
+        <v>0.4875642061233521</v>
       </c>
     </row>
     <row r="13">
@@ -603,13 +603,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>1.483158230781555</v>
+        <v>-1.828346014022827</v>
       </c>
       <c r="C13" t="n">
-        <v>1.163116693496704</v>
+        <v>2.848395824432373</v>
       </c>
       <c r="D13" t="n">
-        <v>1.099806904792786</v>
+        <v>-0.1539393067359924</v>
       </c>
     </row>
     <row r="14">
@@ -617,13 +617,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>1.361065864562988</v>
+        <v>-1.813822507858276</v>
       </c>
       <c r="C14" t="n">
-        <v>1.128326177597046</v>
+        <v>2.733080863952637</v>
       </c>
       <c r="D14" t="n">
-        <v>1.12185275554657</v>
+        <v>0.2041867077350616</v>
       </c>
     </row>
     <row r="15">
@@ -631,13 +631,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>1.474859237670898</v>
+        <v>-1.862646460533142</v>
       </c>
       <c r="C15" t="n">
-        <v>1.013247489929199</v>
+        <v>2.742291927337646</v>
       </c>
       <c r="D15" t="n">
-        <v>1.253808736801147</v>
+        <v>0.2659146785736084</v>
       </c>
     </row>
     <row r="16">
@@ -645,13 +645,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>1.495231986045837</v>
+        <v>-1.905779361724854</v>
       </c>
       <c r="C16" t="n">
-        <v>0.6499451994895935</v>
+        <v>2.822513341903687</v>
       </c>
       <c r="D16" t="n">
-        <v>1.076823353767395</v>
+        <v>0.06902862340211868</v>
       </c>
     </row>
     <row r="17">
@@ -659,13 +659,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>1.505747437477112</v>
+        <v>-1.936476230621338</v>
       </c>
       <c r="C17" t="n">
-        <v>0.5570793151855469</v>
+        <v>2.858734369277954</v>
       </c>
       <c r="D17" t="n">
-        <v>1.072927594184875</v>
+        <v>0.2884494662284851</v>
       </c>
     </row>
     <row r="18">
@@ -673,13 +673,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>1.541347622871399</v>
+        <v>-1.896460771560669</v>
       </c>
       <c r="C18" t="n">
-        <v>0.8448512554168701</v>
+        <v>2.816331148147583</v>
       </c>
       <c r="D18" t="n">
-        <v>1.157833933830261</v>
+        <v>0.2293068170547485</v>
       </c>
     </row>
     <row r="19">
@@ -687,13 +687,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>1.403221726417542</v>
+        <v>-1.797838449478149</v>
       </c>
       <c r="C19" t="n">
-        <v>1.130003452301025</v>
+        <v>2.816625118255615</v>
       </c>
       <c r="D19" t="n">
-        <v>1.184401512145996</v>
+        <v>0.1870786547660828</v>
       </c>
     </row>
     <row r="20">
@@ -701,13 +701,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>1.367342591285706</v>
+        <v>-1.714102745056152</v>
       </c>
       <c r="C20" t="n">
-        <v>1.480726838111877</v>
+        <v>2.721461772918701</v>
       </c>
       <c r="D20" t="n">
-        <v>1.181585669517517</v>
+        <v>0.01620126515626907</v>
       </c>
     </row>
     <row r="21">
@@ -715,13 +715,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>1.32216215133667</v>
+        <v>-1.670921921730042</v>
       </c>
       <c r="C21" t="n">
-        <v>1.402876973152161</v>
+        <v>2.647699117660522</v>
       </c>
       <c r="D21" t="n">
-        <v>1.188481092453003</v>
+        <v>0.04934734851121902</v>
       </c>
     </row>
     <row r="22">
@@ -729,13 +729,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>1.420353889465332</v>
+        <v>-1.694433689117432</v>
       </c>
       <c r="C22" t="n">
-        <v>1.298616766929626</v>
+        <v>2.7182776927948</v>
       </c>
       <c r="D22" t="n">
-        <v>1.124613285064697</v>
+        <v>-0.1850286722183228</v>
       </c>
     </row>
     <row r="23">
@@ -743,13 +743,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>1.555728673934937</v>
+        <v>-1.50579845905304</v>
       </c>
       <c r="C23" t="n">
-        <v>1.26674211025238</v>
+        <v>2.574104309082031</v>
       </c>
       <c r="D23" t="n">
-        <v>1.281672477722168</v>
+        <v>-0.01574056595563889</v>
       </c>
     </row>
     <row r="24">
@@ -757,13 +757,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>1.518223404884338</v>
+        <v>-1.752907991409302</v>
       </c>
       <c r="C24" t="n">
-        <v>1.248093605041504</v>
+        <v>2.785487174987793</v>
       </c>
       <c r="D24" t="n">
-        <v>1.142714023590088</v>
+        <v>-0.1700379848480225</v>
       </c>
     </row>
     <row r="25">
@@ -771,13 +771,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>1.207995653152466</v>
+        <v>-1.694122076034546</v>
       </c>
       <c r="C25" t="n">
-        <v>1.573805093765259</v>
+        <v>2.614879608154297</v>
       </c>
       <c r="D25" t="n">
-        <v>1.117763757705688</v>
+        <v>0.1937214732170105</v>
       </c>
     </row>
     <row r="26">
@@ -785,13 +785,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>1.442306518554688</v>
+        <v>-1.788387298583984</v>
       </c>
       <c r="C26" t="n">
-        <v>1.293964862823486</v>
+        <v>2.68560791015625</v>
       </c>
       <c r="D26" t="n">
-        <v>1.278120875358582</v>
+        <v>0.1549782752990723</v>
       </c>
     </row>
     <row r="27">
@@ -799,13 +799,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>1.409911632537842</v>
+        <v>-1.748939871788025</v>
       </c>
       <c r="C27" t="n">
-        <v>1.277731657028198</v>
+        <v>2.832392454147339</v>
       </c>
       <c r="D27" t="n">
-        <v>1.145419239997864</v>
+        <v>-0.1472378373146057</v>
       </c>
     </row>
     <row r="28">
@@ -813,13 +813,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>1.351502060890198</v>
+        <v>-1.791444897651672</v>
       </c>
       <c r="C28" t="n">
-        <v>1.41516375541687</v>
+        <v>2.909592390060425</v>
       </c>
       <c r="D28" t="n">
-        <v>1.105902433395386</v>
+        <v>-0.3206140995025635</v>
       </c>
     </row>
     <row r="29">
@@ -827,13 +827,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>1.5245600938797</v>
+        <v>-1.723034858703613</v>
       </c>
       <c r="C29" t="n">
-        <v>1.446593999862671</v>
+        <v>2.82050895690918</v>
       </c>
       <c r="D29" t="n">
-        <v>1.248631596565247</v>
+        <v>-0.521527886390686</v>
       </c>
     </row>
     <row r="30">
@@ -841,13 +841,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>1.514808177947998</v>
+        <v>-1.824654221534729</v>
       </c>
       <c r="C30" t="n">
-        <v>1.428151845932007</v>
+        <v>2.908658027648926</v>
       </c>
       <c r="D30" t="n">
-        <v>1.204763293266296</v>
+        <v>-0.5327010154724121</v>
       </c>
     </row>
     <row r="31">
@@ -855,13 +855,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>1.433529615402222</v>
+        <v>-1.83190929889679</v>
       </c>
       <c r="C31" t="n">
-        <v>1.576170682907104</v>
+        <v>2.871374845504761</v>
       </c>
       <c r="D31" t="n">
-        <v>1.230529546737671</v>
+        <v>-0.253440260887146</v>
       </c>
     </row>
     <row r="32">
@@ -869,13 +869,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>1.508894324302673</v>
+        <v>-1.763830900192261</v>
       </c>
       <c r="C32" t="n">
-        <v>1.51477038860321</v>
+        <v>2.842137813568115</v>
       </c>
       <c r="D32" t="n">
-        <v>1.254737019538879</v>
+        <v>-0.5144026875495911</v>
       </c>
     </row>
     <row r="33">
@@ -883,13 +883,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>1.452756524085999</v>
+        <v>-1.797590017318726</v>
       </c>
       <c r="C33" t="n">
-        <v>1.55369770526886</v>
+        <v>2.880486726760864</v>
       </c>
       <c r="D33" t="n">
-        <v>1.223751902580261</v>
+        <v>-0.4107177257537842</v>
       </c>
     </row>
     <row r="34">
@@ -897,13 +897,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>1.465547800064087</v>
+        <v>-1.725706338882446</v>
       </c>
       <c r="C34" t="n">
-        <v>1.805693507194519</v>
+        <v>2.95784592628479</v>
       </c>
       <c r="D34" t="n">
-        <v>1.158925533294678</v>
+        <v>-0.6732915639877319</v>
       </c>
     </row>
     <row r="35">
@@ -911,13 +911,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>1.495615482330322</v>
+        <v>-1.583881497383118</v>
       </c>
       <c r="C35" t="n">
-        <v>1.570710778236389</v>
+        <v>2.828881025314331</v>
       </c>
       <c r="D35" t="n">
-        <v>1.082826614379883</v>
+        <v>-0.450782299041748</v>
       </c>
     </row>
     <row r="36">
@@ -925,13 +925,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>1.441281080245972</v>
+        <v>-1.64953088760376</v>
       </c>
       <c r="C36" t="n">
-        <v>1.184831619262695</v>
+        <v>2.711163282394409</v>
       </c>
       <c r="D36" t="n">
-        <v>1.076450228691101</v>
+        <v>-0.1956029534339905</v>
       </c>
     </row>
     <row r="37">
@@ -939,13 +939,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>1.354833841323853</v>
+        <v>-1.687301397323608</v>
       </c>
       <c r="C37" t="n">
-        <v>1.344171404838562</v>
+        <v>2.524833917617798</v>
       </c>
       <c r="D37" t="n">
-        <v>1.114040613174438</v>
+        <v>0.249151200056076</v>
       </c>
     </row>
     <row r="38">
@@ -953,13 +953,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>1.336213350296021</v>
+        <v>-1.820557475090027</v>
       </c>
       <c r="C38" t="n">
-        <v>1.237080216407776</v>
+        <v>2.635960102081299</v>
       </c>
       <c r="D38" t="n">
-        <v>1.16956639289856</v>
+        <v>0.2984968423843384</v>
       </c>
     </row>
     <row r="39">
@@ -967,13 +967,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>1.404897332191467</v>
+        <v>-1.735683798789978</v>
       </c>
       <c r="C39" t="n">
-        <v>1.409415483474731</v>
+        <v>2.649903297424316</v>
       </c>
       <c r="D39" t="n">
-        <v>1.172039747238159</v>
+        <v>-0.01994150131940842</v>
       </c>
     </row>
     <row r="40">
@@ -981,13 +981,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>1.458954215049744</v>
+        <v>-1.743956685066223</v>
       </c>
       <c r="C40" t="n">
-        <v>1.541328072547913</v>
+        <v>2.58085823059082</v>
       </c>
       <c r="D40" t="n">
-        <v>1.223782181739807</v>
+        <v>-0.00471138209104538</v>
       </c>
     </row>
     <row r="41">
@@ -995,13 +995,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>1.477116227149963</v>
+        <v>-1.740137934684753</v>
       </c>
       <c r="C41" t="n">
-        <v>1.454416871070862</v>
+        <v>2.664073467254639</v>
       </c>
       <c r="D41" t="n">
-        <v>1.134784460067749</v>
+        <v>-0.211656928062439</v>
       </c>
     </row>
     <row r="42">
@@ -1009,13 +1009,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>1.157425403594971</v>
+        <v>-1.818404197692871</v>
       </c>
       <c r="C42" t="n">
-        <v>1.523772358894348</v>
+        <v>2.754018306732178</v>
       </c>
       <c r="D42" t="n">
-        <v>0.9534440636634827</v>
+        <v>-0.02618073672056198</v>
       </c>
     </row>
     <row r="43">
@@ -1023,13 +1023,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>1.413660764694214</v>
+        <v>-1.780189156532288</v>
       </c>
       <c r="C43" t="n">
-        <v>1.423832893371582</v>
+        <v>2.742386341094971</v>
       </c>
       <c r="D43" t="n">
-        <v>1.146169304847717</v>
+        <v>-0.128812313079834</v>
       </c>
     </row>
     <row r="44">
@@ -1037,13 +1037,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>1.421111583709717</v>
+        <v>-1.870034337043762</v>
       </c>
       <c r="C44" t="n">
-        <v>1.391638994216919</v>
+        <v>2.626907587051392</v>
       </c>
       <c r="D44" t="n">
-        <v>1.283087372779846</v>
+        <v>0.2048396170139313</v>
       </c>
     </row>
     <row r="45">
@@ -1051,13 +1051,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>1.258317947387695</v>
+        <v>-1.745854616165161</v>
       </c>
       <c r="C45" t="n">
-        <v>1.422221899032593</v>
+        <v>2.425479412078857</v>
       </c>
       <c r="D45" t="n">
-        <v>1.184150338172913</v>
+        <v>0.6137059926986694</v>
       </c>
     </row>
     <row r="46">
@@ -1065,13 +1065,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>1.284511089324951</v>
+        <v>-1.747787356376648</v>
       </c>
       <c r="C46" t="n">
-        <v>1.363954663276672</v>
+        <v>2.470945596694946</v>
       </c>
       <c r="D46" t="n">
-        <v>1.182343363761902</v>
+        <v>0.5254042148590088</v>
       </c>
     </row>
     <row r="47">
@@ -1079,13 +1079,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>1.272263169288635</v>
+        <v>-1.795293211936951</v>
       </c>
       <c r="C47" t="n">
-        <v>1.39550244808197</v>
+        <v>2.531349658966064</v>
       </c>
       <c r="D47" t="n">
-        <v>1.180385828018188</v>
+        <v>0.544035017490387</v>
       </c>
     </row>
     <row r="48">
@@ -1093,13 +1093,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>1.349089384078979</v>
+        <v>-1.854714870452881</v>
       </c>
       <c r="C48" t="n">
-        <v>1.321830987930298</v>
+        <v>2.545819282531738</v>
       </c>
       <c r="D48" t="n">
-        <v>1.232503652572632</v>
+        <v>0.5901591777801514</v>
       </c>
     </row>
     <row r="49">
@@ -1107,13 +1107,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>1.437482833862305</v>
+        <v>-1.85335099697113</v>
       </c>
       <c r="C49" t="n">
-        <v>0.8898297548294067</v>
+        <v>2.733589649200439</v>
       </c>
       <c r="D49" t="n">
-        <v>1.153773188591003</v>
+        <v>0.1422341465950012</v>
       </c>
     </row>
     <row r="50">
@@ -1121,13 +1121,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>2.003695249557495</v>
+        <v>-1.817363500595093</v>
       </c>
       <c r="C50" t="n">
-        <v>1.489593029022217</v>
+        <v>3.222140312194824</v>
       </c>
       <c r="D50" t="n">
-        <v>0.9864022135734558</v>
+        <v>-1.350210428237915</v>
       </c>
     </row>
     <row r="51">
@@ -1135,13 +1135,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>1.427159905433655</v>
+        <v>-1.500515103340149</v>
       </c>
       <c r="C51" t="n">
-        <v>2.127187728881836</v>
+        <v>2.676211595535278</v>
       </c>
       <c r="D51" t="n">
-        <v>1.645982980728149</v>
+        <v>0.04436785727739334</v>
       </c>
     </row>
     <row r="52">
@@ -1149,13 +1149,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>1.441756963729858</v>
+        <v>-1.693747162818909</v>
       </c>
       <c r="C52" t="n">
-        <v>1.967534184455872</v>
+        <v>2.710513114929199</v>
       </c>
       <c r="D52" t="n">
-        <v>1.679003477096558</v>
+        <v>0.1641238033771515</v>
       </c>
     </row>
     <row r="53">
@@ -1163,13 +1163,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>1.834468483924866</v>
+        <v>-1.859506607055664</v>
       </c>
       <c r="C53" t="n">
-        <v>1.619353055953979</v>
+        <v>3.216312885284424</v>
       </c>
       <c r="D53" t="n">
-        <v>1.002636075019836</v>
+        <v>-1.568763613700867</v>
       </c>
     </row>
     <row r="54">
@@ -1177,13 +1177,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>1.759117603302002</v>
+        <v>-1.306578159332275</v>
       </c>
       <c r="C54" t="n">
-        <v>1.733428120613098</v>
+        <v>2.020320415496826</v>
       </c>
       <c r="D54" t="n">
-        <v>1.47888457775116</v>
+        <v>-0.3541139960289001</v>
       </c>
     </row>
     <row r="55">
@@ -1191,13 +1191,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>2.024714469909668</v>
+        <v>-1.646723628044128</v>
       </c>
       <c r="C55" t="n">
-        <v>1.591212749481201</v>
+        <v>2.546635389328003</v>
       </c>
       <c r="D55" t="n">
-        <v>1.511135339736938</v>
+        <v>-1.053088307380676</v>
       </c>
     </row>
     <row r="56">
@@ -1205,13 +1205,13 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>1.346579432487488</v>
+        <v>-1.745261430740356</v>
       </c>
       <c r="C56" t="n">
-        <v>1.412426471710205</v>
+        <v>3.256208419799805</v>
       </c>
       <c r="D56" t="n">
-        <v>1.121132016181946</v>
+        <v>-0.3198471069335938</v>
       </c>
     </row>
     <row r="57">
@@ -1219,13 +1219,13 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>1.29625415802002</v>
+        <v>-1.526459455490112</v>
       </c>
       <c r="C57" t="n">
-        <v>2.180815935134888</v>
+        <v>2.477005481719971</v>
       </c>
       <c r="D57" t="n">
-        <v>1.243563413619995</v>
+        <v>0.3343901336193085</v>
       </c>
     </row>
     <row r="58">
@@ -1233,13 +1233,13 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>1.388128042221069</v>
+        <v>-1.680849075317383</v>
       </c>
       <c r="C58" t="n">
-        <v>1.691631555557251</v>
+        <v>2.760564804077148</v>
       </c>
       <c r="D58" t="n">
-        <v>1.266273021697998</v>
+        <v>0.1077770665287971</v>
       </c>
     </row>
     <row r="59">
@@ -1247,13 +1247,13 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>1.510433673858643</v>
+        <v>-1.806389212608337</v>
       </c>
       <c r="C59" t="n">
-        <v>1.473437786102295</v>
+        <v>3.061006546020508</v>
       </c>
       <c r="D59" t="n">
-        <v>1.235455632209778</v>
+        <v>-0.1978790163993835</v>
       </c>
     </row>
     <row r="60">
@@ -1261,13 +1261,13 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>1.908511877059937</v>
+        <v>-2.00287127494812</v>
       </c>
       <c r="C60" t="n">
-        <v>1.423482894897461</v>
+        <v>3.450778007507324</v>
       </c>
       <c r="D60" t="n">
-        <v>0.9577713012695312</v>
+        <v>-1.019535303115845</v>
       </c>
     </row>
     <row r="61">
@@ -1275,13 +1275,13 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>1.473905682563782</v>
+        <v>-1.84800910949707</v>
       </c>
       <c r="C61" t="n">
-        <v>1.641622185707092</v>
+        <v>3.443219184875488</v>
       </c>
       <c r="D61" t="n">
-        <v>1.170886874198914</v>
+        <v>-0.4980486631393433</v>
       </c>
     </row>
     <row r="62">
@@ -1289,13 +1289,13 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>1.400728464126587</v>
+        <v>-1.952149510383606</v>
       </c>
       <c r="C62" t="n">
-        <v>1.397239923477173</v>
+        <v>3.414097309112549</v>
       </c>
       <c r="D62" t="n">
-        <v>1.263144493103027</v>
+        <v>0.04054272919893265</v>
       </c>
     </row>
     <row r="63">
@@ -1303,13 +1303,13 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>1.360970735549927</v>
+        <v>-1.708168506622314</v>
       </c>
       <c r="C63" t="n">
-        <v>1.237980604171753</v>
+        <v>2.518898487091064</v>
       </c>
       <c r="D63" t="n">
-        <v>1.327872633934021</v>
+        <v>0.7887579798698425</v>
       </c>
     </row>
     <row r="64">
@@ -1317,13 +1317,13 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>1.375050187110901</v>
+        <v>-1.145947217941284</v>
       </c>
       <c r="C64" t="n">
-        <v>2.153771162033081</v>
+        <v>2.21372127532959</v>
       </c>
       <c r="D64" t="n">
-        <v>0.4185846447944641</v>
+        <v>-0.3564375042915344</v>
       </c>
     </row>
     <row r="65">
@@ -1331,13 +1331,13 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>1.09211802482605</v>
+        <v>-1.35295581817627</v>
       </c>
       <c r="C65" t="n">
-        <v>1.731274366378784</v>
+        <v>2.423404932022095</v>
       </c>
       <c r="D65" t="n">
-        <v>0.9569756984710693</v>
+        <v>0.5142398476600647</v>
       </c>
     </row>
     <row r="66">
@@ -1345,13 +1345,13 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>0.9766467809677124</v>
+        <v>-1.492993116378784</v>
       </c>
       <c r="C66" t="n">
-        <v>1.121377944946289</v>
+        <v>2.278056621551514</v>
       </c>
       <c r="D66" t="n">
-        <v>1.017995595932007</v>
+        <v>0.959328293800354</v>
       </c>
     </row>
     <row r="67">
@@ -1359,13 +1359,13 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>0.4934731721878052</v>
+        <v>-1.651567697525024</v>
       </c>
       <c r="C67" t="n">
-        <v>1.053953051567078</v>
+        <v>2.619035482406616</v>
       </c>
       <c r="D67" t="n">
-        <v>0.2388256192207336</v>
+        <v>-0.4180133640766144</v>
       </c>
     </row>
     <row r="68">
@@ -1373,13 +1373,13 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>1.677116513252258</v>
+        <v>-1.598899126052856</v>
       </c>
       <c r="C68" t="n">
-        <v>0.9818514585494995</v>
+        <v>2.878891944885254</v>
       </c>
       <c r="D68" t="n">
-        <v>1.063097596168518</v>
+        <v>-0.9151967167854309</v>
       </c>
     </row>
     <row r="69">
@@ -1387,13 +1387,13 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>1.17270302772522</v>
+        <v>-1.421025276184082</v>
       </c>
       <c r="C69" t="n">
-        <v>1.504634618759155</v>
+        <v>2.479530096054077</v>
       </c>
       <c r="D69" t="n">
-        <v>1.054217219352722</v>
+        <v>0.5023493766784668</v>
       </c>
     </row>
     <row r="70">
@@ -1401,13 +1401,13 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>1.561233639717102</v>
+        <v>-1.784129738807678</v>
       </c>
       <c r="C70" t="n">
-        <v>1.228689908981323</v>
+        <v>2.909031629562378</v>
       </c>
       <c r="D70" t="n">
-        <v>1.22369909286499</v>
+        <v>-0.1432114839553833</v>
       </c>
     </row>
     <row r="71">
@@ -1415,13 +1415,13 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>1.471372127532959</v>
+        <v>-1.721899390220642</v>
       </c>
       <c r="C71" t="n">
-        <v>1.548112392425537</v>
+        <v>3.051913261413574</v>
       </c>
       <c r="D71" t="n">
-        <v>1.11443817615509</v>
+        <v>-0.4195650219917297</v>
       </c>
     </row>
     <row r="72">
@@ -1429,13 +1429,13 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>1.328602194786072</v>
+        <v>-1.535071015357971</v>
       </c>
       <c r="C72" t="n">
-        <v>1.61630117893219</v>
+        <v>2.846559286117554</v>
       </c>
       <c r="D72" t="n">
-        <v>1.039539217948914</v>
+        <v>-0.3042086362838745</v>
       </c>
     </row>
     <row r="73">
@@ -1443,13 +1443,13 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>1.302505135536194</v>
+        <v>-1.588250398635864</v>
       </c>
       <c r="C73" t="n">
-        <v>1.705398917198181</v>
+        <v>2.764822006225586</v>
       </c>
       <c r="D73" t="n">
-        <v>1.058629274368286</v>
+        <v>0.1498149335384369</v>
       </c>
     </row>
     <row r="74">
@@ -1457,13 +1457,13 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>1.205953478813171</v>
+        <v>-1.439719915390015</v>
       </c>
       <c r="C74" t="n">
-        <v>1.596913814544678</v>
+        <v>2.563395261764526</v>
       </c>
       <c r="D74" t="n">
-        <v>1.028964638710022</v>
+        <v>0.4454854130744934</v>
       </c>
     </row>
     <row r="75">
@@ -1471,13 +1471,13 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>1.0496826171875</v>
+        <v>-1.391136407852173</v>
       </c>
       <c r="C75" t="n">
-        <v>1.467570185661316</v>
+        <v>2.362955093383789</v>
       </c>
       <c r="D75" t="n">
-        <v>0.9656482338905334</v>
+        <v>0.6192845702171326</v>
       </c>
     </row>
     <row r="76">
@@ -1485,13 +1485,13 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>1.192092299461365</v>
+        <v>-1.633471131324768</v>
       </c>
       <c r="C76" t="n">
-        <v>1.203312158584595</v>
+        <v>2.718760251998901</v>
       </c>
       <c r="D76" t="n">
-        <v>1.066016554832458</v>
+        <v>0.5195736885070801</v>
       </c>
     </row>
     <row r="77">
@@ -1499,13 +1499,13 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>1.154064655303955</v>
+        <v>-1.563079357147217</v>
       </c>
       <c r="C77" t="n">
-        <v>1.726412653923035</v>
+        <v>2.102933645248413</v>
       </c>
       <c r="D77" t="n">
-        <v>1.149245023727417</v>
+        <v>0.2035261988639832</v>
       </c>
     </row>
     <row r="78">
@@ -1513,13 +1513,13 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>1.071556925773621</v>
+        <v>-1.452157258987427</v>
       </c>
       <c r="C78" t="n">
-        <v>1.720579028129578</v>
+        <v>2.15067720413208</v>
       </c>
       <c r="D78" t="n">
-        <v>1.178492903709412</v>
+        <v>0.3720082640647888</v>
       </c>
     </row>
     <row r="79">
@@ -1527,13 +1527,13 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>1.455895781517029</v>
+        <v>-1.908830881118774</v>
       </c>
       <c r="C79" t="n">
-        <v>0.8853147029876709</v>
+        <v>3.26392674446106</v>
       </c>
       <c r="D79" t="n">
-        <v>1.021504521369934</v>
+        <v>-0.358924925327301</v>
       </c>
     </row>
     <row r="80">
@@ -1541,13 +1541,13 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>1.136869788169861</v>
+        <v>-1.42959725856781</v>
       </c>
       <c r="C80" t="n">
-        <v>1.874251484870911</v>
+        <v>1.855496883392334</v>
       </c>
       <c r="D80" t="n">
-        <v>1.145687460899353</v>
+        <v>0.1648955941200256</v>
       </c>
     </row>
     <row r="81">
@@ -1555,13 +1555,13 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>1.043880105018616</v>
+        <v>-1.561155319213867</v>
       </c>
       <c r="C81" t="n">
-        <v>1.676045536994934</v>
+        <v>2.038600444793701</v>
       </c>
       <c r="D81" t="n">
-        <v>1.10271143913269</v>
+        <v>0.3416443467140198</v>
       </c>
     </row>
     <row r="82">
@@ -1569,13 +1569,13 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>1.245814323425293</v>
+        <v>-1.561890840530396</v>
       </c>
       <c r="C82" t="n">
-        <v>1.601518750190735</v>
+        <v>2.409461736679077</v>
       </c>
       <c r="D82" t="n">
-        <v>1.173317193984985</v>
+        <v>0.5335104465484619</v>
       </c>
     </row>
     <row r="83">
@@ -1583,13 +1583,13 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>1.282585263252258</v>
+        <v>-1.667166709899902</v>
       </c>
       <c r="C83" t="n">
-        <v>1.48673951625824</v>
+        <v>2.339317798614502</v>
       </c>
       <c r="D83" t="n">
-        <v>1.180336475372314</v>
+        <v>0.3354045450687408</v>
       </c>
     </row>
     <row r="84">
@@ -1597,13 +1597,13 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>1.484570264816284</v>
+        <v>-1.470922470092773</v>
       </c>
       <c r="C84" t="n">
-        <v>1.692958831787109</v>
+        <v>2.713351249694824</v>
       </c>
       <c r="D84" t="n">
-        <v>1.364233613014221</v>
+        <v>-0.3337305188179016</v>
       </c>
     </row>
     <row r="85">
@@ -1611,13 +1611,13 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>1.307663917541504</v>
+        <v>-1.628491878509521</v>
       </c>
       <c r="C85" t="n">
-        <v>1.595051646232605</v>
+        <v>2.35552191734314</v>
       </c>
       <c r="D85" t="n">
-        <v>1.144386291503906</v>
+        <v>0.2257018685340881</v>
       </c>
     </row>
     <row r="86">
@@ -1625,13 +1625,13 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>1.199769258499146</v>
+        <v>-1.570354461669922</v>
       </c>
       <c r="C86" t="n">
-        <v>1.55948543548584</v>
+        <v>2.289345026016235</v>
       </c>
       <c r="D86" t="n">
-        <v>1.026269555091858</v>
+        <v>0.2823072969913483</v>
       </c>
     </row>
     <row r="87">
@@ -1639,13 +1639,13 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>1.382409572601318</v>
+        <v>-1.699010372161865</v>
       </c>
       <c r="C87" t="n">
-        <v>1.517946481704712</v>
+        <v>2.455431938171387</v>
       </c>
       <c r="D87" t="n">
-        <v>1.197680711746216</v>
+        <v>0.15760138630867</v>
       </c>
     </row>
     <row r="88">
@@ -1653,13 +1653,13 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>1.268410086631775</v>
+        <v>-2.003421306610107</v>
       </c>
       <c r="C88" t="n">
-        <v>0.7043652534484863</v>
+        <v>2.331815719604492</v>
       </c>
       <c r="D88" t="n">
-        <v>1.1117844581604</v>
+        <v>0.7353770732879639</v>
       </c>
     </row>
     <row r="89">
@@ -1667,13 +1667,13 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>1.396916627883911</v>
+        <v>-1.636141538619995</v>
       </c>
       <c r="C89" t="n">
-        <v>1.605281114578247</v>
+        <v>2.162195205688477</v>
       </c>
       <c r="D89" t="n">
-        <v>1.24239706993103</v>
+        <v>0.3506918251514435</v>
       </c>
     </row>
     <row r="90">
@@ -1681,13 +1681,13 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>1.352335929870605</v>
+        <v>-1.65019416809082</v>
       </c>
       <c r="C90" t="n">
-        <v>1.642978549003601</v>
+        <v>2.200159549713135</v>
       </c>
       <c r="D90" t="n">
-        <v>1.213842153549194</v>
+        <v>0.4149023592472076</v>
       </c>
     </row>
     <row r="91">
@@ -1695,13 +1695,13 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>1.430204391479492</v>
+        <v>-1.845911502838135</v>
       </c>
       <c r="C91" t="n">
-        <v>0.9190539121627808</v>
+        <v>3.407876968383789</v>
       </c>
       <c r="D91" t="n">
-        <v>0.6131792664527893</v>
+        <v>-0.8249303102493286</v>
       </c>
     </row>
     <row r="92">
@@ -1709,13 +1709,13 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>1.0543133020401</v>
+        <v>-1.593366503715515</v>
       </c>
       <c r="C92" t="n">
-        <v>0.8825486898422241</v>
+        <v>2.922791004180908</v>
       </c>
       <c r="D92" t="n">
-        <v>0.6587885022163391</v>
+        <v>-0.2950654029846191</v>
       </c>
     </row>
     <row r="93">
@@ -1723,13 +1723,13 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>1.071239113807678</v>
+        <v>-1.586970448493958</v>
       </c>
       <c r="C93" t="n">
-        <v>1.013058185577393</v>
+        <v>2.905118465423584</v>
       </c>
       <c r="D93" t="n">
-        <v>0.6216095685958862</v>
+        <v>-0.3067135214805603</v>
       </c>
     </row>
     <row r="94">
@@ -1737,13 +1737,13 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>1.122625231742859</v>
+        <v>-1.656199216842651</v>
       </c>
       <c r="C94" t="n">
-        <v>0.9549543857574463</v>
+        <v>3.014358043670654</v>
       </c>
       <c r="D94" t="n">
-        <v>0.7096114158630371</v>
+        <v>-0.2385635375976562</v>
       </c>
     </row>
     <row r="95">
@@ -1751,13 +1751,13 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>1.109021544456482</v>
+        <v>-2.053280115127563</v>
       </c>
       <c r="C95" t="n">
-        <v>0.8717786073684692</v>
+        <v>2.951084613800049</v>
       </c>
       <c r="D95" t="n">
-        <v>0.8313714861869812</v>
+        <v>-0.04589628428220749</v>
       </c>
     </row>
     <row r="96">
@@ -1765,13 +1765,13 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>1.376821160316467</v>
+        <v>-1.73750901222229</v>
       </c>
       <c r="C96" t="n">
-        <v>1.643838047981262</v>
+        <v>2.908074855804443</v>
       </c>
       <c r="D96" t="n">
-        <v>1.057790398597717</v>
+        <v>-0.8872619867324829</v>
       </c>
     </row>
     <row r="97">
@@ -1779,13 +1779,13 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>1.355890870094299</v>
+        <v>-1.780130982398987</v>
       </c>
       <c r="C97" t="n">
-        <v>1.675790905952454</v>
+        <v>2.450564861297607</v>
       </c>
       <c r="D97" t="n">
-        <v>1.23691201210022</v>
+        <v>0.3095099031925201</v>
       </c>
     </row>
     <row r="98">
@@ -1793,13 +1793,13 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>1.170557737350464</v>
+        <v>-1.887764811515808</v>
       </c>
       <c r="C98" t="n">
-        <v>1.105569243431091</v>
+        <v>3.187839984893799</v>
       </c>
       <c r="D98" t="n">
-        <v>0.8687484264373779</v>
+        <v>-0.2156050801277161</v>
       </c>
     </row>
     <row r="99">
@@ -1807,13 +1807,13 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>0.9825742840766907</v>
+        <v>-1.867316722869873</v>
       </c>
       <c r="C99" t="n">
-        <v>1.544201612472534</v>
+        <v>3.353143453598022</v>
       </c>
       <c r="D99" t="n">
-        <v>0.8120055198669434</v>
+        <v>0.1847504377365112</v>
       </c>
     </row>
     <row r="100">
@@ -1821,13 +1821,13 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>1.192088842391968</v>
+        <v>-1.496890068054199</v>
       </c>
       <c r="C100" t="n">
-        <v>1.318864941596985</v>
+        <v>3.266568183898926</v>
       </c>
       <c r="D100" t="n">
-        <v>0.9891304969787598</v>
+        <v>-0.2860920429229736</v>
       </c>
     </row>
     <row r="101">
@@ -1835,13 +1835,13 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>1.211865305900574</v>
+        <v>-0.6310759782791138</v>
       </c>
       <c r="C101" t="n">
-        <v>1.458596348762512</v>
+        <v>2.936360359191895</v>
       </c>
       <c r="D101" t="n">
-        <v>0.7452729940414429</v>
+        <v>-1.074450612068176</v>
       </c>
     </row>
     <row r="102">
@@ -1849,13 +1849,13 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>1.519873857498169</v>
+        <v>-1.372061610221863</v>
       </c>
       <c r="C102" t="n">
-        <v>1.331158876419067</v>
+        <v>2.942946910858154</v>
       </c>
       <c r="D102" t="n">
-        <v>0.9322522282600403</v>
+        <v>-1.269001603126526</v>
       </c>
     </row>
     <row r="103">
@@ -1863,13 +1863,13 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>1.470897555351257</v>
+        <v>-1.387020945549011</v>
       </c>
       <c r="C103" t="n">
-        <v>1.390973925590515</v>
+        <v>3.06696891784668</v>
       </c>
       <c r="D103" t="n">
-        <v>0.8680629730224609</v>
+        <v>-1.022855162620544</v>
       </c>
     </row>
     <row r="104">
@@ -1877,13 +1877,13 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>1.809769034385681</v>
+        <v>-2.159872531890869</v>
       </c>
       <c r="C104" t="n">
-        <v>1.058686971664429</v>
+        <v>3.085267543792725</v>
       </c>
       <c r="D104" t="n">
-        <v>1.468475341796875</v>
+        <v>0.1878882050514221</v>
       </c>
     </row>
     <row r="105">
@@ -1891,13 +1891,13 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>1.589665293693542</v>
+        <v>-1.638098120689392</v>
       </c>
       <c r="C105" t="n">
-        <v>1.549652218818665</v>
+        <v>2.889097452163696</v>
       </c>
       <c r="D105" t="n">
-        <v>1.158284306526184</v>
+        <v>-0.2802909016609192</v>
       </c>
     </row>
     <row r="106">
@@ -1905,13 +1905,13 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>0.8239054083824158</v>
+        <v>-1.598346948623657</v>
       </c>
       <c r="C106" t="n">
-        <v>0.8499857187271118</v>
+        <v>3.112810850143433</v>
       </c>
       <c r="D106" t="n">
-        <v>0.4693102836608887</v>
+        <v>-0.6549816131591797</v>
       </c>
     </row>
     <row r="107">
@@ -1919,13 +1919,13 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>1.024374842643738</v>
+        <v>-1.732353091239929</v>
       </c>
       <c r="C107" t="n">
-        <v>0.8772999048233032</v>
+        <v>3.266454935073853</v>
       </c>
       <c r="D107" t="n">
-        <v>0.5714027285575867</v>
+        <v>-0.5796715617179871</v>
       </c>
     </row>
     <row r="108">
@@ -1933,13 +1933,13 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>1.260234832763672</v>
+        <v>-2.122333765029907</v>
       </c>
       <c r="C108" t="n">
-        <v>0.5600496530532837</v>
+        <v>3.421588897705078</v>
       </c>
       <c r="D108" t="n">
-        <v>0.9083471894264221</v>
+        <v>0.1676618456840515</v>
       </c>
     </row>
     <row r="109">
@@ -1947,13 +1947,13 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>1.621909856796265</v>
+        <v>-1.750489234924316</v>
       </c>
       <c r="C109" t="n">
-        <v>1.171980500221252</v>
+        <v>3.032720565795898</v>
       </c>
       <c r="D109" t="n">
-        <v>1.04813539981842</v>
+        <v>-0.653384804725647</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2022/11.09 16:21 update ae intersect
</commit_message>
<xml_diff>
--- a/documents/latent_vector/dqn_enc.xlsx
+++ b/documents/latent_vector/dqn_enc.xlsx
@@ -449,13 +449,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>-1.788830041885376</v>
+        <v>0.2664260864257812</v>
       </c>
       <c r="C2" t="n">
-        <v>2.761813163757324</v>
+        <v>0.648847222328186</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1770073771476746</v>
+        <v>0.006257821805775166</v>
       </c>
     </row>
     <row r="3">
@@ -463,13 +463,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-1.796534776687622</v>
+        <v>0.2685320973396301</v>
       </c>
       <c r="C3" t="n">
-        <v>2.82730770111084</v>
+        <v>0.6317225694656372</v>
       </c>
       <c r="D3" t="n">
-        <v>0.02859849482774734</v>
+        <v>-0.0004622291307896376</v>
       </c>
     </row>
     <row r="4">
@@ -477,13 +477,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-1.785569071769714</v>
+        <v>0.2612994909286499</v>
       </c>
       <c r="C4" t="n">
-        <v>2.735684394836426</v>
+        <v>0.6445318460464478</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2609202265739441</v>
+        <v>0.005507540889084339</v>
       </c>
     </row>
     <row r="5">
@@ -491,13 +491,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-1.793572783470154</v>
+        <v>0.2735463082790375</v>
       </c>
       <c r="C5" t="n">
-        <v>2.871055126190186</v>
+        <v>0.6667757034301758</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.1036283895373344</v>
+        <v>0.001726453425362706</v>
       </c>
     </row>
     <row r="6">
@@ -505,13 +505,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.770533204078674</v>
+        <v>0.2817603945732117</v>
       </c>
       <c r="C6" t="n">
-        <v>2.83265495300293</v>
+        <v>0.6681255698204041</v>
       </c>
       <c r="D6" t="n">
-        <v>0.05916494876146317</v>
+        <v>0.03344858810305595</v>
       </c>
     </row>
     <row r="7">
@@ -519,13 +519,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-1.74581241607666</v>
+        <v>0.2638928592205048</v>
       </c>
       <c r="C7" t="n">
-        <v>2.842475414276123</v>
+        <v>0.6673364043235779</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.1689754724502563</v>
+        <v>0.02527406625449657</v>
       </c>
     </row>
     <row r="8">
@@ -533,13 +533,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-1.803113222122192</v>
+        <v>0.2702624201774597</v>
       </c>
       <c r="C8" t="n">
-        <v>2.7734055519104</v>
+        <v>0.6472333073616028</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3271746635437012</v>
+        <v>0.0133428992703557</v>
       </c>
     </row>
     <row r="9">
@@ -547,13 +547,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>-1.759005308151245</v>
+        <v>0.2650624811649323</v>
       </c>
       <c r="C9" t="n">
-        <v>2.781376123428345</v>
+        <v>0.6631730198860168</v>
       </c>
       <c r="D9" t="n">
-        <v>0.1302592158317566</v>
+        <v>0.01029693800956011</v>
       </c>
     </row>
     <row r="10">
@@ -561,13 +561,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-1.83262026309967</v>
+        <v>0.2627106308937073</v>
       </c>
       <c r="C10" t="n">
-        <v>2.703132629394531</v>
+        <v>0.6413992643356323</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4844480752944946</v>
+        <v>0.004524593241512775</v>
       </c>
     </row>
     <row r="11">
@@ -575,13 +575,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-1.457583546638489</v>
+        <v>0.2833506166934967</v>
       </c>
       <c r="C11" t="n">
-        <v>2.556679964065552</v>
+        <v>0.6797158122062683</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.5258376598358154</v>
+        <v>-0.04492827877402306</v>
       </c>
     </row>
     <row r="12">
@@ -589,13 +589,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>-1.954383373260498</v>
+        <v>0.2460916340351105</v>
       </c>
       <c r="C12" t="n">
-        <v>2.729389190673828</v>
+        <v>0.6257547736167908</v>
       </c>
       <c r="D12" t="n">
-        <v>0.4875642061233521</v>
+        <v>-0.004036027006804943</v>
       </c>
     </row>
     <row r="13">
@@ -603,13 +603,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>-1.828346014022827</v>
+        <v>0.2692782878875732</v>
       </c>
       <c r="C13" t="n">
-        <v>2.848395824432373</v>
+        <v>0.6775692701339722</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.1539393067359924</v>
+        <v>-0.02587408758699894</v>
       </c>
     </row>
     <row r="14">
@@ -617,13 +617,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>-1.813822507858276</v>
+        <v>0.251497358083725</v>
       </c>
       <c r="C14" t="n">
-        <v>2.733080863952637</v>
+        <v>0.6415874361991882</v>
       </c>
       <c r="D14" t="n">
-        <v>0.2041867077350616</v>
+        <v>-0.0008179049473255873</v>
       </c>
     </row>
     <row r="15">
@@ -631,13 +631,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>-1.862646460533142</v>
+        <v>0.2605743408203125</v>
       </c>
       <c r="C15" t="n">
-        <v>2.742291927337646</v>
+        <v>0.674394428730011</v>
       </c>
       <c r="D15" t="n">
-        <v>0.2659146785736084</v>
+        <v>-0.005164711736142635</v>
       </c>
     </row>
     <row r="16">
@@ -645,13 +645,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>-1.905779361724854</v>
+        <v>0.2492799907922745</v>
       </c>
       <c r="C16" t="n">
-        <v>2.822513341903687</v>
+        <v>0.7193794250488281</v>
       </c>
       <c r="D16" t="n">
-        <v>0.06902862340211868</v>
+        <v>0.04309358447790146</v>
       </c>
     </row>
     <row r="17">
@@ -659,13 +659,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>-1.936476230621338</v>
+        <v>0.2360272705554962</v>
       </c>
       <c r="C17" t="n">
-        <v>2.858734369277954</v>
+        <v>0.7315543293952942</v>
       </c>
       <c r="D17" t="n">
-        <v>0.2884494662284851</v>
+        <v>0.08003737032413483</v>
       </c>
     </row>
     <row r="18">
@@ -673,13 +673,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>-1.896460771560669</v>
+        <v>0.2504982948303223</v>
       </c>
       <c r="C18" t="n">
-        <v>2.816331148147583</v>
+        <v>0.7065553665161133</v>
       </c>
       <c r="D18" t="n">
-        <v>0.2293068170547485</v>
+        <v>0.01061974186450243</v>
       </c>
     </row>
     <row r="19">
@@ -687,13 +687,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>-1.797838449478149</v>
+        <v>0.2631286382675171</v>
       </c>
       <c r="C19" t="n">
-        <v>2.816625118255615</v>
+        <v>0.6587488055229187</v>
       </c>
       <c r="D19" t="n">
-        <v>0.1870786547660828</v>
+        <v>0.01003144402056932</v>
       </c>
     </row>
     <row r="20">
@@ -701,13 +701,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>-1.714102745056152</v>
+        <v>0.2744163572788239</v>
       </c>
       <c r="C20" t="n">
-        <v>2.721461772918701</v>
+        <v>0.6667273044586182</v>
       </c>
       <c r="D20" t="n">
-        <v>0.01620126515626907</v>
+        <v>0.002296773018315434</v>
       </c>
     </row>
     <row r="21">
@@ -715,13 +715,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>-1.670921921730042</v>
+        <v>0.2809521555900574</v>
       </c>
       <c r="C21" t="n">
-        <v>2.647699117660522</v>
+        <v>0.6843045353889465</v>
       </c>
       <c r="D21" t="n">
-        <v>0.04934734851121902</v>
+        <v>0.01586962677538395</v>
       </c>
     </row>
     <row r="22">
@@ -729,13 +729,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>-1.694433689117432</v>
+        <v>0.2532158195972443</v>
       </c>
       <c r="C22" t="n">
-        <v>2.7182776927948</v>
+        <v>0.6412532925605774</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.1850286722183228</v>
+        <v>0.03109738789498806</v>
       </c>
     </row>
     <row r="23">
@@ -743,13 +743,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>-1.50579845905304</v>
+        <v>0.2571897506713867</v>
       </c>
       <c r="C23" t="n">
-        <v>2.574104309082031</v>
+        <v>0.675843358039856</v>
       </c>
       <c r="D23" t="n">
-        <v>-0.01574056595563889</v>
+        <v>0.006066803820431232</v>
       </c>
     </row>
     <row r="24">
@@ -757,13 +757,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>-1.752907991409302</v>
+        <v>0.2605628371238708</v>
       </c>
       <c r="C24" t="n">
-        <v>2.785487174987793</v>
+        <v>0.6730467677116394</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.1700379848480225</v>
+        <v>0.002613698365166783</v>
       </c>
     </row>
     <row r="25">
@@ -771,13 +771,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>-1.694122076034546</v>
+        <v>0.2463047355413437</v>
       </c>
       <c r="C25" t="n">
-        <v>2.614879608154297</v>
+        <v>0.6194472312927246</v>
       </c>
       <c r="D25" t="n">
-        <v>0.1937214732170105</v>
+        <v>0.0214551780372858</v>
       </c>
     </row>
     <row r="26">
@@ -785,13 +785,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>-1.788387298583984</v>
+        <v>0.2472080737352371</v>
       </c>
       <c r="C26" t="n">
-        <v>2.68560791015625</v>
+        <v>0.6511561274528503</v>
       </c>
       <c r="D26" t="n">
-        <v>0.1549782752990723</v>
+        <v>0.02218163572251797</v>
       </c>
     </row>
     <row r="27">
@@ -799,13 +799,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>-1.748939871788025</v>
+        <v>0.2366319000720978</v>
       </c>
       <c r="C27" t="n">
-        <v>2.832392454147339</v>
+        <v>0.6454380750656128</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.1472378373146057</v>
+        <v>0.030525928363204</v>
       </c>
     </row>
     <row r="28">
@@ -813,13 +813,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>-1.791444897651672</v>
+        <v>0.2622062861919403</v>
       </c>
       <c r="C28" t="n">
-        <v>2.909592390060425</v>
+        <v>0.6235539317131042</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.3206140995025635</v>
+        <v>0.003572893561795354</v>
       </c>
     </row>
     <row r="29">
@@ -827,13 +827,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>-1.723034858703613</v>
+        <v>0.2783145010471344</v>
       </c>
       <c r="C29" t="n">
-        <v>2.82050895690918</v>
+        <v>0.6491417288780212</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.521527886390686</v>
+        <v>-0.009267206303775311</v>
       </c>
     </row>
     <row r="30">
@@ -841,13 +841,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>-1.824654221534729</v>
+        <v>0.2809744477272034</v>
       </c>
       <c r="C30" t="n">
-        <v>2.908658027648926</v>
+        <v>0.6393743753433228</v>
       </c>
       <c r="D30" t="n">
-        <v>-0.5327010154724121</v>
+        <v>-0.01747854985296726</v>
       </c>
     </row>
     <row r="31">
@@ -855,13 +855,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>-1.83190929889679</v>
+        <v>0.2675471007823944</v>
       </c>
       <c r="C31" t="n">
-        <v>2.871374845504761</v>
+        <v>0.6116402149200439</v>
       </c>
       <c r="D31" t="n">
-        <v>-0.253440260887146</v>
+        <v>-0.01962635107338428</v>
       </c>
     </row>
     <row r="32">
@@ -869,13 +869,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>-1.763830900192261</v>
+        <v>0.2820245921611786</v>
       </c>
       <c r="C32" t="n">
-        <v>2.842137813568115</v>
+        <v>0.6476053595542908</v>
       </c>
       <c r="D32" t="n">
-        <v>-0.5144026875495911</v>
+        <v>-0.02070611901581287</v>
       </c>
     </row>
     <row r="33">
@@ -883,13 +883,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>-1.797590017318726</v>
+        <v>0.255298376083374</v>
       </c>
       <c r="C33" t="n">
-        <v>2.880486726760864</v>
+        <v>0.6067289710044861</v>
       </c>
       <c r="D33" t="n">
-        <v>-0.4107177257537842</v>
+        <v>-0.02059216983616352</v>
       </c>
     </row>
     <row r="34">
@@ -897,13 +897,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>-1.725706338882446</v>
+        <v>0.257289707660675</v>
       </c>
       <c r="C34" t="n">
-        <v>2.95784592628479</v>
+        <v>0.6041221022605896</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.6732915639877319</v>
+        <v>-0.0243732426315546</v>
       </c>
     </row>
     <row r="35">
@@ -911,13 +911,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>-1.583881497383118</v>
+        <v>0.220881387591362</v>
       </c>
       <c r="C35" t="n">
-        <v>2.828881025314331</v>
+        <v>0.6232128739356995</v>
       </c>
       <c r="D35" t="n">
-        <v>-0.450782299041748</v>
+        <v>0.006093484349548817</v>
       </c>
     </row>
     <row r="36">
@@ -925,13 +925,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>-1.64953088760376</v>
+        <v>0.2232494801282883</v>
       </c>
       <c r="C36" t="n">
-        <v>2.711163282394409</v>
+        <v>0.6153203845024109</v>
       </c>
       <c r="D36" t="n">
-        <v>-0.1956029534339905</v>
+        <v>0.03371736034750938</v>
       </c>
     </row>
     <row r="37">
@@ -939,13 +939,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>-1.687301397323608</v>
+        <v>0.2781234085559845</v>
       </c>
       <c r="C37" t="n">
-        <v>2.524833917617798</v>
+        <v>0.6395302414894104</v>
       </c>
       <c r="D37" t="n">
-        <v>0.249151200056076</v>
+        <v>-0.006170745007693768</v>
       </c>
     </row>
     <row r="38">
@@ -953,13 +953,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>-1.820557475090027</v>
+        <v>0.2940637469291687</v>
       </c>
       <c r="C38" t="n">
-        <v>2.635960102081299</v>
+        <v>0.6250672340393066</v>
       </c>
       <c r="D38" t="n">
-        <v>0.2984968423843384</v>
+        <v>-0.04447906464338303</v>
       </c>
     </row>
     <row r="39">
@@ -967,13 +967,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>-1.735683798789978</v>
+        <v>0.2946504354476929</v>
       </c>
       <c r="C39" t="n">
-        <v>2.649903297424316</v>
+        <v>0.6589730381965637</v>
       </c>
       <c r="D39" t="n">
-        <v>-0.01994150131940842</v>
+        <v>0.01015757489949465</v>
       </c>
     </row>
     <row r="40">
@@ -981,13 +981,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>-1.743956685066223</v>
+        <v>0.3088955283164978</v>
       </c>
       <c r="C40" t="n">
-        <v>2.58085823059082</v>
+        <v>0.6672388315200806</v>
       </c>
       <c r="D40" t="n">
-        <v>-0.00471138209104538</v>
+        <v>-0.01201942097395658</v>
       </c>
     </row>
     <row r="41">
@@ -995,13 +995,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>-1.740137934684753</v>
+        <v>0.3115738034248352</v>
       </c>
       <c r="C41" t="n">
-        <v>2.664073467254639</v>
+        <v>0.6759269833564758</v>
       </c>
       <c r="D41" t="n">
-        <v>-0.211656928062439</v>
+        <v>-0.009336180053651333</v>
       </c>
     </row>
     <row r="42">
@@ -1009,13 +1009,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>-1.818404197692871</v>
+        <v>0.2933615148067474</v>
       </c>
       <c r="C42" t="n">
-        <v>2.754018306732178</v>
+        <v>0.6040554642677307</v>
       </c>
       <c r="D42" t="n">
-        <v>-0.02618073672056198</v>
+        <v>-0.005730926059186459</v>
       </c>
     </row>
     <row r="43">
@@ -1023,13 +1023,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>-1.780189156532288</v>
+        <v>0.2915279269218445</v>
       </c>
       <c r="C43" t="n">
-        <v>2.742386341094971</v>
+        <v>0.6482939124107361</v>
       </c>
       <c r="D43" t="n">
-        <v>-0.128812313079834</v>
+        <v>0.01159847993403673</v>
       </c>
     </row>
     <row r="44">
@@ -1037,13 +1037,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>-1.870034337043762</v>
+        <v>0.3013015389442444</v>
       </c>
       <c r="C44" t="n">
-        <v>2.626907587051392</v>
+        <v>0.6537688970565796</v>
       </c>
       <c r="D44" t="n">
-        <v>0.2048396170139313</v>
+        <v>-0.03122072853147984</v>
       </c>
     </row>
     <row r="45">
@@ -1051,13 +1051,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>-1.745854616165161</v>
+        <v>0.2963208556175232</v>
       </c>
       <c r="C45" t="n">
-        <v>2.425479412078857</v>
+        <v>0.6096335649490356</v>
       </c>
       <c r="D45" t="n">
-        <v>0.6137059926986694</v>
+        <v>-0.0409470722079277</v>
       </c>
     </row>
     <row r="46">
@@ -1065,13 +1065,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>-1.747787356376648</v>
+        <v>0.2977321743965149</v>
       </c>
       <c r="C46" t="n">
-        <v>2.470945596694946</v>
+        <v>0.6120379567146301</v>
       </c>
       <c r="D46" t="n">
-        <v>0.5254042148590088</v>
+        <v>-0.03880958631634712</v>
       </c>
     </row>
     <row r="47">
@@ -1079,13 +1079,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>-1.795293211936951</v>
+        <v>0.297637403011322</v>
       </c>
       <c r="C47" t="n">
-        <v>2.531349658966064</v>
+        <v>0.6145109534263611</v>
       </c>
       <c r="D47" t="n">
-        <v>0.544035017490387</v>
+        <v>-0.03943720459938049</v>
       </c>
     </row>
     <row r="48">
@@ -1093,13 +1093,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>-1.854714870452881</v>
+        <v>0.3001566827297211</v>
       </c>
       <c r="C48" t="n">
-        <v>2.545819282531738</v>
+        <v>0.6191834211349487</v>
       </c>
       <c r="D48" t="n">
-        <v>0.5901591777801514</v>
+        <v>-0.05023006722331047</v>
       </c>
     </row>
     <row r="49">
@@ -1107,13 +1107,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>-1.85335099697113</v>
+        <v>0.2364149838685989</v>
       </c>
       <c r="C49" t="n">
-        <v>2.733589649200439</v>
+        <v>0.638400673866272</v>
       </c>
       <c r="D49" t="n">
-        <v>0.1422341465950012</v>
+        <v>0.03257723525166512</v>
       </c>
     </row>
     <row r="50">
@@ -1121,13 +1121,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>-1.817363500595093</v>
+        <v>0.3181438446044922</v>
       </c>
       <c r="C50" t="n">
-        <v>3.222140312194824</v>
+        <v>0.7626717686653137</v>
       </c>
       <c r="D50" t="n">
-        <v>-1.350210428237915</v>
+        <v>-0.06358947604894638</v>
       </c>
     </row>
     <row r="51">
@@ -1135,13 +1135,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>-1.500515103340149</v>
+        <v>0.2895421981811523</v>
       </c>
       <c r="C51" t="n">
-        <v>2.676211595535278</v>
+        <v>0.6459152102470398</v>
       </c>
       <c r="D51" t="n">
-        <v>0.04436785727739334</v>
+        <v>0.04735403135418892</v>
       </c>
     </row>
     <row r="52">
@@ -1149,13 +1149,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>-1.693747162818909</v>
+        <v>0.2630741596221924</v>
       </c>
       <c r="C52" t="n">
-        <v>2.710513114929199</v>
+        <v>0.6273863315582275</v>
       </c>
       <c r="D52" t="n">
-        <v>0.1641238033771515</v>
+        <v>0.06460031867027283</v>
       </c>
     </row>
     <row r="53">
@@ -1163,13 +1163,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>-1.859506607055664</v>
+        <v>0.3802274465560913</v>
       </c>
       <c r="C53" t="n">
-        <v>3.216312885284424</v>
+        <v>0.7616562843322754</v>
       </c>
       <c r="D53" t="n">
-        <v>-1.568763613700867</v>
+        <v>-0.07184354960918427</v>
       </c>
     </row>
     <row r="54">
@@ -1177,13 +1177,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>-1.306578159332275</v>
+        <v>0.2757600247859955</v>
       </c>
       <c r="C54" t="n">
-        <v>2.020320415496826</v>
+        <v>0.7006799578666687</v>
       </c>
       <c r="D54" t="n">
-        <v>-0.3541139960289001</v>
+        <v>0.0312936045229435</v>
       </c>
     </row>
     <row r="55">
@@ -1191,13 +1191,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>-1.646723628044128</v>
+        <v>0.3277468085289001</v>
       </c>
       <c r="C55" t="n">
-        <v>2.546635389328003</v>
+        <v>0.7888743877410889</v>
       </c>
       <c r="D55" t="n">
-        <v>-1.053088307380676</v>
+        <v>0.07694433629512787</v>
       </c>
     </row>
     <row r="56">
@@ -1205,13 +1205,13 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>-1.745261430740356</v>
+        <v>0.3012381196022034</v>
       </c>
       <c r="C56" t="n">
-        <v>3.256208419799805</v>
+        <v>0.6688922643661499</v>
       </c>
       <c r="D56" t="n">
-        <v>-0.3198471069335938</v>
+        <v>-0.05056856200098991</v>
       </c>
     </row>
     <row r="57">
@@ -1219,13 +1219,13 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>-1.526459455490112</v>
+        <v>0.2903702557086945</v>
       </c>
       <c r="C57" t="n">
-        <v>2.477005481719971</v>
+        <v>0.6197267174720764</v>
       </c>
       <c r="D57" t="n">
-        <v>0.3343901336193085</v>
+        <v>-0.0126697076484561</v>
       </c>
     </row>
     <row r="58">
@@ -1233,13 +1233,13 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>-1.680849075317383</v>
+        <v>0.2776203751564026</v>
       </c>
       <c r="C58" t="n">
-        <v>2.760564804077148</v>
+        <v>0.6252539157867432</v>
       </c>
       <c r="D58" t="n">
-        <v>0.1077770665287971</v>
+        <v>-0.01979565061628819</v>
       </c>
     </row>
     <row r="59">
@@ -1247,13 +1247,13 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>-1.806389212608337</v>
+        <v>0.2697232067584991</v>
       </c>
       <c r="C59" t="n">
-        <v>3.061006546020508</v>
+        <v>0.6948001384735107</v>
       </c>
       <c r="D59" t="n">
-        <v>-0.1978790163993835</v>
+        <v>0.0410330556333065</v>
       </c>
     </row>
     <row r="60">
@@ -1261,13 +1261,13 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>-2.00287127494812</v>
+        <v>0.328652560710907</v>
       </c>
       <c r="C60" t="n">
-        <v>3.450778007507324</v>
+        <v>0.7788655161857605</v>
       </c>
       <c r="D60" t="n">
-        <v>-1.019535303115845</v>
+        <v>-0.04485651478171349</v>
       </c>
     </row>
     <row r="61">
@@ -1275,13 +1275,13 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>-1.84800910949707</v>
+        <v>0.2802637815475464</v>
       </c>
       <c r="C61" t="n">
-        <v>3.443219184875488</v>
+        <v>0.6914541125297546</v>
       </c>
       <c r="D61" t="n">
-        <v>-0.4980486631393433</v>
+        <v>-0.01934750191867352</v>
       </c>
     </row>
     <row r="62">
@@ -1289,13 +1289,13 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>-1.952149510383606</v>
+        <v>0.309709757566452</v>
       </c>
       <c r="C62" t="n">
-        <v>3.414097309112549</v>
+        <v>0.6786558032035828</v>
       </c>
       <c r="D62" t="n">
-        <v>0.04054272919893265</v>
+        <v>-0.03649889305233955</v>
       </c>
     </row>
     <row r="63">
@@ -1303,13 +1303,13 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>-1.708168506622314</v>
+        <v>0.3309531211853027</v>
       </c>
       <c r="C63" t="n">
-        <v>2.518898487091064</v>
+        <v>0.7585431337356567</v>
       </c>
       <c r="D63" t="n">
-        <v>0.7887579798698425</v>
+        <v>0.04927822574973106</v>
       </c>
     </row>
     <row r="64">
@@ -1317,13 +1317,13 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>-1.145947217941284</v>
+        <v>0.2778111398220062</v>
       </c>
       <c r="C64" t="n">
-        <v>2.21372127532959</v>
+        <v>0.6507033705711365</v>
       </c>
       <c r="D64" t="n">
-        <v>-0.3564375042915344</v>
+        <v>-0.04148483648896217</v>
       </c>
     </row>
     <row r="65">
@@ -1331,13 +1331,13 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>-1.35295581817627</v>
+        <v>0.2704644203186035</v>
       </c>
       <c r="C65" t="n">
-        <v>2.423404932022095</v>
+        <v>0.5882279276847839</v>
       </c>
       <c r="D65" t="n">
-        <v>0.5142398476600647</v>
+        <v>-0.01401156466454268</v>
       </c>
     </row>
     <row r="66">
@@ -1345,13 +1345,13 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>-1.492993116378784</v>
+        <v>0.2938117384910583</v>
       </c>
       <c r="C66" t="n">
-        <v>2.278056621551514</v>
+        <v>0.6004683375358582</v>
       </c>
       <c r="D66" t="n">
-        <v>0.959328293800354</v>
+        <v>-0.04677809029817581</v>
       </c>
     </row>
     <row r="67">
@@ -1359,13 +1359,13 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>-1.651567697525024</v>
+        <v>0.243002250790596</v>
       </c>
       <c r="C67" t="n">
-        <v>2.619035482406616</v>
+        <v>0.5443406105041504</v>
       </c>
       <c r="D67" t="n">
-        <v>-0.4180133640766144</v>
+        <v>0.02213357202708721</v>
       </c>
     </row>
     <row r="68">
@@ -1373,13 +1373,13 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>-1.598899126052856</v>
+        <v>0.1544641554355621</v>
       </c>
       <c r="C68" t="n">
-        <v>2.878891944885254</v>
+        <v>0.626908004283905</v>
       </c>
       <c r="D68" t="n">
-        <v>-0.9151967167854309</v>
+        <v>0.08464200794696808</v>
       </c>
     </row>
     <row r="69">
@@ -1387,13 +1387,13 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>-1.421025276184082</v>
+        <v>0.2766607999801636</v>
       </c>
       <c r="C69" t="n">
-        <v>2.479530096054077</v>
+        <v>0.6093487143516541</v>
       </c>
       <c r="D69" t="n">
-        <v>0.5023493766784668</v>
+        <v>-0.01282935123890638</v>
       </c>
     </row>
     <row r="70">
@@ -1401,13 +1401,13 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>-1.784129738807678</v>
+        <v>0.2291892766952515</v>
       </c>
       <c r="C70" t="n">
-        <v>2.909031629562378</v>
+        <v>0.6763365864753723</v>
       </c>
       <c r="D70" t="n">
-        <v>-0.1432114839553833</v>
+        <v>0.06174615398049355</v>
       </c>
     </row>
     <row r="71">
@@ -1415,13 +1415,13 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>-1.721899390220642</v>
+        <v>0.2291549146175385</v>
       </c>
       <c r="C71" t="n">
-        <v>3.051913261413574</v>
+        <v>0.6336483955383301</v>
       </c>
       <c r="D71" t="n">
-        <v>-0.4195650219917297</v>
+        <v>0.04827026650309563</v>
       </c>
     </row>
     <row r="72">
@@ -1429,13 +1429,13 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>-1.535071015357971</v>
+        <v>0.2522068321704865</v>
       </c>
       <c r="C72" t="n">
-        <v>2.846559286117554</v>
+        <v>0.5857676267623901</v>
       </c>
       <c r="D72" t="n">
-        <v>-0.3042086362838745</v>
+        <v>0.05672628059983253</v>
       </c>
     </row>
     <row r="73">
@@ -1443,13 +1443,13 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>-1.588250398635864</v>
+        <v>0.2455205172300339</v>
       </c>
       <c r="C73" t="n">
-        <v>2.764822006225586</v>
+        <v>0.5851485729217529</v>
       </c>
       <c r="D73" t="n">
-        <v>0.1498149335384369</v>
+        <v>0.02929545007646084</v>
       </c>
     </row>
     <row r="74">
@@ -1457,13 +1457,13 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>-1.439719915390015</v>
+        <v>0.2489051073789597</v>
       </c>
       <c r="C74" t="n">
-        <v>2.563395261764526</v>
+        <v>0.5929679870605469</v>
       </c>
       <c r="D74" t="n">
-        <v>0.4454854130744934</v>
+        <v>0.01280758995562792</v>
       </c>
     </row>
     <row r="75">
@@ -1471,13 +1471,13 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>-1.391136407852173</v>
+        <v>0.2900951504707336</v>
       </c>
       <c r="C75" t="n">
-        <v>2.362955093383789</v>
+        <v>0.6063517332077026</v>
       </c>
       <c r="D75" t="n">
-        <v>0.6192845702171326</v>
+        <v>-0.03421608731150627</v>
       </c>
     </row>
     <row r="76">
@@ -1485,13 +1485,13 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>-1.633471131324768</v>
+        <v>0.2646459937095642</v>
       </c>
       <c r="C76" t="n">
-        <v>2.718760251998901</v>
+        <v>0.6510897278785706</v>
       </c>
       <c r="D76" t="n">
-        <v>0.5195736885070801</v>
+        <v>-0.01787109114229679</v>
       </c>
     </row>
     <row r="77">
@@ -1499,13 +1499,13 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>-1.563079357147217</v>
+        <v>0.2612802684307098</v>
       </c>
       <c r="C77" t="n">
-        <v>2.102933645248413</v>
+        <v>0.6430612802505493</v>
       </c>
       <c r="D77" t="n">
-        <v>0.2035261988639832</v>
+        <v>-0.002751069841906428</v>
       </c>
     </row>
     <row r="78">
@@ -1513,13 +1513,13 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>-1.452157258987427</v>
+        <v>0.2589626610279083</v>
       </c>
       <c r="C78" t="n">
-        <v>2.15067720413208</v>
+        <v>0.6299439072608948</v>
       </c>
       <c r="D78" t="n">
-        <v>0.3720082640647888</v>
+        <v>-0.01124752592295408</v>
       </c>
     </row>
     <row r="79">
@@ -1527,13 +1527,13 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>-1.908830881118774</v>
+        <v>0.2354486584663391</v>
       </c>
       <c r="C79" t="n">
-        <v>3.26392674446106</v>
+        <v>0.6984711885452271</v>
       </c>
       <c r="D79" t="n">
-        <v>-0.358924925327301</v>
+        <v>0.05917864665389061</v>
       </c>
     </row>
     <row r="80">
@@ -1541,13 +1541,13 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>-1.42959725856781</v>
+        <v>0.2932033240795135</v>
       </c>
       <c r="C80" t="n">
-        <v>1.855496883392334</v>
+        <v>0.6488298177719116</v>
       </c>
       <c r="D80" t="n">
-        <v>0.1648955941200256</v>
+        <v>-0.02532858215272427</v>
       </c>
     </row>
     <row r="81">
@@ -1555,13 +1555,13 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>-1.561155319213867</v>
+        <v>0.2741170823574066</v>
       </c>
       <c r="C81" t="n">
-        <v>2.038600444793701</v>
+        <v>0.6358624696731567</v>
       </c>
       <c r="D81" t="n">
-        <v>0.3416443467140198</v>
+        <v>-0.03057688660919666</v>
       </c>
     </row>
     <row r="82">
@@ -1569,13 +1569,13 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>-1.561890840530396</v>
+        <v>0.3075407147407532</v>
       </c>
       <c r="C82" t="n">
-        <v>2.409461736679077</v>
+        <v>0.6215934157371521</v>
       </c>
       <c r="D82" t="n">
-        <v>0.5335104465484619</v>
+        <v>-0.009303535334765911</v>
       </c>
     </row>
     <row r="83">
@@ -1583,13 +1583,13 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>-1.667166709899902</v>
+        <v>0.3446000516414642</v>
       </c>
       <c r="C83" t="n">
-        <v>2.339317798614502</v>
+        <v>0.6564664244651794</v>
       </c>
       <c r="D83" t="n">
-        <v>0.3354045450687408</v>
+        <v>-0.01097910758107901</v>
       </c>
     </row>
     <row r="84">
@@ -1597,13 +1597,13 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>-1.470922470092773</v>
+        <v>0.3271609544754028</v>
       </c>
       <c r="C84" t="n">
-        <v>2.713351249694824</v>
+        <v>0.7200009226799011</v>
       </c>
       <c r="D84" t="n">
-        <v>-0.3337305188179016</v>
+        <v>-0.006261053495109081</v>
       </c>
     </row>
     <row r="85">
@@ -1611,13 +1611,13 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>-1.628491878509521</v>
+        <v>0.3438205718994141</v>
       </c>
       <c r="C85" t="n">
-        <v>2.35552191734314</v>
+        <v>0.645734965801239</v>
       </c>
       <c r="D85" t="n">
-        <v>0.2257018685340881</v>
+        <v>-0.03103981353342533</v>
       </c>
     </row>
     <row r="86">
@@ -1625,13 +1625,13 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>-1.570354461669922</v>
+        <v>0.3308832049369812</v>
       </c>
       <c r="C86" t="n">
-        <v>2.289345026016235</v>
+        <v>0.6503903865814209</v>
       </c>
       <c r="D86" t="n">
-        <v>0.2823072969913483</v>
+        <v>-0.03756753727793694</v>
       </c>
     </row>
     <row r="87">
@@ -1639,13 +1639,13 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>-1.699010372161865</v>
+        <v>0.3368951082229614</v>
       </c>
       <c r="C87" t="n">
-        <v>2.455431938171387</v>
+        <v>0.6615633368492126</v>
       </c>
       <c r="D87" t="n">
-        <v>0.15760138630867</v>
+        <v>-0.001027296064421535</v>
       </c>
     </row>
     <row r="88">
@@ -1653,13 +1653,13 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>-2.003421306610107</v>
+        <v>0.3093470931053162</v>
       </c>
       <c r="C88" t="n">
-        <v>2.331815719604492</v>
+        <v>0.6742972731590271</v>
       </c>
       <c r="D88" t="n">
-        <v>0.7353770732879639</v>
+        <v>-0.1017387807369232</v>
       </c>
     </row>
     <row r="89">
@@ -1667,13 +1667,13 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>-1.636141538619995</v>
+        <v>0.328909695148468</v>
       </c>
       <c r="C89" t="n">
-        <v>2.162195205688477</v>
+        <v>0.6559138894081116</v>
       </c>
       <c r="D89" t="n">
-        <v>0.3506918251514435</v>
+        <v>-0.03054380975663662</v>
       </c>
     </row>
     <row r="90">
@@ -1681,13 +1681,13 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>-1.65019416809082</v>
+        <v>0.323961466550827</v>
       </c>
       <c r="C90" t="n">
-        <v>2.200159549713135</v>
+        <v>0.6420326828956604</v>
       </c>
       <c r="D90" t="n">
-        <v>0.4149023592472076</v>
+        <v>-0.01371017005294561</v>
       </c>
     </row>
     <row r="91">
@@ -1695,13 +1695,13 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>-1.845911502838135</v>
+        <v>0.1858139932155609</v>
       </c>
       <c r="C91" t="n">
-        <v>3.407876968383789</v>
+        <v>0.6684508919715881</v>
       </c>
       <c r="D91" t="n">
-        <v>-0.8249303102493286</v>
+        <v>-0.0123892230913043</v>
       </c>
     </row>
     <row r="92">
@@ -1709,13 +1709,13 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>-1.593366503715515</v>
+        <v>0.113928385078907</v>
       </c>
       <c r="C92" t="n">
-        <v>2.922791004180908</v>
+        <v>0.5926311016082764</v>
       </c>
       <c r="D92" t="n">
-        <v>-0.2950654029846191</v>
+        <v>0.03954857960343361</v>
       </c>
     </row>
     <row r="93">
@@ -1723,13 +1723,13 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>-1.586970448493958</v>
+        <v>0.1463579088449478</v>
       </c>
       <c r="C93" t="n">
-        <v>2.905118465423584</v>
+        <v>0.6002684831619263</v>
       </c>
       <c r="D93" t="n">
-        <v>-0.3067135214805603</v>
+        <v>0.005467464216053486</v>
       </c>
     </row>
     <row r="94">
@@ -1737,13 +1737,13 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>-1.656199216842651</v>
+        <v>0.1251584738492966</v>
       </c>
       <c r="C94" t="n">
-        <v>3.014358043670654</v>
+        <v>0.5876222252845764</v>
       </c>
       <c r="D94" t="n">
-        <v>-0.2385635375976562</v>
+        <v>0.03570344671607018</v>
       </c>
     </row>
     <row r="95">
@@ -1751,13 +1751,13 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>-2.053280115127563</v>
+        <v>0.2653766572475433</v>
       </c>
       <c r="C95" t="n">
-        <v>2.951084613800049</v>
+        <v>0.7161501049995422</v>
       </c>
       <c r="D95" t="n">
-        <v>-0.04589628428220749</v>
+        <v>0.09360665827989578</v>
       </c>
     </row>
     <row r="96">
@@ -1765,13 +1765,13 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>-1.73750901222229</v>
+        <v>0.274729311466217</v>
       </c>
       <c r="C96" t="n">
-        <v>2.908074855804443</v>
+        <v>0.6074049472808838</v>
       </c>
       <c r="D96" t="n">
-        <v>-0.8872619867324829</v>
+        <v>-0.06174364313483238</v>
       </c>
     </row>
     <row r="97">
@@ -1779,13 +1779,13 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>-1.780130982398987</v>
+        <v>0.3417177200317383</v>
       </c>
       <c r="C97" t="n">
-        <v>2.450564861297607</v>
+        <v>0.6574380993843079</v>
       </c>
       <c r="D97" t="n">
-        <v>0.3095099031925201</v>
+        <v>-0.0109863979741931</v>
       </c>
     </row>
     <row r="98">
@@ -1793,13 +1793,13 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>-1.887764811515808</v>
+        <v>0.2413844615221024</v>
       </c>
       <c r="C98" t="n">
-        <v>3.187839984893799</v>
+        <v>0.6275184154510498</v>
       </c>
       <c r="D98" t="n">
-        <v>-0.2156050801277161</v>
+        <v>0.0203790869563818</v>
       </c>
     </row>
     <row r="99">
@@ -1807,13 +1807,13 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>-1.867316722869873</v>
+        <v>0.3252526223659515</v>
       </c>
       <c r="C99" t="n">
-        <v>3.353143453598022</v>
+        <v>0.6268348693847656</v>
       </c>
       <c r="D99" t="n">
-        <v>0.1847504377365112</v>
+        <v>-0.07080281525850296</v>
       </c>
     </row>
     <row r="100">
@@ -1821,13 +1821,13 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>-1.496890068054199</v>
+        <v>0.2446257025003433</v>
       </c>
       <c r="C100" t="n">
-        <v>3.266568183898926</v>
+        <v>0.5866054892539978</v>
       </c>
       <c r="D100" t="n">
-        <v>-0.2860920429229736</v>
+        <v>0.01153383869677782</v>
       </c>
     </row>
     <row r="101">
@@ -1835,13 +1835,13 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>-0.6310759782791138</v>
+        <v>0.2683464288711548</v>
       </c>
       <c r="C101" t="n">
-        <v>2.936360359191895</v>
+        <v>0.644130527973175</v>
       </c>
       <c r="D101" t="n">
-        <v>-1.074450612068176</v>
+        <v>0.08908354490995407</v>
       </c>
     </row>
     <row r="102">
@@ -1849,13 +1849,13 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>-1.372061610221863</v>
+        <v>0.2267144918441772</v>
       </c>
       <c r="C102" t="n">
-        <v>2.942946910858154</v>
+        <v>0.6838650703430176</v>
       </c>
       <c r="D102" t="n">
-        <v>-1.269001603126526</v>
+        <v>0.0751708522439003</v>
       </c>
     </row>
     <row r="103">
@@ -1863,13 +1863,13 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>-1.387020945549011</v>
+        <v>0.1779344081878662</v>
       </c>
       <c r="C103" t="n">
-        <v>3.06696891784668</v>
+        <v>0.5754459500312805</v>
       </c>
       <c r="D103" t="n">
-        <v>-1.022855162620544</v>
+        <v>0.03304407000541687</v>
       </c>
     </row>
     <row r="104">
@@ -1877,13 +1877,13 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>-2.159872531890869</v>
+        <v>0.1893597543239594</v>
       </c>
       <c r="C104" t="n">
-        <v>3.085267543792725</v>
+        <v>0.6309283971786499</v>
       </c>
       <c r="D104" t="n">
-        <v>0.1878882050514221</v>
+        <v>0.06214623525738716</v>
       </c>
     </row>
     <row r="105">
@@ -1891,13 +1891,13 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>-1.638098120689392</v>
+        <v>0.212966725230217</v>
       </c>
       <c r="C105" t="n">
-        <v>2.889097452163696</v>
+        <v>0.7056659460067749</v>
       </c>
       <c r="D105" t="n">
-        <v>-0.2802909016609192</v>
+        <v>0.04280313476920128</v>
       </c>
     </row>
     <row r="106">
@@ -1905,13 +1905,13 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>-1.598346948623657</v>
+        <v>0.1549113094806671</v>
       </c>
       <c r="C106" t="n">
-        <v>3.112810850143433</v>
+        <v>0.5823915600776672</v>
       </c>
       <c r="D106" t="n">
-        <v>-0.6549816131591797</v>
+        <v>0.08974611759185791</v>
       </c>
     </row>
     <row r="107">
@@ -1919,13 +1919,13 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>-1.732353091239929</v>
+        <v>0.1559800654649734</v>
       </c>
       <c r="C107" t="n">
-        <v>3.266454935073853</v>
+        <v>0.6279996037483215</v>
       </c>
       <c r="D107" t="n">
-        <v>-0.5796715617179871</v>
+        <v>0.08242625743150711</v>
       </c>
     </row>
     <row r="108">
@@ -1933,13 +1933,13 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>-2.122333765029907</v>
+        <v>0.2405606061220169</v>
       </c>
       <c r="C108" t="n">
-        <v>3.421588897705078</v>
+        <v>0.7839590311050415</v>
       </c>
       <c r="D108" t="n">
-        <v>0.1676618456840515</v>
+        <v>0.1417016685009003</v>
       </c>
     </row>
     <row r="109">
@@ -1947,13 +1947,13 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>-1.750489234924316</v>
+        <v>0.2327449768781662</v>
       </c>
       <c r="C109" t="n">
-        <v>3.032720565795898</v>
+        <v>0.6885680556297302</v>
       </c>
       <c r="D109" t="n">
-        <v>-0.653384804725647</v>
+        <v>0.08632232993841171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2022/11.10 22:43 update ae gen, ae
</commit_message>
<xml_diff>
--- a/documents/latent_vector/dqn_enc.xlsx
+++ b/documents/latent_vector/dqn_enc.xlsx
@@ -449,13 +449,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.2664260864257812</v>
+        <v>-0.8774068355560303</v>
       </c>
       <c r="C2" t="n">
-        <v>0.648847222328186</v>
+        <v>-0.7383936643600464</v>
       </c>
       <c r="D2" t="n">
-        <v>0.006257821805775166</v>
+        <v>-0.2346171140670776</v>
       </c>
     </row>
     <row r="3">
@@ -463,13 +463,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.2685320973396301</v>
+        <v>-0.9186053872108459</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6317225694656372</v>
+        <v>-0.7034066915512085</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.0004622291307896376</v>
+        <v>-0.1846785545349121</v>
       </c>
     </row>
     <row r="4">
@@ -477,13 +477,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.2612994909286499</v>
+        <v>-0.8609176874160767</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6445318460464478</v>
+        <v>-0.7189714908599854</v>
       </c>
       <c r="D4" t="n">
-        <v>0.005507540889084339</v>
+        <v>-0.1842665076255798</v>
       </c>
     </row>
     <row r="5">
@@ -491,13 +491,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2735463082790375</v>
+        <v>-0.9566603302955627</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6667757034301758</v>
+        <v>-0.7575868964195251</v>
       </c>
       <c r="D5" t="n">
-        <v>0.001726453425362706</v>
+        <v>-0.2478329539299011</v>
       </c>
     </row>
     <row r="6">
@@ -505,13 +505,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.2817603945732117</v>
+        <v>-0.8675116896629333</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6681255698204041</v>
+        <v>-0.7727258205413818</v>
       </c>
       <c r="D6" t="n">
-        <v>0.03344858810305595</v>
+        <v>-0.3054336905479431</v>
       </c>
     </row>
     <row r="7">
@@ -519,13 +519,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.2638928592205048</v>
+        <v>-0.9408020973205566</v>
       </c>
       <c r="C7" t="n">
-        <v>0.6673364043235779</v>
+        <v>-0.7823367118835449</v>
       </c>
       <c r="D7" t="n">
-        <v>0.02527406625449657</v>
+        <v>-0.3440484404563904</v>
       </c>
     </row>
     <row r="8">
@@ -533,13 +533,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.2702624201774597</v>
+        <v>-0.8622509837150574</v>
       </c>
       <c r="C8" t="n">
-        <v>0.6472333073616028</v>
+        <v>-0.6972945332527161</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0133428992703557</v>
+        <v>-0.1856018900871277</v>
       </c>
     </row>
     <row r="9">
@@ -547,13 +547,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.2650624811649323</v>
+        <v>-0.9113166332244873</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6631730198860168</v>
+        <v>-0.7507771253585815</v>
       </c>
       <c r="D9" t="n">
-        <v>0.01029693800956011</v>
+        <v>-0.2932602763175964</v>
       </c>
     </row>
     <row r="10">
@@ -561,13 +561,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.2627106308937073</v>
+        <v>-0.816106379032135</v>
       </c>
       <c r="C10" t="n">
-        <v>0.6413992643356323</v>
+        <v>-0.6514130234718323</v>
       </c>
       <c r="D10" t="n">
-        <v>0.004524593241512775</v>
+        <v>-0.1786742508411407</v>
       </c>
     </row>
     <row r="11">
@@ -575,13 +575,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.2833506166934967</v>
+        <v>-0.9811093211174011</v>
       </c>
       <c r="C11" t="n">
-        <v>0.6797158122062683</v>
+        <v>-0.8581236600875854</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.04492827877402306</v>
+        <v>-0.4552638530731201</v>
       </c>
     </row>
     <row r="12">
@@ -589,13 +589,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.2460916340351105</v>
+        <v>-0.8466823697090149</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6257547736167908</v>
+        <v>-0.6582441926002502</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.004036027006804943</v>
+        <v>-0.1511086225509644</v>
       </c>
     </row>
     <row r="13">
@@ -603,13 +603,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.2692782878875732</v>
+        <v>-0.9953675270080566</v>
       </c>
       <c r="C13" t="n">
-        <v>0.6775692701339722</v>
+        <v>-0.7804772853851318</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.02587408758699894</v>
+        <v>-0.2526264786720276</v>
       </c>
     </row>
     <row r="14">
@@ -617,13 +617,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.251497358083725</v>
+        <v>-0.8919361233711243</v>
       </c>
       <c r="C14" t="n">
-        <v>0.6415874361991882</v>
+        <v>-0.7302467823028564</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.0008179049473255873</v>
+        <v>-0.2182176411151886</v>
       </c>
     </row>
     <row r="15">
@@ -631,13 +631,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.2605743408203125</v>
+        <v>-0.8620424866676331</v>
       </c>
       <c r="C15" t="n">
-        <v>0.674394428730011</v>
+        <v>-0.7769688367843628</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.005164711736142635</v>
+        <v>-0.3466309309005737</v>
       </c>
     </row>
     <row r="16">
@@ -645,13 +645,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.2492799907922745</v>
+        <v>-0.8507569432258606</v>
       </c>
       <c r="C16" t="n">
-        <v>0.7193794250488281</v>
+        <v>-0.7782182693481445</v>
       </c>
       <c r="D16" t="n">
-        <v>0.04309358447790146</v>
+        <v>-0.6273947954177856</v>
       </c>
     </row>
     <row r="17">
@@ -659,13 +659,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.2360272705554962</v>
+        <v>-0.7930828332901001</v>
       </c>
       <c r="C17" t="n">
-        <v>0.7315543293952942</v>
+        <v>-0.7877063155174255</v>
       </c>
       <c r="D17" t="n">
-        <v>0.08003737032413483</v>
+        <v>-0.8255119323730469</v>
       </c>
     </row>
     <row r="18">
@@ -673,13 +673,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.2504982948303223</v>
+        <v>-0.8147932887077332</v>
       </c>
       <c r="C18" t="n">
-        <v>0.7065553665161133</v>
+        <v>-0.7664750814437866</v>
       </c>
       <c r="D18" t="n">
-        <v>0.01061974186450243</v>
+        <v>-0.5391026735305786</v>
       </c>
     </row>
     <row r="19">
@@ -687,13 +687,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.2631286382675171</v>
+        <v>-0.8702529668807983</v>
       </c>
       <c r="C19" t="n">
-        <v>0.6587488055229187</v>
+        <v>-0.7287623882293701</v>
       </c>
       <c r="D19" t="n">
-        <v>0.01003144402056932</v>
+        <v>-0.3113494515419006</v>
       </c>
     </row>
     <row r="20">
@@ -701,13 +701,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.2744163572788239</v>
+        <v>-0.9391471743583679</v>
       </c>
       <c r="C20" t="n">
-        <v>0.6667273044586182</v>
+        <v>-0.7798076868057251</v>
       </c>
       <c r="D20" t="n">
-        <v>0.002296773018315434</v>
+        <v>-0.09585863351821899</v>
       </c>
     </row>
     <row r="21">
@@ -715,13 +715,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.2809521555900574</v>
+        <v>-0.9158798456192017</v>
       </c>
       <c r="C21" t="n">
-        <v>0.6843045353889465</v>
+        <v>-0.8201900124549866</v>
       </c>
       <c r="D21" t="n">
-        <v>0.01586962677538395</v>
+        <v>-0.1289330720901489</v>
       </c>
     </row>
     <row r="22">
@@ -729,13 +729,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.2532158195972443</v>
+        <v>-0.9638277888298035</v>
       </c>
       <c r="C22" t="n">
-        <v>0.6412532925605774</v>
+        <v>-0.8074393272399902</v>
       </c>
       <c r="D22" t="n">
-        <v>0.03109738789498806</v>
+        <v>-0.2746186852455139</v>
       </c>
     </row>
     <row r="23">
@@ -743,13 +743,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.2571897506713867</v>
+        <v>-0.8498709201812744</v>
       </c>
       <c r="C23" t="n">
-        <v>0.675843358039856</v>
+        <v>-0.839926540851593</v>
       </c>
       <c r="D23" t="n">
-        <v>0.006066803820431232</v>
+        <v>-0.3209908008575439</v>
       </c>
     </row>
     <row r="24">
@@ -757,13 +757,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.2605628371238708</v>
+        <v>-0.9768247008323669</v>
       </c>
       <c r="C24" t="n">
-        <v>0.6730467677116394</v>
+        <v>-0.8339508771896362</v>
       </c>
       <c r="D24" t="n">
-        <v>0.002613698365166783</v>
+        <v>-0.1955572068691254</v>
       </c>
     </row>
     <row r="25">
@@ -771,13 +771,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.2463047355413437</v>
+        <v>-0.9113130569458008</v>
       </c>
       <c r="C25" t="n">
-        <v>0.6194472312927246</v>
+        <v>-0.7337418794631958</v>
       </c>
       <c r="D25" t="n">
-        <v>0.0214551780372858</v>
+        <v>-0.009817942976951599</v>
       </c>
     </row>
     <row r="26">
@@ -785,13 +785,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>0.2472080737352371</v>
+        <v>-0.8702506422996521</v>
       </c>
       <c r="C26" t="n">
-        <v>0.6511561274528503</v>
+        <v>-0.768538236618042</v>
       </c>
       <c r="D26" t="n">
-        <v>0.02218163572251797</v>
+        <v>-0.2041963338851929</v>
       </c>
     </row>
     <row r="27">
@@ -799,13 +799,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>0.2366319000720978</v>
+        <v>-0.9325038194656372</v>
       </c>
       <c r="C27" t="n">
-        <v>0.6454380750656128</v>
+        <v>-0.6933842897415161</v>
       </c>
       <c r="D27" t="n">
-        <v>0.030525928363204</v>
+        <v>-0.2322947978973389</v>
       </c>
     </row>
     <row r="28">
@@ -813,13 +813,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>0.2622062861919403</v>
+        <v>-0.9567565321922302</v>
       </c>
       <c r="C28" t="n">
-        <v>0.6235539317131042</v>
+        <v>-0.7441583871841431</v>
       </c>
       <c r="D28" t="n">
-        <v>0.003572893561795354</v>
+        <v>-0.09162810444831848</v>
       </c>
     </row>
     <row r="29">
@@ -827,13 +827,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>0.2783145010471344</v>
+        <v>-0.8933591842651367</v>
       </c>
       <c r="C29" t="n">
-        <v>0.6491417288780212</v>
+        <v>-0.8059036135673523</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.009267206303775311</v>
+        <v>-0.2341111600399017</v>
       </c>
     </row>
     <row r="30">
@@ -841,13 +841,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>0.2809744477272034</v>
+        <v>-0.9299925565719604</v>
       </c>
       <c r="C30" t="n">
-        <v>0.6393743753433228</v>
+        <v>-0.8046311140060425</v>
       </c>
       <c r="D30" t="n">
-        <v>-0.01747854985296726</v>
+        <v>-0.1849361658096313</v>
       </c>
     </row>
     <row r="31">
@@ -855,13 +855,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>0.2675471007823944</v>
+        <v>-0.876373827457428</v>
       </c>
       <c r="C31" t="n">
-        <v>0.6116402149200439</v>
+        <v>-0.7470036745071411</v>
       </c>
       <c r="D31" t="n">
-        <v>-0.01962635107338428</v>
+        <v>-0.08855932950973511</v>
       </c>
     </row>
     <row r="32">
@@ -869,13 +869,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>0.2820245921611786</v>
+        <v>-0.9010275602340698</v>
       </c>
       <c r="C32" t="n">
-        <v>0.6476053595542908</v>
+        <v>-0.8084818124771118</v>
       </c>
       <c r="D32" t="n">
-        <v>-0.02070611901581287</v>
+        <v>-0.1852150559425354</v>
       </c>
     </row>
     <row r="33">
@@ -883,13 +883,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>0.255298376083374</v>
+        <v>-0.8761732578277588</v>
       </c>
       <c r="C33" t="n">
-        <v>0.6067289710044861</v>
+        <v>-0.7376439571380615</v>
       </c>
       <c r="D33" t="n">
-        <v>-0.02059216983616352</v>
+        <v>-0.1311497986316681</v>
       </c>
     </row>
     <row r="34">
@@ -897,13 +897,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>0.257289707660675</v>
+        <v>-0.9619056582450867</v>
       </c>
       <c r="C34" t="n">
-        <v>0.6041221022605896</v>
+        <v>-0.7438372373580933</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.0243732426315546</v>
+        <v>-0.03058096766471863</v>
       </c>
     </row>
     <row r="35">
@@ -911,13 +911,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>0.220881387591362</v>
+        <v>-1.063008308410645</v>
       </c>
       <c r="C35" t="n">
-        <v>0.6232128739356995</v>
+        <v>-0.7170872092247009</v>
       </c>
       <c r="D35" t="n">
-        <v>0.006093484349548817</v>
+        <v>-0.1024332642555237</v>
       </c>
     </row>
     <row r="36">
@@ -925,13 +925,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>0.2232494801282883</v>
+        <v>-0.931325376033783</v>
       </c>
       <c r="C36" t="n">
-        <v>0.6153203845024109</v>
+        <v>-0.6872330904006958</v>
       </c>
       <c r="D36" t="n">
-        <v>0.03371736034750938</v>
+        <v>-0.2540508508682251</v>
       </c>
     </row>
     <row r="37">
@@ -939,13 +939,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>0.2781234085559845</v>
+        <v>-0.8784062266349792</v>
       </c>
       <c r="C37" t="n">
-        <v>0.6395302414894104</v>
+        <v>-0.6572571992874146</v>
       </c>
       <c r="D37" t="n">
-        <v>-0.006170745007693768</v>
+        <v>-0.3483367562294006</v>
       </c>
     </row>
     <row r="38">
@@ -953,13 +953,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>0.2940637469291687</v>
+        <v>-0.672127902507782</v>
       </c>
       <c r="C38" t="n">
-        <v>0.6250672340393066</v>
+        <v>-0.5604920387268066</v>
       </c>
       <c r="D38" t="n">
-        <v>-0.04447906464338303</v>
+        <v>-0.4841903448104858</v>
       </c>
     </row>
     <row r="39">
@@ -967,13 +967,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>0.2946504354476929</v>
+        <v>-0.9214125275611877</v>
       </c>
       <c r="C39" t="n">
-        <v>0.6589730381965637</v>
+        <v>-0.7168911695480347</v>
       </c>
       <c r="D39" t="n">
-        <v>0.01015757489949465</v>
+        <v>-0.340360701084137</v>
       </c>
     </row>
     <row r="40">
@@ -981,13 +981,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>0.3088955283164978</v>
+        <v>-0.9229697585105896</v>
       </c>
       <c r="C40" t="n">
-        <v>0.6672388315200806</v>
+        <v>-0.6833274364471436</v>
       </c>
       <c r="D40" t="n">
-        <v>-0.01201942097395658</v>
+        <v>-0.3721800446510315</v>
       </c>
     </row>
     <row r="41">
@@ -995,13 +995,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>0.3115738034248352</v>
+        <v>-0.9724355340003967</v>
       </c>
       <c r="C41" t="n">
-        <v>0.6759269833564758</v>
+        <v>-0.7387970089912415</v>
       </c>
       <c r="D41" t="n">
-        <v>-0.009336180053651333</v>
+        <v>-0.3970728516578674</v>
       </c>
     </row>
     <row r="42">
@@ -1009,13 +1009,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>0.2933615148067474</v>
+        <v>-0.9347510933876038</v>
       </c>
       <c r="C42" t="n">
-        <v>0.6040554642677307</v>
+        <v>-0.5326456427574158</v>
       </c>
       <c r="D42" t="n">
-        <v>-0.005730926059186459</v>
+        <v>-0.2284276187419891</v>
       </c>
     </row>
     <row r="43">
@@ -1023,13 +1023,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>0.2915279269218445</v>
+        <v>-0.9229821562767029</v>
       </c>
       <c r="C43" t="n">
-        <v>0.6482939124107361</v>
+        <v>-0.7050019502639771</v>
       </c>
       <c r="D43" t="n">
-        <v>0.01159847993403673</v>
+        <v>-0.3344995379447937</v>
       </c>
     </row>
     <row r="44">
@@ -1037,13 +1037,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>0.3013015389442444</v>
+        <v>-0.8722541332244873</v>
       </c>
       <c r="C44" t="n">
-        <v>0.6537688970565796</v>
+        <v>-0.6703691482543945</v>
       </c>
       <c r="D44" t="n">
-        <v>-0.03122072853147984</v>
+        <v>-0.3964746594429016</v>
       </c>
     </row>
     <row r="45">
@@ -1051,13 +1051,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>0.2963208556175232</v>
+        <v>-0.5858168601989746</v>
       </c>
       <c r="C45" t="n">
-        <v>0.6096335649490356</v>
+        <v>-0.5052000880241394</v>
       </c>
       <c r="D45" t="n">
-        <v>-0.0409470722079277</v>
+        <v>-0.3992400169372559</v>
       </c>
     </row>
     <row r="46">
@@ -1065,13 +1065,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>0.2977321743965149</v>
+        <v>-0.6317669153213501</v>
       </c>
       <c r="C46" t="n">
-        <v>0.6120379567146301</v>
+        <v>-0.5336444973945618</v>
       </c>
       <c r="D46" t="n">
-        <v>-0.03880958631634712</v>
+        <v>-0.4222643971443176</v>
       </c>
     </row>
     <row r="47">
@@ -1079,13 +1079,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>0.297637403011322</v>
+        <v>-0.6196783185005188</v>
       </c>
       <c r="C47" t="n">
-        <v>0.6145109534263611</v>
+        <v>-0.5134835839271545</v>
       </c>
       <c r="D47" t="n">
-        <v>-0.03943720459938049</v>
+        <v>-0.4220762252807617</v>
       </c>
     </row>
     <row r="48">
@@ -1093,13 +1093,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>0.3001566827297211</v>
+        <v>-0.6037497520446777</v>
       </c>
       <c r="C48" t="n">
-        <v>0.6191834211349487</v>
+        <v>-0.5197960734367371</v>
       </c>
       <c r="D48" t="n">
-        <v>-0.05023006722331047</v>
+        <v>-0.4393643736839294</v>
       </c>
     </row>
     <row r="49">
@@ -1107,13 +1107,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>0.2364149838685989</v>
+        <v>-0.819627583026886</v>
       </c>
       <c r="C49" t="n">
-        <v>0.638400673866272</v>
+        <v>-0.7662175297737122</v>
       </c>
       <c r="D49" t="n">
-        <v>0.03257723525166512</v>
+        <v>-0.4405239224433899</v>
       </c>
     </row>
     <row r="50">
@@ -1121,13 +1121,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>0.3181438446044922</v>
+        <v>-1.400162935256958</v>
       </c>
       <c r="C50" t="n">
-        <v>0.7626717686653137</v>
+        <v>-0.9566746950149536</v>
       </c>
       <c r="D50" t="n">
-        <v>-0.06358947604894638</v>
+        <v>-0.03369809687137604</v>
       </c>
     </row>
     <row r="51">
@@ -1135,13 +1135,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>0.2895421981811523</v>
+        <v>-0.8442731499671936</v>
       </c>
       <c r="C51" t="n">
-        <v>0.6459152102470398</v>
+        <v>-0.7557651996612549</v>
       </c>
       <c r="D51" t="n">
-        <v>0.04735403135418892</v>
+        <v>0.123165637254715</v>
       </c>
     </row>
     <row r="52">
@@ -1149,13 +1149,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>0.2630741596221924</v>
+        <v>-0.8398253321647644</v>
       </c>
       <c r="C52" t="n">
-        <v>0.6273863315582275</v>
+        <v>-0.7660485506057739</v>
       </c>
       <c r="D52" t="n">
-        <v>0.06460031867027283</v>
+        <v>0.1208779066801071</v>
       </c>
     </row>
     <row r="53">
@@ -1163,13 +1163,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>0.3802274465560913</v>
+        <v>-1.310978651046753</v>
       </c>
       <c r="C53" t="n">
-        <v>0.7616562843322754</v>
+        <v>-0.9460172057151794</v>
       </c>
       <c r="D53" t="n">
-        <v>-0.07184354960918427</v>
+        <v>-0.227546215057373</v>
       </c>
     </row>
     <row r="54">
@@ -1177,13 +1177,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>0.2757600247859955</v>
+        <v>-0.731418251991272</v>
       </c>
       <c r="C54" t="n">
-        <v>0.7006799578666687</v>
+        <v>-0.9099568724632263</v>
       </c>
       <c r="D54" t="n">
-        <v>0.0312936045229435</v>
+        <v>-0.5547305345535278</v>
       </c>
     </row>
     <row r="55">
@@ -1191,13 +1191,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>0.3277468085289001</v>
+        <v>-1.118304014205933</v>
       </c>
       <c r="C55" t="n">
-        <v>0.7888743877410889</v>
+        <v>-1.07854688167572</v>
       </c>
       <c r="D55" t="n">
-        <v>0.07694433629512787</v>
+        <v>-0.5860914587974548</v>
       </c>
     </row>
     <row r="56">
@@ -1205,13 +1205,13 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>0.3012381196022034</v>
+        <v>-0.8974708318710327</v>
       </c>
       <c r="C56" t="n">
-        <v>0.6688922643661499</v>
+        <v>-0.5383338332176208</v>
       </c>
       <c r="D56" t="n">
-        <v>-0.05056856200098991</v>
+        <v>-0.334769070148468</v>
       </c>
     </row>
     <row r="57">
@@ -1219,13 +1219,13 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>0.2903702557086945</v>
+        <v>-0.7136864066123962</v>
       </c>
       <c r="C57" t="n">
-        <v>0.6197267174720764</v>
+        <v>-0.5790572166442871</v>
       </c>
       <c r="D57" t="n">
-        <v>-0.0126697076484561</v>
+        <v>-0.120156466960907</v>
       </c>
     </row>
     <row r="58">
@@ -1233,13 +1233,13 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>0.2776203751564026</v>
+        <v>-0.7789818644523621</v>
       </c>
       <c r="C58" t="n">
-        <v>0.6252539157867432</v>
+        <v>-0.6184816360473633</v>
       </c>
       <c r="D58" t="n">
-        <v>-0.01979565061628819</v>
+        <v>-0.2397118806838989</v>
       </c>
     </row>
     <row r="59">
@@ -1247,13 +1247,13 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>0.2697232067584991</v>
+        <v>-1.003947973251343</v>
       </c>
       <c r="C59" t="n">
-        <v>0.6948001384735107</v>
+        <v>-0.8050851225852966</v>
       </c>
       <c r="D59" t="n">
-        <v>0.0410330556333065</v>
+        <v>-0.1685780584812164</v>
       </c>
     </row>
     <row r="60">
@@ -1261,13 +1261,13 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>0.328652560710907</v>
+        <v>-1.418603420257568</v>
       </c>
       <c r="C60" t="n">
-        <v>0.7788655161857605</v>
+        <v>-0.9027448892593384</v>
       </c>
       <c r="D60" t="n">
-        <v>-0.04485651478171349</v>
+        <v>0.04229003190994263</v>
       </c>
     </row>
     <row r="61">
@@ -1275,13 +1275,13 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>0.2802637815475464</v>
+        <v>-1.110793948173523</v>
       </c>
       <c r="C61" t="n">
-        <v>0.6914541125297546</v>
+        <v>-0.6732813715934753</v>
       </c>
       <c r="D61" t="n">
-        <v>-0.01934750191867352</v>
+        <v>-0.06197705864906311</v>
       </c>
     </row>
     <row r="62">
@@ -1289,13 +1289,13 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>0.309709757566452</v>
+        <v>-0.8194100856781006</v>
       </c>
       <c r="C62" t="n">
-        <v>0.6786558032035828</v>
+        <v>-0.5357325077056885</v>
       </c>
       <c r="D62" t="n">
-        <v>-0.03649889305233955</v>
+        <v>-0.3365902304649353</v>
       </c>
     </row>
     <row r="63">
@@ -1303,13 +1303,13 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>0.3309531211853027</v>
+        <v>-0.6620504856109619</v>
       </c>
       <c r="C63" t="n">
-        <v>0.7585431337356567</v>
+        <v>-0.8748719692230225</v>
       </c>
       <c r="D63" t="n">
-        <v>0.04927822574973106</v>
+        <v>-0.5809007287025452</v>
       </c>
     </row>
     <row r="64">
@@ -1317,13 +1317,13 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>0.2778111398220062</v>
+        <v>-1.010077357292175</v>
       </c>
       <c r="C64" t="n">
-        <v>0.6507033705711365</v>
+        <v>-0.8484398722648621</v>
       </c>
       <c r="D64" t="n">
-        <v>-0.04148483648896217</v>
+        <v>-0.2630506753921509</v>
       </c>
     </row>
     <row r="65">
@@ -1331,13 +1331,13 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>0.2704644203186035</v>
+        <v>-0.6523619294166565</v>
       </c>
       <c r="C65" t="n">
-        <v>0.5882279276847839</v>
+        <v>-0.5528481602668762</v>
       </c>
       <c r="D65" t="n">
-        <v>-0.01401156466454268</v>
+        <v>-0.08960515260696411</v>
       </c>
     </row>
     <row r="66">
@@ -1345,13 +1345,13 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>0.2938117384910583</v>
+        <v>-0.5157608389854431</v>
       </c>
       <c r="C66" t="n">
-        <v>0.6004683375358582</v>
+        <v>-0.5098051428794861</v>
       </c>
       <c r="D66" t="n">
-        <v>-0.04677809029817581</v>
+        <v>-0.2801095247268677</v>
       </c>
     </row>
     <row r="67">
@@ -1359,13 +1359,13 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>0.243002250790596</v>
+        <v>-0.7892442941665649</v>
       </c>
       <c r="C67" t="n">
-        <v>0.5443406105041504</v>
+        <v>-0.2910152077674866</v>
       </c>
       <c r="D67" t="n">
-        <v>0.02213357202708721</v>
+        <v>-0.4437853097915649</v>
       </c>
     </row>
     <row r="68">
@@ -1373,13 +1373,13 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>0.1544641554355621</v>
+        <v>-1.252237558364868</v>
       </c>
       <c r="C68" t="n">
-        <v>0.626908004283905</v>
+        <v>-0.9243879318237305</v>
       </c>
       <c r="D68" t="n">
-        <v>0.08464200794696808</v>
+        <v>-0.395668089389801</v>
       </c>
     </row>
     <row r="69">
@@ -1387,13 +1387,13 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>0.2766607999801636</v>
+        <v>-0.6584404706954956</v>
       </c>
       <c r="C69" t="n">
-        <v>0.6093487143516541</v>
+        <v>-0.5859214663505554</v>
       </c>
       <c r="D69" t="n">
-        <v>-0.01282935123890638</v>
+        <v>-0.1544092297554016</v>
       </c>
     </row>
     <row r="70">
@@ -1401,13 +1401,13 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>0.2291892766952515</v>
+        <v>-0.9030315279960632</v>
       </c>
       <c r="C70" t="n">
-        <v>0.6763365864753723</v>
+        <v>-0.8191682100296021</v>
       </c>
       <c r="D70" t="n">
-        <v>0.06174615398049355</v>
+        <v>-0.3347437381744385</v>
       </c>
     </row>
     <row r="71">
@@ -1415,13 +1415,13 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>0.2291549146175385</v>
+        <v>-0.9266481995582581</v>
       </c>
       <c r="C71" t="n">
-        <v>0.6336483955383301</v>
+        <v>-0.8069517016410828</v>
       </c>
       <c r="D71" t="n">
-        <v>0.04827026650309563</v>
+        <v>-0.1643447279930115</v>
       </c>
     </row>
     <row r="72">
@@ -1429,13 +1429,13 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>0.2522068321704865</v>
+        <v>-0.8937005400657654</v>
       </c>
       <c r="C72" t="n">
-        <v>0.5857676267623901</v>
+        <v>-0.8671473264694214</v>
       </c>
       <c r="D72" t="n">
-        <v>0.05672628059983253</v>
+        <v>-0.2104970812797546</v>
       </c>
     </row>
     <row r="73">
@@ -1443,13 +1443,13 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>0.2455205172300339</v>
+        <v>-0.7115880846977234</v>
       </c>
       <c r="C73" t="n">
-        <v>0.5851485729217529</v>
+        <v>-0.6350852251052856</v>
       </c>
       <c r="D73" t="n">
-        <v>0.02929545007646084</v>
+        <v>-0.1761727929115295</v>
       </c>
     </row>
     <row r="74">
@@ -1457,13 +1457,13 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>0.2489051073789597</v>
+        <v>-0.6285414099693298</v>
       </c>
       <c r="C74" t="n">
-        <v>0.5929679870605469</v>
+        <v>-0.5604482293128967</v>
       </c>
       <c r="D74" t="n">
-        <v>0.01280758995562792</v>
+        <v>-0.1903518736362457</v>
       </c>
     </row>
     <row r="75">
@@ -1471,13 +1471,13 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>0.2900951504707336</v>
+        <v>-0.6371750831604004</v>
       </c>
       <c r="C75" t="n">
-        <v>0.6063517332077026</v>
+        <v>-0.5297112464904785</v>
       </c>
       <c r="D75" t="n">
-        <v>-0.03421608731150627</v>
+        <v>-0.1422064304351807</v>
       </c>
     </row>
     <row r="76">
@@ -1485,13 +1485,13 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>0.2646459937095642</v>
+        <v>-0.7414934635162354</v>
       </c>
       <c r="C76" t="n">
-        <v>0.6510897278785706</v>
+        <v>-0.6893380284309387</v>
       </c>
       <c r="D76" t="n">
-        <v>-0.01787109114229679</v>
+        <v>-0.1294722557067871</v>
       </c>
     </row>
     <row r="77">
@@ -1499,13 +1499,13 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>0.2612802684307098</v>
+        <v>-0.8807417750358582</v>
       </c>
       <c r="C77" t="n">
-        <v>0.6430612802505493</v>
+        <v>-0.7832221984863281</v>
       </c>
       <c r="D77" t="n">
-        <v>-0.002751069841906428</v>
+        <v>0.04081235826015472</v>
       </c>
     </row>
     <row r="78">
@@ -1513,13 +1513,13 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>0.2589626610279083</v>
+        <v>-0.8170123100280762</v>
       </c>
       <c r="C78" t="n">
-        <v>0.6299439072608948</v>
+        <v>-0.7336433529853821</v>
       </c>
       <c r="D78" t="n">
-        <v>-0.01124752592295408</v>
+        <v>0.04615232348442078</v>
       </c>
     </row>
     <row r="79">
@@ -1527,13 +1527,13 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>0.2354486584663391</v>
+        <v>-1.005516290664673</v>
       </c>
       <c r="C79" t="n">
-        <v>0.6984711885452271</v>
+        <v>-0.8315661549568176</v>
       </c>
       <c r="D79" t="n">
-        <v>0.05917864665389061</v>
+        <v>-0.2537497282028198</v>
       </c>
     </row>
     <row r="80">
@@ -1541,13 +1541,13 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>0.2932033240795135</v>
+        <v>-0.9059018492698669</v>
       </c>
       <c r="C80" t="n">
-        <v>0.6488298177719116</v>
+        <v>-0.7591546177864075</v>
       </c>
       <c r="D80" t="n">
-        <v>-0.02532858215272427</v>
+        <v>0.06129594147205353</v>
       </c>
     </row>
     <row r="81">
@@ -1555,13 +1555,13 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>0.2741170823574066</v>
+        <v>-0.8367088437080383</v>
       </c>
       <c r="C81" t="n">
-        <v>0.6358624696731567</v>
+        <v>-0.7220001220703125</v>
       </c>
       <c r="D81" t="n">
-        <v>-0.03057688660919666</v>
+        <v>0.03110097348690033</v>
       </c>
     </row>
     <row r="82">
@@ -1569,13 +1569,13 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>0.3075407147407532</v>
+        <v>-0.6509606838226318</v>
       </c>
       <c r="C82" t="n">
-        <v>0.6215934157371521</v>
+        <v>-0.5716146230697632</v>
       </c>
       <c r="D82" t="n">
-        <v>-0.009303535334765911</v>
+        <v>-0.2604126632213593</v>
       </c>
     </row>
     <row r="83">
@@ -1583,13 +1583,13 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>0.3446000516414642</v>
+        <v>-0.793902575969696</v>
       </c>
       <c r="C83" t="n">
-        <v>0.6564664244651794</v>
+        <v>-0.5813690423965454</v>
       </c>
       <c r="D83" t="n">
-        <v>-0.01097910758107901</v>
+        <v>-0.4137298464775085</v>
       </c>
     </row>
     <row r="84">
@@ -1597,13 +1597,13 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>0.3271609544754028</v>
+        <v>-1.02420699596405</v>
       </c>
       <c r="C84" t="n">
-        <v>0.7200009226799011</v>
+        <v>-0.8435726165771484</v>
       </c>
       <c r="D84" t="n">
-        <v>-0.006261053495109081</v>
+        <v>0.01820382475852966</v>
       </c>
     </row>
     <row r="85">
@@ -1611,13 +1611,13 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>0.3438205718994141</v>
+        <v>-0.8467736840248108</v>
       </c>
       <c r="C85" t="n">
-        <v>0.645734965801239</v>
+        <v>-0.5616253614425659</v>
       </c>
       <c r="D85" t="n">
-        <v>-0.03103981353342533</v>
+        <v>-0.3505874872207642</v>
       </c>
     </row>
     <row r="86">
@@ -1625,13 +1625,13 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>0.3308832049369812</v>
+        <v>-0.8272479176521301</v>
       </c>
       <c r="C86" t="n">
-        <v>0.6503903865814209</v>
+        <v>-0.5727234482765198</v>
       </c>
       <c r="D86" t="n">
-        <v>-0.03756753727793694</v>
+        <v>-0.3598759770393372</v>
       </c>
     </row>
     <row r="87">
@@ -1639,13 +1639,13 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>0.3368951082229614</v>
+        <v>-0.8322588205337524</v>
       </c>
       <c r="C87" t="n">
-        <v>0.6615633368492126</v>
+        <v>-0.6074560880661011</v>
       </c>
       <c r="D87" t="n">
-        <v>-0.001027296064421535</v>
+        <v>-0.4309888482093811</v>
       </c>
     </row>
     <row r="88">
@@ -1653,13 +1653,13 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>0.3093470931053162</v>
+        <v>-0.8355688452720642</v>
       </c>
       <c r="C88" t="n">
-        <v>0.6742972731590271</v>
+        <v>-0.5805323719978333</v>
       </c>
       <c r="D88" t="n">
-        <v>-0.1017387807369232</v>
+        <v>-0.4553248286247253</v>
       </c>
     </row>
     <row r="89">
@@ -1667,13 +1667,13 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>0.328909695148468</v>
+        <v>-0.8363886475563049</v>
       </c>
       <c r="C89" t="n">
-        <v>0.6559138894081116</v>
+        <v>-0.6319226026535034</v>
       </c>
       <c r="D89" t="n">
-        <v>-0.03054380975663662</v>
+        <v>-0.4785870313644409</v>
       </c>
     </row>
     <row r="90">
@@ -1681,13 +1681,13 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>0.323961466550827</v>
+        <v>-0.7561878561973572</v>
       </c>
       <c r="C90" t="n">
-        <v>0.6420326828956604</v>
+        <v>-0.5967325568199158</v>
       </c>
       <c r="D90" t="n">
-        <v>-0.01371017005294561</v>
+        <v>-0.5032638311386108</v>
       </c>
     </row>
     <row r="91">
@@ -1695,13 +1695,13 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>0.1858139932155609</v>
+        <v>-1.187577962875366</v>
       </c>
       <c r="C91" t="n">
-        <v>0.6684508919715881</v>
+        <v>-0.7695111632347107</v>
       </c>
       <c r="D91" t="n">
-        <v>-0.0123892230913043</v>
+        <v>0.02995775640010834</v>
       </c>
     </row>
     <row r="92">
@@ -1709,13 +1709,13 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>0.113928385078907</v>
+        <v>-0.825555682182312</v>
       </c>
       <c r="C92" t="n">
-        <v>0.5926311016082764</v>
+        <v>-0.68916255235672</v>
       </c>
       <c r="D92" t="n">
-        <v>0.03954857960343361</v>
+        <v>-0.009141802787780762</v>
       </c>
     </row>
     <row r="93">
@@ -1723,13 +1723,13 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>0.1463579088449478</v>
+        <v>-0.8738554716110229</v>
       </c>
       <c r="C93" t="n">
-        <v>0.6002684831619263</v>
+        <v>-0.6865558624267578</v>
       </c>
       <c r="D93" t="n">
-        <v>0.005467464216053486</v>
+        <v>0.0009653568267822266</v>
       </c>
     </row>
     <row r="94">
@@ -1737,13 +1737,13 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>0.1251584738492966</v>
+        <v>-0.845971405506134</v>
       </c>
       <c r="C94" t="n">
-        <v>0.5876222252845764</v>
+        <v>-0.7025161385536194</v>
       </c>
       <c r="D94" t="n">
-        <v>0.03570344671607018</v>
+        <v>0.05642545223236084</v>
       </c>
     </row>
     <row r="95">
@@ -1751,13 +1751,13 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>0.2653766572475433</v>
+        <v>-0.9693118929862976</v>
       </c>
       <c r="C95" t="n">
-        <v>0.7161501049995422</v>
+        <v>-0.856134295463562</v>
       </c>
       <c r="D95" t="n">
-        <v>0.09360665827989578</v>
+        <v>-0.5356988310813904</v>
       </c>
     </row>
     <row r="96">
@@ -1765,13 +1765,13 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>0.274729311466217</v>
+        <v>-0.78933185338974</v>
       </c>
       <c r="C96" t="n">
-        <v>0.6074049472808838</v>
+        <v>-0.7073398232460022</v>
       </c>
       <c r="D96" t="n">
-        <v>-0.06174364313483238</v>
+        <v>-0.2124965190887451</v>
       </c>
     </row>
     <row r="97">
@@ -1779,13 +1779,13 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>0.3417177200317383</v>
+        <v>-0.8622241616249084</v>
       </c>
       <c r="C97" t="n">
-        <v>0.6574380993843079</v>
+        <v>-0.6075205206871033</v>
       </c>
       <c r="D97" t="n">
-        <v>-0.0109863979741931</v>
+        <v>-0.35872483253479</v>
       </c>
     </row>
     <row r="98">
@@ -1793,13 +1793,13 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>0.2413844615221024</v>
+        <v>-0.9633070826530457</v>
       </c>
       <c r="C98" t="n">
-        <v>0.6275184154510498</v>
+        <v>-0.6741501688957214</v>
       </c>
       <c r="D98" t="n">
-        <v>0.0203790869563818</v>
+        <v>-0.135686844587326</v>
       </c>
     </row>
     <row r="99">
@@ -1807,13 +1807,13 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>0.3252526223659515</v>
+        <v>-0.9218026995658875</v>
       </c>
       <c r="C99" t="n">
-        <v>0.6268348693847656</v>
+        <v>-0.5011181235313416</v>
       </c>
       <c r="D99" t="n">
-        <v>-0.07080281525850296</v>
+        <v>0.03567130863666534</v>
       </c>
     </row>
     <row r="100">
@@ -1821,13 +1821,13 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>0.2446257025003433</v>
+        <v>-0.8433488607406616</v>
       </c>
       <c r="C100" t="n">
-        <v>0.5866054892539978</v>
+        <v>-0.6030845642089844</v>
       </c>
       <c r="D100" t="n">
-        <v>0.01153383869677782</v>
+        <v>0.09999153017997742</v>
       </c>
     </row>
     <row r="101">
@@ -1835,13 +1835,13 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>0.2683464288711548</v>
+        <v>-1.04547655582428</v>
       </c>
       <c r="C101" t="n">
-        <v>0.644130527973175</v>
+        <v>-0.6583418846130371</v>
       </c>
       <c r="D101" t="n">
-        <v>0.08908354490995407</v>
+        <v>0.2069518119096756</v>
       </c>
     </row>
     <row r="102">
@@ -1849,13 +1849,13 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>0.2267144918441772</v>
+        <v>-1.140744686126709</v>
       </c>
       <c r="C102" t="n">
-        <v>0.6838650703430176</v>
+        <v>-0.8207313418388367</v>
       </c>
       <c r="D102" t="n">
-        <v>0.0751708522439003</v>
+        <v>-0.3160637617111206</v>
       </c>
     </row>
     <row r="103">
@@ -1863,13 +1863,13 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>0.1779344081878662</v>
+        <v>-1.645563244819641</v>
       </c>
       <c r="C103" t="n">
-        <v>0.5754459500312805</v>
+        <v>-1.027688264846802</v>
       </c>
       <c r="D103" t="n">
-        <v>0.03304407000541687</v>
+        <v>0.1231574863195419</v>
       </c>
     </row>
     <row r="104">
@@ -1877,13 +1877,13 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>0.1893597543239594</v>
+        <v>-0.8744520545005798</v>
       </c>
       <c r="C104" t="n">
-        <v>0.6309283971786499</v>
+        <v>-0.6345198154449463</v>
       </c>
       <c r="D104" t="n">
-        <v>0.06214623525738716</v>
+        <v>-0.185737133026123</v>
       </c>
     </row>
     <row r="105">
@@ -1891,13 +1891,13 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>0.212966725230217</v>
+        <v>-0.9828851819038391</v>
       </c>
       <c r="C105" t="n">
-        <v>0.7056659460067749</v>
+        <v>-0.6749557256698608</v>
       </c>
       <c r="D105" t="n">
-        <v>0.04280313476920128</v>
+        <v>-0.2315666973590851</v>
       </c>
     </row>
     <row r="106">
@@ -1905,13 +1905,13 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>0.1549113094806671</v>
+        <v>-0.8915205597877502</v>
       </c>
       <c r="C106" t="n">
-        <v>0.5823915600776672</v>
+        <v>-0.5506216883659363</v>
       </c>
       <c r="D106" t="n">
-        <v>0.08974611759185791</v>
+        <v>0.006046682596206665</v>
       </c>
     </row>
     <row r="107">
@@ -1919,13 +1919,13 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>0.1559800654649734</v>
+        <v>-0.9132879376411438</v>
       </c>
       <c r="C107" t="n">
-        <v>0.6279996037483215</v>
+        <v>-0.6573213934898376</v>
       </c>
       <c r="D107" t="n">
-        <v>0.08242625743150711</v>
+        <v>0.05412334203720093</v>
       </c>
     </row>
     <row r="108">
@@ -1933,13 +1933,13 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>0.2405606061220169</v>
+        <v>-0.901584804058075</v>
       </c>
       <c r="C108" t="n">
-        <v>0.7839590311050415</v>
+        <v>-0.7726903557777405</v>
       </c>
       <c r="D108" t="n">
-        <v>0.1417016685009003</v>
+        <v>-0.5430350303649902</v>
       </c>
     </row>
     <row r="109">
@@ -1947,13 +1947,13 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>0.2327449768781662</v>
+        <v>-1.13560676574707</v>
       </c>
       <c r="C109" t="n">
-        <v>0.6885680556297302</v>
+        <v>-0.9305006265640259</v>
       </c>
       <c r="D109" t="n">
-        <v>0.08632232993841171</v>
+        <v>-0.2799254953861237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2022/11/19 14:52 update dqn
</commit_message>
<xml_diff>
--- a/documents/latent_vector/dqn_enc.xlsx
+++ b/documents/latent_vector/dqn_enc.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D109"/>
+  <dimension ref="A1:D100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,13 +449,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.8774068355560303</v>
+        <v>-0.05751755461096764</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.7383936643600464</v>
+        <v>-0.07863876223564148</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.2346171140670776</v>
+        <v>-2.797753810882568</v>
       </c>
     </row>
     <row r="3">
@@ -463,13 +463,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.9186053872108459</v>
+        <v>0.01273531094193459</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.7034066915512085</v>
+        <v>-0.1090948879718781</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.1846785545349121</v>
+        <v>-2.563391923904419</v>
       </c>
     </row>
     <row r="4">
@@ -477,13 +477,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.8609176874160767</v>
+        <v>0.01083723083138466</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.7189714908599854</v>
+        <v>-0.1189725995063782</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.1842665076255798</v>
+        <v>-2.497375965118408</v>
       </c>
     </row>
     <row r="5">
@@ -491,13 +491,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.9566603302955627</v>
+        <v>-0.05504673346877098</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.7575868964195251</v>
+        <v>-0.09577482938766479</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.2478329539299011</v>
+        <v>-2.812888383865356</v>
       </c>
     </row>
     <row r="6">
@@ -505,13 +505,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.8675116896629333</v>
+        <v>-0.04941287264227867</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.7727258205413818</v>
+        <v>-0.08105501532554626</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.3054336905479431</v>
+        <v>-2.676848649978638</v>
       </c>
     </row>
     <row r="7">
@@ -519,13 +519,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.9408020973205566</v>
+        <v>-0.02731805667281151</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.7823367118835449</v>
+        <v>-0.1104910373687744</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.3440484404563904</v>
+        <v>-2.615088939666748</v>
       </c>
     </row>
     <row r="8">
@@ -533,13 +533,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.8622509837150574</v>
+        <v>-0.1334226429462433</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.6972945332527161</v>
+        <v>-0.05446475744247437</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.1856018900871277</v>
+        <v>-2.884277820587158</v>
       </c>
     </row>
     <row r="9">
@@ -547,13 +547,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.9113166332244873</v>
+        <v>-0.02164807543158531</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.7507771253585815</v>
+        <v>-0.1055441498756409</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.2932602763175964</v>
+        <v>-2.686341524124146</v>
       </c>
     </row>
     <row r="10">
@@ -561,13 +561,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.816106379032135</v>
+        <v>-0.0387059710919857</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.6514130234718323</v>
+        <v>-0.09468626976013184</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.1786742508411407</v>
+        <v>-2.668492555618286</v>
       </c>
     </row>
     <row r="11">
@@ -575,13 +575,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.9811093211174011</v>
+        <v>-0.008524205535650253</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.8581236600875854</v>
+        <v>-0.1100817024707794</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.4552638530731201</v>
+        <v>-2.696887969970703</v>
       </c>
     </row>
     <row r="12">
@@ -589,13 +589,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.8466823697090149</v>
+        <v>0.0689026415348053</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.6582441926002502</v>
+        <v>-0.1124202311038971</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.1511086225509644</v>
+        <v>-2.420565605163574</v>
       </c>
     </row>
     <row r="13">
@@ -603,13 +603,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.9953675270080566</v>
+        <v>-0.03202873095870018</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.7804772853851318</v>
+        <v>-0.08437672257423401</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.2526264786720276</v>
+        <v>-2.499280214309692</v>
       </c>
     </row>
     <row r="14">
@@ -617,13 +617,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.8919361233711243</v>
+        <v>-0.04944312199950218</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.7302467823028564</v>
+        <v>-0.09857445955276489</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.2182176411151886</v>
+        <v>-2.761451959609985</v>
       </c>
     </row>
     <row r="15">
@@ -631,13 +631,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.8620424866676331</v>
+        <v>-0.09258949756622314</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.7769688367843628</v>
+        <v>-0.08368837833404541</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.3466309309005737</v>
+        <v>-2.677727460861206</v>
       </c>
     </row>
     <row r="16">
@@ -645,13 +645,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.8507569432258606</v>
+        <v>-0.1066428124904633</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.7782182693481445</v>
+        <v>-0.08763685822486877</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.6273947954177856</v>
+        <v>-2.847096920013428</v>
       </c>
     </row>
     <row r="17">
@@ -659,13 +659,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.7930828332901001</v>
+        <v>0.01349187269806862</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.7877063155174255</v>
+        <v>-0.1164636611938477</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.8255119323730469</v>
+        <v>-2.574641704559326</v>
       </c>
     </row>
     <row r="18">
@@ -673,13 +673,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.8147932887077332</v>
+        <v>-0.170587033033371</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.7664750814437866</v>
+        <v>-0.04318028688430786</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.5391026735305786</v>
+        <v>-3.234835624694824</v>
       </c>
     </row>
     <row r="19">
@@ -687,13 +687,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.8702529668807983</v>
+        <v>-0.2406007349491119</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.7287623882293701</v>
+        <v>0.05269283056259155</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.3113494515419006</v>
+        <v>-2.930032014846802</v>
       </c>
     </row>
     <row r="20">
@@ -701,13 +701,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.9391471743583679</v>
+        <v>0.01010498777031898</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.7798076868057251</v>
+        <v>-0.1531925201416016</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.09585863351821899</v>
+        <v>-3.470056295394897</v>
       </c>
     </row>
     <row r="21">
@@ -715,13 +715,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.9158798456192017</v>
+        <v>-0.1814344525337219</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.8201900124549866</v>
+        <v>-0.002209365367889404</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.1289330720901489</v>
+        <v>-3.066163063049316</v>
       </c>
     </row>
     <row r="22">
@@ -729,13 +729,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.9638277888298035</v>
+        <v>-0.2329969704151154</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.8074393272399902</v>
+        <v>0.0416833758354187</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.2746186852455139</v>
+        <v>-3.115118980407715</v>
       </c>
     </row>
     <row r="23">
@@ -743,13 +743,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.8498709201812744</v>
+        <v>-0.1754093766212463</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.839926540851593</v>
+        <v>0.01195508241653442</v>
       </c>
       <c r="D23" t="n">
-        <v>-0.3209908008575439</v>
+        <v>-2.897769927978516</v>
       </c>
     </row>
     <row r="24">
@@ -757,13 +757,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.9768247008323669</v>
+        <v>-0.2048318386077881</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.8339508771896362</v>
+        <v>0.02741223573684692</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.1955572068691254</v>
+        <v>-2.844274759292603</v>
       </c>
     </row>
     <row r="25">
@@ -771,13 +771,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>-0.9113130569458008</v>
+        <v>0.03706547990441322</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.7337418794631958</v>
+        <v>-0.1384758353233337</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.009817942976951599</v>
+        <v>-3.235979318618774</v>
       </c>
     </row>
     <row r="26">
@@ -785,13 +785,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>-0.8702506422996521</v>
+        <v>0.1436060070991516</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.768538236618042</v>
+        <v>-0.06466120481491089</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.2041963338851929</v>
+        <v>-1.942356824874878</v>
       </c>
     </row>
     <row r="27">
@@ -799,13 +799,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>-0.9325038194656372</v>
+        <v>0.1117128729820251</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.6933842897415161</v>
+        <v>-0.04439681768417358</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.2322947978973389</v>
+        <v>-1.676313161849976</v>
       </c>
     </row>
     <row r="28">
@@ -813,13 +813,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>-0.9567565321922302</v>
+        <v>0.305801659822464</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.7441583871841431</v>
+        <v>-0.2349746227264404</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.09162810444831848</v>
+        <v>-2.900626659393311</v>
       </c>
     </row>
     <row r="29">
@@ -827,13 +827,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>-0.8933591842651367</v>
+        <v>0.07463529706001282</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.8059036135673523</v>
+        <v>-0.1652590334415436</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.2341111600399017</v>
+        <v>-1.854342103004456</v>
       </c>
     </row>
     <row r="30">
@@ -841,13 +841,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>-0.9299925565719604</v>
+        <v>0.06223228946328163</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.8046311140060425</v>
+        <v>-0.1271074116230011</v>
       </c>
       <c r="D30" t="n">
-        <v>-0.1849361658096313</v>
+        <v>-2.078770875930786</v>
       </c>
     </row>
     <row r="31">
@@ -855,13 +855,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>-0.876373827457428</v>
+        <v>0.07020518183708191</v>
       </c>
       <c r="C31" t="n">
-        <v>-0.7470036745071411</v>
+        <v>-0.1105251014232635</v>
       </c>
       <c r="D31" t="n">
-        <v>-0.08855932950973511</v>
+        <v>-2.11706018447876</v>
       </c>
     </row>
     <row r="32">
@@ -869,13 +869,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>-0.9010275602340698</v>
+        <v>0.08978855609893799</v>
       </c>
       <c r="C32" t="n">
-        <v>-0.8084818124771118</v>
+        <v>-0.1504288911819458</v>
       </c>
       <c r="D32" t="n">
-        <v>-0.1852150559425354</v>
+        <v>-2.246080636978149</v>
       </c>
     </row>
     <row r="33">
@@ -883,13 +883,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>-0.8761732578277588</v>
+        <v>-0.1380027830600739</v>
       </c>
       <c r="C33" t="n">
-        <v>-0.7376439571380615</v>
+        <v>-0.005804121494293213</v>
       </c>
       <c r="D33" t="n">
-        <v>-0.1311497986316681</v>
+        <v>-2.826929807662964</v>
       </c>
     </row>
     <row r="34">
@@ -897,13 +897,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>-0.9619056582450867</v>
+        <v>-0.09299525618553162</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.7438372373580933</v>
+        <v>-0.02088028192520142</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.03058096766471863</v>
+        <v>-2.653265237808228</v>
       </c>
     </row>
     <row r="35">
@@ -911,13 +911,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>-1.063008308410645</v>
+        <v>-0.1369346082210541</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.7170872092247009</v>
+        <v>-0.08139866590499878</v>
       </c>
       <c r="D35" t="n">
-        <v>-0.1024332642555237</v>
+        <v>-3.393769025802612</v>
       </c>
     </row>
     <row r="36">
@@ -925,13 +925,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>-0.931325376033783</v>
+        <v>-0.2423937022686005</v>
       </c>
       <c r="C36" t="n">
-        <v>-0.6872330904006958</v>
+        <v>-0.07859289646148682</v>
       </c>
       <c r="D36" t="n">
-        <v>-0.2540508508682251</v>
+        <v>-3.607364654541016</v>
       </c>
     </row>
     <row r="37">
@@ -939,13 +939,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>-0.8784062266349792</v>
+        <v>-0.0318167470395565</v>
       </c>
       <c r="C37" t="n">
-        <v>-0.6572571992874146</v>
+        <v>-0.1305981278419495</v>
       </c>
       <c r="D37" t="n">
-        <v>-0.3483367562294006</v>
+        <v>-2.875092029571533</v>
       </c>
     </row>
     <row r="38">
@@ -953,13 +953,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>-0.672127902507782</v>
+        <v>0.1032951176166534</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.5604920387268066</v>
+        <v>-0.07205832004547119</v>
       </c>
       <c r="D38" t="n">
-        <v>-0.4841903448104858</v>
+        <v>-2.260465383529663</v>
       </c>
     </row>
     <row r="39">
@@ -967,13 +967,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>-0.9214125275611877</v>
+        <v>0.2972818315029144</v>
       </c>
       <c r="C39" t="n">
-        <v>-0.7168911695480347</v>
+        <v>-0.228283554315567</v>
       </c>
       <c r="D39" t="n">
-        <v>-0.340360701084137</v>
+        <v>-2.427710056304932</v>
       </c>
     </row>
     <row r="40">
@@ -981,13 +981,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>-0.9229697585105896</v>
+        <v>0.3209034204483032</v>
       </c>
       <c r="C40" t="n">
-        <v>-0.6833274364471436</v>
+        <v>-0.2813079655170441</v>
       </c>
       <c r="D40" t="n">
-        <v>-0.3721800446510315</v>
+        <v>-2.571775674819946</v>
       </c>
     </row>
     <row r="41">
@@ -995,13 +995,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>-0.9724355340003967</v>
+        <v>0.1690127551555634</v>
       </c>
       <c r="C41" t="n">
-        <v>-0.7387970089912415</v>
+        <v>-0.06046938896179199</v>
       </c>
       <c r="D41" t="n">
-        <v>-0.3970728516578674</v>
+        <v>-2.039803266525269</v>
       </c>
     </row>
     <row r="42">
@@ -1009,13 +1009,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>-0.9347510933876038</v>
+        <v>0.1860611736774445</v>
       </c>
       <c r="C42" t="n">
-        <v>-0.5326456427574158</v>
+        <v>-0.0391312837600708</v>
       </c>
       <c r="D42" t="n">
-        <v>-0.2284276187419891</v>
+        <v>-1.744403958320618</v>
       </c>
     </row>
     <row r="43">
@@ -1023,13 +1023,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>-0.9229821562767029</v>
+        <v>0.02863732352852821</v>
       </c>
       <c r="C43" t="n">
-        <v>-0.7050019502639771</v>
+        <v>-0.1198796331882477</v>
       </c>
       <c r="D43" t="n">
-        <v>-0.3344995379447937</v>
+        <v>-2.277817010879517</v>
       </c>
     </row>
     <row r="44">
@@ -1037,13 +1037,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>-0.8722541332244873</v>
+        <v>-0.04293495044112206</v>
       </c>
       <c r="C44" t="n">
-        <v>-0.6703691482543945</v>
+        <v>-0.1232431828975677</v>
       </c>
       <c r="D44" t="n">
-        <v>-0.3964746594429016</v>
+        <v>-2.783573389053345</v>
       </c>
     </row>
     <row r="45">
@@ -1051,13 +1051,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>-0.5858168601989746</v>
+        <v>-0.01973041519522667</v>
       </c>
       <c r="C45" t="n">
-        <v>-0.5052000880241394</v>
+        <v>-0.1497257649898529</v>
       </c>
       <c r="D45" t="n">
-        <v>-0.3992400169372559</v>
+        <v>-2.887499809265137</v>
       </c>
     </row>
     <row r="46">
@@ -1065,13 +1065,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>-0.6317669153213501</v>
+        <v>-0.2274078726768494</v>
       </c>
       <c r="C46" t="n">
-        <v>-0.5336444973945618</v>
+        <v>0.03873777389526367</v>
       </c>
       <c r="D46" t="n">
-        <v>-0.4222643971443176</v>
+        <v>-2.692956924438477</v>
       </c>
     </row>
     <row r="47">
@@ -1079,13 +1079,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>-0.6196783185005188</v>
+        <v>-0.1602712571620941</v>
       </c>
       <c r="C47" t="n">
-        <v>-0.5134835839271545</v>
+        <v>-0.03351470828056335</v>
       </c>
       <c r="D47" t="n">
-        <v>-0.4220762252807617</v>
+        <v>-2.843706130981445</v>
       </c>
     </row>
     <row r="48">
@@ -1093,13 +1093,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>-0.6037497520446777</v>
+        <v>-0.1580313444137573</v>
       </c>
       <c r="C48" t="n">
-        <v>-0.5197960734367371</v>
+        <v>-0.03174009919166565</v>
       </c>
       <c r="D48" t="n">
-        <v>-0.4393643736839294</v>
+        <v>-2.798237085342407</v>
       </c>
     </row>
     <row r="49">
@@ -1107,13 +1107,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>-0.819627583026886</v>
+        <v>-0.1340716183185577</v>
       </c>
       <c r="C49" t="n">
-        <v>-0.7662175297737122</v>
+        <v>-0.05264505743980408</v>
       </c>
       <c r="D49" t="n">
-        <v>-0.4405239224433899</v>
+        <v>-2.641139030456543</v>
       </c>
     </row>
     <row r="50">
@@ -1121,13 +1121,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>-1.400162935256958</v>
+        <v>-0.408252626657486</v>
       </c>
       <c r="C50" t="n">
-        <v>-0.9566746950149536</v>
+        <v>-0.01370185613632202</v>
       </c>
       <c r="D50" t="n">
-        <v>-0.03369809687137604</v>
+        <v>-4.861169815063477</v>
       </c>
     </row>
     <row r="51">
@@ -1135,13 +1135,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>-0.8442731499671936</v>
+        <v>0.02376875653862953</v>
       </c>
       <c r="C51" t="n">
-        <v>-0.7557651996612549</v>
+        <v>-0.2015618681907654</v>
       </c>
       <c r="D51" t="n">
-        <v>0.123165637254715</v>
+        <v>-3.177826404571533</v>
       </c>
     </row>
     <row r="52">
@@ -1149,13 +1149,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>-0.8398253321647644</v>
+        <v>-0.2332378327846527</v>
       </c>
       <c r="C52" t="n">
-        <v>-0.7660485506057739</v>
+        <v>-0.01380401849746704</v>
       </c>
       <c r="D52" t="n">
-        <v>0.1208779066801071</v>
+        <v>-3.05435037612915</v>
       </c>
     </row>
     <row r="53">
@@ -1163,13 +1163,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>-1.310978651046753</v>
+        <v>0.04719511047005653</v>
       </c>
       <c r="C53" t="n">
-        <v>-0.9460172057151794</v>
+        <v>-0.2161309123039246</v>
       </c>
       <c r="D53" t="n">
-        <v>-0.227546215057373</v>
+        <v>-2.614461660385132</v>
       </c>
     </row>
     <row r="54">
@@ -1177,13 +1177,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>-0.731418251991272</v>
+        <v>0.1160457730293274</v>
       </c>
       <c r="C54" t="n">
-        <v>-0.9099568724632263</v>
+        <v>-0.1695345342159271</v>
       </c>
       <c r="D54" t="n">
-        <v>-0.5547305345535278</v>
+        <v>-2.262586116790771</v>
       </c>
     </row>
     <row r="55">
@@ -1191,13 +1191,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>-1.118304014205933</v>
+        <v>0.04817662015557289</v>
       </c>
       <c r="C55" t="n">
-        <v>-1.07854688167572</v>
+        <v>-0.1400728821754456</v>
       </c>
       <c r="D55" t="n">
-        <v>-0.5860914587974548</v>
+        <v>-3.006462812423706</v>
       </c>
     </row>
     <row r="56">
@@ -1205,13 +1205,13 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>-0.8974708318710327</v>
+        <v>0.05764985457062721</v>
       </c>
       <c r="C56" t="n">
-        <v>-0.5383338332176208</v>
+        <v>-0.1287521123886108</v>
       </c>
       <c r="D56" t="n">
-        <v>-0.334769070148468</v>
+        <v>-2.765556812286377</v>
       </c>
     </row>
     <row r="57">
@@ -1219,13 +1219,13 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>-0.7136864066123962</v>
+        <v>0.06040966883301735</v>
       </c>
       <c r="C57" t="n">
-        <v>-0.5790572166442871</v>
+        <v>-0.1432388722896576</v>
       </c>
       <c r="D57" t="n">
-        <v>-0.120156466960907</v>
+        <v>-2.746853351593018</v>
       </c>
     </row>
     <row r="58">
@@ -1233,13 +1233,13 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>-0.7789818644523621</v>
+        <v>0.1371645331382751</v>
       </c>
       <c r="C58" t="n">
-        <v>-0.6184816360473633</v>
+        <v>-0.1792178153991699</v>
       </c>
       <c r="D58" t="n">
-        <v>-0.2397118806838989</v>
+        <v>-2.380915641784668</v>
       </c>
     </row>
     <row r="59">
@@ -1247,13 +1247,13 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>-1.003947973251343</v>
+        <v>0.2011048495769501</v>
       </c>
       <c r="C59" t="n">
-        <v>-0.8050851225852966</v>
+        <v>-0.1381255090236664</v>
       </c>
       <c r="D59" t="n">
-        <v>-0.1685780584812164</v>
+        <v>-1.920045971870422</v>
       </c>
     </row>
     <row r="60">
@@ -1261,13 +1261,13 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>-1.418603420257568</v>
+        <v>-0.1721980273723602</v>
       </c>
       <c r="C60" t="n">
-        <v>-0.9027448892593384</v>
+        <v>0.0758381187915802</v>
       </c>
       <c r="D60" t="n">
-        <v>0.04229003190994263</v>
+        <v>-2.677392482757568</v>
       </c>
     </row>
     <row r="61">
@@ -1275,13 +1275,13 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>-1.110793948173523</v>
+        <v>0.1336536407470703</v>
       </c>
       <c r="C61" t="n">
-        <v>-0.6732813715934753</v>
+        <v>-0.1759807467460632</v>
       </c>
       <c r="D61" t="n">
-        <v>-0.06197705864906311</v>
+        <v>-2.146183729171753</v>
       </c>
     </row>
     <row r="62">
@@ -1289,13 +1289,13 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>-0.8194100856781006</v>
+        <v>0.02083036676049232</v>
       </c>
       <c r="C62" t="n">
-        <v>-0.5357325077056885</v>
+        <v>-0.1363022327423096</v>
       </c>
       <c r="D62" t="n">
-        <v>-0.3365902304649353</v>
+        <v>-2.825505256652832</v>
       </c>
     </row>
     <row r="63">
@@ -1303,13 +1303,13 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>-0.6620504856109619</v>
+        <v>-0.1459465324878693</v>
       </c>
       <c r="C63" t="n">
-        <v>-0.8748719692230225</v>
+        <v>-0.08133071660995483</v>
       </c>
       <c r="D63" t="n">
-        <v>-0.5809007287025452</v>
+        <v>-2.54502534866333</v>
       </c>
     </row>
     <row r="64">
@@ -1317,13 +1317,13 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>-1.010077357292175</v>
+        <v>-0.2054524123668671</v>
       </c>
       <c r="C64" t="n">
-        <v>-0.8484398722648621</v>
+        <v>-0.1417455673217773</v>
       </c>
       <c r="D64" t="n">
-        <v>-0.2630506753921509</v>
+        <v>-2.923673391342163</v>
       </c>
     </row>
     <row r="65">
@@ -1331,13 +1331,13 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>-0.6523619294166565</v>
+        <v>-0.1532022058963776</v>
       </c>
       <c r="C65" t="n">
-        <v>-0.5528481602668762</v>
+        <v>-0.08654096722602844</v>
       </c>
       <c r="D65" t="n">
-        <v>-0.08960515260696411</v>
+        <v>-2.501302242279053</v>
       </c>
     </row>
     <row r="66">
@@ -1345,13 +1345,13 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>-0.5157608389854431</v>
+        <v>-0.2158795595169067</v>
       </c>
       <c r="C66" t="n">
-        <v>-0.5098051428794861</v>
+        <v>-0.08667004108428955</v>
       </c>
       <c r="D66" t="n">
-        <v>-0.2801095247268677</v>
+        <v>-2.785763502120972</v>
       </c>
     </row>
     <row r="67">
@@ -1359,13 +1359,13 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>-0.7892442941665649</v>
+        <v>-0.241128534078598</v>
       </c>
       <c r="C67" t="n">
-        <v>-0.2910152077674866</v>
+        <v>-0.08384248614311218</v>
       </c>
       <c r="D67" t="n">
-        <v>-0.4437853097915649</v>
+        <v>-2.853880167007446</v>
       </c>
     </row>
     <row r="68">
@@ -1373,13 +1373,13 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>-1.252237558364868</v>
+        <v>-0.03373393043875694</v>
       </c>
       <c r="C68" t="n">
-        <v>-0.9243879318237305</v>
+        <v>-0.1055137515068054</v>
       </c>
       <c r="D68" t="n">
-        <v>-0.395668089389801</v>
+        <v>-2.51575779914856</v>
       </c>
     </row>
     <row r="69">
@@ -1387,13 +1387,13 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>-0.6584404706954956</v>
+        <v>0.1154593825340271</v>
       </c>
       <c r="C69" t="n">
-        <v>-0.5859214663505554</v>
+        <v>-0.136609673500061</v>
       </c>
       <c r="D69" t="n">
-        <v>-0.1544092297554016</v>
+        <v>-2.272549152374268</v>
       </c>
     </row>
     <row r="70">
@@ -1401,13 +1401,13 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>-0.9030315279960632</v>
+        <v>0.1926577687263489</v>
       </c>
       <c r="C70" t="n">
-        <v>-0.8191682100296021</v>
+        <v>-0.1192178428173065</v>
       </c>
       <c r="D70" t="n">
-        <v>-0.3347437381744385</v>
+        <v>-2.281721830368042</v>
       </c>
     </row>
     <row r="71">
@@ -1415,13 +1415,13 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>-0.9266481995582581</v>
+        <v>-0.09850943088531494</v>
       </c>
       <c r="C71" t="n">
-        <v>-0.8069517016410828</v>
+        <v>-0.1141476631164551</v>
       </c>
       <c r="D71" t="n">
-        <v>-0.1643447279930115</v>
+        <v>-3.132748603820801</v>
       </c>
     </row>
     <row r="72">
@@ -1429,13 +1429,13 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>-0.8937005400657654</v>
+        <v>-0.05152466520667076</v>
       </c>
       <c r="C72" t="n">
-        <v>-0.8671473264694214</v>
+        <v>-0.1361389756202698</v>
       </c>
       <c r="D72" t="n">
-        <v>-0.2104970812797546</v>
+        <v>-3.177457809448242</v>
       </c>
     </row>
     <row r="73">
@@ -1443,13 +1443,13 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>-0.7115880846977234</v>
+        <v>0.04531669989228249</v>
       </c>
       <c r="C73" t="n">
-        <v>-0.6350852251052856</v>
+        <v>-0.1157335937023163</v>
       </c>
       <c r="D73" t="n">
-        <v>-0.1761727929115295</v>
+        <v>-2.734886884689331</v>
       </c>
     </row>
     <row r="74">
@@ -1457,13 +1457,13 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>-0.6285414099693298</v>
+        <v>-0.03438576683402061</v>
       </c>
       <c r="C74" t="n">
-        <v>-0.5604482293128967</v>
+        <v>-0.09674900770187378</v>
       </c>
       <c r="D74" t="n">
-        <v>-0.1903518736362457</v>
+        <v>-2.986640930175781</v>
       </c>
     </row>
     <row r="75">
@@ -1471,13 +1471,13 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>-0.6371750831604004</v>
+        <v>0.09863817691802979</v>
       </c>
       <c r="C75" t="n">
-        <v>-0.5297112464904785</v>
+        <v>-0.1327765285968781</v>
       </c>
       <c r="D75" t="n">
-        <v>-0.1422064304351807</v>
+        <v>-2.287463426589966</v>
       </c>
     </row>
     <row r="76">
@@ -1485,13 +1485,13 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>-0.7414934635162354</v>
+        <v>0.007495258003473282</v>
       </c>
       <c r="C76" t="n">
-        <v>-0.6893380284309387</v>
+        <v>-0.1201707720756531</v>
       </c>
       <c r="D76" t="n">
-        <v>-0.1294722557067871</v>
+        <v>-2.971428155899048</v>
       </c>
     </row>
     <row r="77">
@@ -1499,13 +1499,13 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>-0.8807417750358582</v>
+        <v>0.09950897097587585</v>
       </c>
       <c r="C77" t="n">
-        <v>-0.7832221984863281</v>
+        <v>-0.1035781502723694</v>
       </c>
       <c r="D77" t="n">
-        <v>0.04081235826015472</v>
+        <v>-2.20732045173645</v>
       </c>
     </row>
     <row r="78">
@@ -1513,13 +1513,13 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>-0.8170123100280762</v>
+        <v>0.131886750459671</v>
       </c>
       <c r="C78" t="n">
-        <v>-0.7336433529853821</v>
+        <v>-0.1420256495475769</v>
       </c>
       <c r="D78" t="n">
-        <v>0.04615232348442078</v>
+        <v>-2.103585481643677</v>
       </c>
     </row>
     <row r="79">
@@ -1527,13 +1527,13 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>-1.005516290664673</v>
+        <v>0.1496081948280334</v>
       </c>
       <c r="C79" t="n">
-        <v>-0.8315661549568176</v>
+        <v>-0.1380329728126526</v>
       </c>
       <c r="D79" t="n">
-        <v>-0.2537497282028198</v>
+        <v>-2.061406850814819</v>
       </c>
     </row>
     <row r="80">
@@ -1541,13 +1541,13 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>-0.9059018492698669</v>
+        <v>-0.1314238309860229</v>
       </c>
       <c r="C80" t="n">
-        <v>-0.7591546177864075</v>
+        <v>-0.1088929176330566</v>
       </c>
       <c r="D80" t="n">
-        <v>0.06129594147205353</v>
+        <v>-2.999143838882446</v>
       </c>
     </row>
     <row r="81">
@@ -1555,13 +1555,13 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>-0.8367088437080383</v>
+        <v>-0.1481694877147675</v>
       </c>
       <c r="C81" t="n">
-        <v>-0.7220001220703125</v>
+        <v>-0.09768828749656677</v>
       </c>
       <c r="D81" t="n">
-        <v>0.03110097348690033</v>
+        <v>-2.562745571136475</v>
       </c>
     </row>
     <row r="82">
@@ -1569,13 +1569,13 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>-0.6509606838226318</v>
+        <v>-0.188601016998291</v>
       </c>
       <c r="C82" t="n">
-        <v>-0.5716146230697632</v>
+        <v>-0.09587067365646362</v>
       </c>
       <c r="D82" t="n">
-        <v>-0.2604126632213593</v>
+        <v>-2.896140336990356</v>
       </c>
     </row>
     <row r="83">
@@ -1583,13 +1583,13 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>-0.793902575969696</v>
+        <v>0.101457804441452</v>
       </c>
       <c r="C83" t="n">
-        <v>-0.5813690423965454</v>
+        <v>-0.0904543399810791</v>
       </c>
       <c r="D83" t="n">
-        <v>-0.4137298464775085</v>
+        <v>-2.150952339172363</v>
       </c>
     </row>
     <row r="84">
@@ -1597,13 +1597,13 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>-1.02420699596405</v>
+        <v>-0.2753960788249969</v>
       </c>
       <c r="C84" t="n">
-        <v>-0.8435726165771484</v>
+        <v>0.05077797174453735</v>
       </c>
       <c r="D84" t="n">
-        <v>0.01820382475852966</v>
+        <v>-2.850231885910034</v>
       </c>
     </row>
     <row r="85">
@@ -1611,13 +1611,13 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>-0.8467736840248108</v>
+        <v>-0.4625209271907806</v>
       </c>
       <c r="C85" t="n">
-        <v>-0.5616253614425659</v>
+        <v>0.09635978937149048</v>
       </c>
       <c r="D85" t="n">
-        <v>-0.3505874872207642</v>
+        <v>-3.478387594223022</v>
       </c>
     </row>
     <row r="86">
@@ -1625,13 +1625,13 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>-0.8272479176521301</v>
+        <v>-0.4625254571437836</v>
       </c>
       <c r="C86" t="n">
-        <v>-0.5727234482765198</v>
+        <v>0.09599491953849792</v>
       </c>
       <c r="D86" t="n">
-        <v>-0.3598759770393372</v>
+        <v>-3.455483675003052</v>
       </c>
     </row>
     <row r="87">
@@ -1639,13 +1639,13 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>-0.8322588205337524</v>
+        <v>-0.4051770269870758</v>
       </c>
       <c r="C87" t="n">
-        <v>-0.6074560880661011</v>
+        <v>0.0720934271812439</v>
       </c>
       <c r="D87" t="n">
-        <v>-0.4309888482093811</v>
+        <v>-3.402441501617432</v>
       </c>
     </row>
     <row r="88">
@@ -1653,13 +1653,13 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>-0.8355688452720642</v>
+        <v>-0.3486715853214264</v>
       </c>
       <c r="C88" t="n">
-        <v>-0.5805323719978333</v>
+        <v>0.06162047386169434</v>
       </c>
       <c r="D88" t="n">
-        <v>-0.4553248286247253</v>
+        <v>-3.143232107162476</v>
       </c>
     </row>
     <row r="89">
@@ -1667,13 +1667,13 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>-0.8363886475563049</v>
+        <v>-0.2869142889976501</v>
       </c>
       <c r="C89" t="n">
-        <v>-0.6319226026535034</v>
+        <v>0.02983152866363525</v>
       </c>
       <c r="D89" t="n">
-        <v>-0.4785870313644409</v>
+        <v>-3.278631687164307</v>
       </c>
     </row>
     <row r="90">
@@ -1681,13 +1681,13 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>-0.7561878561973572</v>
+        <v>-0.3461761474609375</v>
       </c>
       <c r="C90" t="n">
-        <v>-0.5967325568199158</v>
+        <v>0.07443785667419434</v>
       </c>
       <c r="D90" t="n">
-        <v>-0.5032638311386108</v>
+        <v>-3.287724733352661</v>
       </c>
     </row>
     <row r="91">
@@ -1695,13 +1695,13 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>-1.187577962875366</v>
+        <v>-0.3154140412807465</v>
       </c>
       <c r="C91" t="n">
-        <v>-0.7695111632347107</v>
+        <v>0.04979372024536133</v>
       </c>
       <c r="D91" t="n">
-        <v>0.02995775640010834</v>
+        <v>-3.258182048797607</v>
       </c>
     </row>
     <row r="92">
@@ -1709,13 +1709,13 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>-0.825555682182312</v>
+        <v>-0.4016518890857697</v>
       </c>
       <c r="C92" t="n">
-        <v>-0.68916255235672</v>
+        <v>0.0213019847869873</v>
       </c>
       <c r="D92" t="n">
-        <v>-0.009141802787780762</v>
+        <v>-4.125308036804199</v>
       </c>
     </row>
     <row r="93">
@@ -1723,13 +1723,13 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>-0.8738554716110229</v>
+        <v>-0.121614933013916</v>
       </c>
       <c r="C93" t="n">
-        <v>-0.6865558624267578</v>
+        <v>-0.05936133861541748</v>
       </c>
       <c r="D93" t="n">
-        <v>0.0009653568267822266</v>
+        <v>-2.436002969741821</v>
       </c>
     </row>
     <row r="94">
@@ -1737,13 +1737,13 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>-0.845971405506134</v>
+        <v>-0.1854446530342102</v>
       </c>
       <c r="C94" t="n">
-        <v>-0.7025161385536194</v>
+        <v>-0.09737381339073181</v>
       </c>
       <c r="D94" t="n">
-        <v>0.05642545223236084</v>
+        <v>-3.198138952255249</v>
       </c>
     </row>
     <row r="95">
@@ -1751,13 +1751,13 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>-0.9693118929862976</v>
+        <v>-0.03998666629195213</v>
       </c>
       <c r="C95" t="n">
-        <v>-0.856134295463562</v>
+        <v>-0.1216610074043274</v>
       </c>
       <c r="D95" t="n">
-        <v>-0.5356988310813904</v>
+        <v>-2.312078952789307</v>
       </c>
     </row>
     <row r="96">
@@ -1765,13 +1765,13 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>-0.78933185338974</v>
+        <v>0.09084233641624451</v>
       </c>
       <c r="C96" t="n">
-        <v>-0.7073398232460022</v>
+        <v>0.01657706499099731</v>
       </c>
       <c r="D96" t="n">
-        <v>-0.2124965190887451</v>
+        <v>-1.752875685691833</v>
       </c>
     </row>
     <row r="97">
@@ -1779,13 +1779,13 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>-0.8622241616249084</v>
+        <v>-0.01284446939826012</v>
       </c>
       <c r="C97" t="n">
-        <v>-0.6075205206871033</v>
+        <v>0.09933459758758545</v>
       </c>
       <c r="D97" t="n">
-        <v>-0.35872483253479</v>
+        <v>-1.535300135612488</v>
       </c>
     </row>
     <row r="98">
@@ -1793,13 +1793,13 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>-0.9633070826530457</v>
+        <v>0.06207868829369545</v>
       </c>
       <c r="C98" t="n">
-        <v>-0.6741501688957214</v>
+        <v>-0.2703513205051422</v>
       </c>
       <c r="D98" t="n">
-        <v>-0.135686844587326</v>
+        <v>-2.465483903884888</v>
       </c>
     </row>
     <row r="99">
@@ -1807,13 +1807,13 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>-0.9218026995658875</v>
+        <v>0.03135386481881142</v>
       </c>
       <c r="C99" t="n">
-        <v>-0.5011181235313416</v>
+        <v>-0.229522705078125</v>
       </c>
       <c r="D99" t="n">
-        <v>0.03567130863666534</v>
+        <v>-2.624319314956665</v>
       </c>
     </row>
     <row r="100">
@@ -1821,139 +1821,13 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>-0.8433488607406616</v>
+        <v>0.02335214987397194</v>
       </c>
       <c r="C100" t="n">
-        <v>-0.6030845642089844</v>
+        <v>-0.209313839673996</v>
       </c>
       <c r="D100" t="n">
-        <v>0.09999153017997742</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="1" t="n">
-        <v>99</v>
-      </c>
-      <c r="B101" t="n">
-        <v>-1.04547655582428</v>
-      </c>
-      <c r="C101" t="n">
-        <v>-0.6583418846130371</v>
-      </c>
-      <c r="D101" t="n">
-        <v>0.2069518119096756</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="B102" t="n">
-        <v>-1.140744686126709</v>
-      </c>
-      <c r="C102" t="n">
-        <v>-0.8207313418388367</v>
-      </c>
-      <c r="D102" t="n">
-        <v>-0.3160637617111206</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" s="1" t="n">
-        <v>101</v>
-      </c>
-      <c r="B103" t="n">
-        <v>-1.645563244819641</v>
-      </c>
-      <c r="C103" t="n">
-        <v>-1.027688264846802</v>
-      </c>
-      <c r="D103" t="n">
-        <v>0.1231574863195419</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="1" t="n">
-        <v>102</v>
-      </c>
-      <c r="B104" t="n">
-        <v>-0.8744520545005798</v>
-      </c>
-      <c r="C104" t="n">
-        <v>-0.6345198154449463</v>
-      </c>
-      <c r="D104" t="n">
-        <v>-0.185737133026123</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="1" t="n">
-        <v>103</v>
-      </c>
-      <c r="B105" t="n">
-        <v>-0.9828851819038391</v>
-      </c>
-      <c r="C105" t="n">
-        <v>-0.6749557256698608</v>
-      </c>
-      <c r="D105" t="n">
-        <v>-0.2315666973590851</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="1" t="n">
-        <v>104</v>
-      </c>
-      <c r="B106" t="n">
-        <v>-0.8915205597877502</v>
-      </c>
-      <c r="C106" t="n">
-        <v>-0.5506216883659363</v>
-      </c>
-      <c r="D106" t="n">
-        <v>0.006046682596206665</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" s="1" t="n">
-        <v>105</v>
-      </c>
-      <c r="B107" t="n">
-        <v>-0.9132879376411438</v>
-      </c>
-      <c r="C107" t="n">
-        <v>-0.6573213934898376</v>
-      </c>
-      <c r="D107" t="n">
-        <v>0.05412334203720093</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="1" t="n">
-        <v>106</v>
-      </c>
-      <c r="B108" t="n">
-        <v>-0.901584804058075</v>
-      </c>
-      <c r="C108" t="n">
-        <v>-0.7726903557777405</v>
-      </c>
-      <c r="D108" t="n">
-        <v>-0.5430350303649902</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" s="1" t="n">
-        <v>107</v>
-      </c>
-      <c r="B109" t="n">
-        <v>-1.13560676574707</v>
-      </c>
-      <c r="C109" t="n">
-        <v>-0.9305006265640259</v>
-      </c>
-      <c r="D109" t="n">
-        <v>-0.2799254953861237</v>
+        <v>-2.324379920959473</v>
       </c>
     </row>
   </sheetData>

</xml_diff>